<commit_message>
updating new size GSD for elowyn
</commit_message>
<xml_diff>
--- a/GSD/baskets_new_sizes/basketGSD_hypflux_NEW_SIZES.xlsx
+++ b/GSD/baskets_new_sizes/basketGSD_hypflux_NEW_SIZES.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\huck4481\Documents\GitHub\La_Jara\GSD\baskets_new_sizes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CF5FB02-E28D-4B0D-A847-21ECFA244204}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1F7AC3F-710B-4DB0-84EB-CC2007DED5D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{FF2C68C4-0230-4397-BD30-01ABAA0FCBBF}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="702" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="702" uniqueCount="112">
   <si>
     <t>Size</t>
   </si>
@@ -362,6 +362,18 @@
   </si>
   <si>
     <t>SUMMER 2023 - NORMALIZE USING CLOSED BASKET WEIGHTS- NO OUTLIER</t>
+  </si>
+  <si>
+    <t>Fine Sand (0.06 mm - 0.5 mm)</t>
+  </si>
+  <si>
+    <t>Fine Sand  (0.06 mm - 0.5 mm)</t>
+  </si>
+  <si>
+    <t>Silt (0.002 mm - 0.06 mm)</t>
+  </si>
+  <si>
+    <t>Coarse Sand (0.5-2 mm)</t>
   </si>
 </sst>
 </file>
@@ -2515,6 +2527,150 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="38" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="40" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="21" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="22" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="24" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="25" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="49" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="26" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="26" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="23" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="24" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="25" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="49" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="26" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="31" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="31" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="31" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="31" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="31" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="31" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="29" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="29" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="29" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="29" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="29" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="29" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="30" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="30" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="30" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2533,108 +2689,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="31" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="31" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="31" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="30" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="30" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="30" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="29" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="29" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="29" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="29" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="29" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="29" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="36" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="36" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="36" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="36" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="36" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="36" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="31" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="31" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="31" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="38" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="38" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="38" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="38" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="38" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="38" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="30" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2653,6 +2710,9 @@
     <xf numFmtId="0" fontId="0" fillId="33" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2660,54 +2720,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="38" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="40" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="21" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="22" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="24" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="25" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="49" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="26" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="26" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="23" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="24" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="25" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="49" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="26" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -4342,7 +4354,7 @@
             </a:r>
             <a:r>
               <a:rPr lang="es-AR"/>
-              <a:t>sed* vs Hyp Flux </a:t>
+              <a:t>sed* vs Hyp Flux - New Sizes </a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -4391,7 +4403,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Coarse Sand (0.2-2 mm)</c:v>
+                  <c:v>Coarse Sand (0.5-2 mm)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -4573,7 +4585,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Fine Sand (0.02-0.2 mm)</c:v>
+                  <c:v>Fine Sand (0.06 mm - 0.5 mm)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -4755,7 +4767,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Silt (0.002-0.02 mm)</c:v>
+                  <c:v>Silt (0.002 mm - 0.06 mm)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -5565,7 +5577,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Coarse Sand (0.2-2 mm)</c:v>
+                  <c:v>Coarse Sand (0.5-2 mm)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -5735,7 +5747,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Fine Sand (0.02-0.2 mm)</c:v>
+                  <c:v>Fine Sand (0.06 mm - 0.5 mm)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -5905,7 +5917,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Silt (0.002-0.02 mm)</c:v>
+                  <c:v>Silt (0.002 mm - 0.06 mm)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -6642,15 +6654,7 @@
             </a:r>
             <a:r>
               <a:rPr lang="es-AR"/>
-              <a:t>sed* vs Hyp Flux - No</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="es-AR" baseline="0"/>
-              <a:t> </a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="es-AR"/>
-              <a:t>Outlier </a:t>
+              <a:t>sed* vs Hyp Flux - New Sizes</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -6699,7 +6703,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Coarse Sand (0.2-2 mm)</c:v>
+                  <c:v>Coarse Sand (0.5-2 mm)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -6742,8 +6746,8 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-0.43166515048760512"/>
-                  <c:y val="-0.43831946539225197"/>
+                  <c:x val="-0.21779710250835815"/>
+                  <c:y val="-0.44794181190775917"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -6863,7 +6867,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Fine Sand (0.02-0.2 mm)</c:v>
+                  <c:v>Fine Sand (0.06 mm - 0.5 mm)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -6906,8 +6910,8 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-0.43359131146842"/>
-                  <c:y val="-0.1845965499148933"/>
+                  <c:x val="-0.2184004725627394"/>
+                  <c:y val="-0.20057324246482053"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -7027,7 +7031,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Silt (0.002-0.02 mm)</c:v>
+                  <c:v>Silt (0.002 mm - 0.06 mm)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -10577,8 +10581,8 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>353984</xdr:colOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>504825</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>10737</xdr:rowOff>
     </xdr:from>
@@ -10613,8 +10617,8 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>342035</xdr:colOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>485775</xdr:colOff>
       <xdr:row>19</xdr:row>
       <xdr:rowOff>76201</xdr:rowOff>
     </xdr:from>
@@ -10651,14 +10655,14 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>371475</xdr:colOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>428625</xdr:colOff>
       <xdr:row>37</xdr:row>
       <xdr:rowOff>161925</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>68060</xdr:colOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
       <xdr:row>56</xdr:row>
       <xdr:rowOff>125729</xdr:rowOff>
     </xdr:to>
@@ -11032,22 +11036,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:38" ht="14.45" customHeight="1">
-      <c r="AG1" s="436" t="s">
+      <c r="AG1" s="469" t="s">
         <v>56</v>
       </c>
-      <c r="AH1" s="436" t="s">
+      <c r="AH1" s="469" t="s">
         <v>57</v>
       </c>
-      <c r="AI1" s="436" t="s">
+      <c r="AI1" s="469" t="s">
         <v>52</v>
       </c>
-      <c r="AJ1" s="436" t="s">
+      <c r="AJ1" s="469" t="s">
         <v>56</v>
       </c>
-      <c r="AK1" s="430" t="s">
+      <c r="AK1" s="478" t="s">
         <v>57</v>
       </c>
-      <c r="AL1" s="430" t="s">
+      <c r="AL1" s="478" t="s">
         <v>52</v>
       </c>
     </row>
@@ -11124,23 +11128,23 @@
       <c r="Y2" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="AB2" s="433" t="s">
+      <c r="AB2" s="481" t="s">
         <v>25</v>
       </c>
-      <c r="AC2" s="434"/>
-      <c r="AD2" s="437" t="s">
+      <c r="AC2" s="482"/>
+      <c r="AD2" s="476" t="s">
         <v>58</v>
       </c>
-      <c r="AE2" s="437"/>
+      <c r="AE2" s="476"/>
       <c r="AF2" s="97" t="s">
         <v>104</v>
       </c>
-      <c r="AG2" s="438"/>
-      <c r="AH2" s="436"/>
-      <c r="AI2" s="436"/>
-      <c r="AJ2" s="436"/>
-      <c r="AK2" s="430"/>
-      <c r="AL2" s="430"/>
+      <c r="AG2" s="484"/>
+      <c r="AH2" s="469"/>
+      <c r="AI2" s="469"/>
+      <c r="AJ2" s="469"/>
+      <c r="AK2" s="478"/>
+      <c r="AL2" s="478"/>
     </row>
     <row r="3" spans="2:38" ht="15">
       <c r="B3" s="14">
@@ -12727,22 +12731,22 @@
       <c r="Y16" s="41">
         <v>1.1583636475738333</v>
       </c>
-      <c r="AG16" s="436" t="s">
+      <c r="AG16" s="469" t="s">
         <v>56</v>
       </c>
-      <c r="AH16" s="436" t="s">
+      <c r="AH16" s="469" t="s">
         <v>57</v>
       </c>
-      <c r="AI16" s="436" t="s">
+      <c r="AI16" s="469" t="s">
         <v>52</v>
       </c>
-      <c r="AJ16" s="436" t="s">
+      <c r="AJ16" s="469" t="s">
         <v>56</v>
       </c>
-      <c r="AK16" s="430" t="s">
+      <c r="AK16" s="478" t="s">
         <v>57</v>
       </c>
-      <c r="AL16" s="430" t="s">
+      <c r="AL16" s="478" t="s">
         <v>52</v>
       </c>
     </row>
@@ -12819,23 +12823,23 @@
       <c r="Y17" s="41">
         <v>1.2284974412725813</v>
       </c>
-      <c r="AB17" s="433" t="s">
+      <c r="AB17" s="481" t="s">
         <v>40</v>
       </c>
-      <c r="AC17" s="435"/>
-      <c r="AD17" s="437" t="s">
+      <c r="AC17" s="483"/>
+      <c r="AD17" s="476" t="s">
         <v>58</v>
       </c>
-      <c r="AE17" s="437"/>
+      <c r="AE17" s="476"/>
       <c r="AF17" s="261" t="s">
         <v>104</v>
       </c>
-      <c r="AG17" s="436"/>
-      <c r="AH17" s="436"/>
-      <c r="AI17" s="436"/>
-      <c r="AJ17" s="436"/>
-      <c r="AK17" s="430"/>
-      <c r="AL17" s="430"/>
+      <c r="AG17" s="469"/>
+      <c r="AH17" s="469"/>
+      <c r="AI17" s="469"/>
+      <c r="AJ17" s="469"/>
+      <c r="AK17" s="478"/>
+      <c r="AL17" s="478"/>
     </row>
     <row r="18" spans="2:39" ht="15">
       <c r="B18" s="28">
@@ -14454,14 +14458,14 @@
       <c r="Y32" s="41">
         <v>6.9971946482520506</v>
       </c>
-      <c r="AA32" s="431" t="s">
+      <c r="AA32" s="479" t="s">
         <v>25</v>
       </c>
-      <c r="AB32" s="431"/>
-      <c r="AC32" s="432" t="s">
+      <c r="AB32" s="479"/>
+      <c r="AC32" s="480" t="s">
         <v>40</v>
       </c>
-      <c r="AD32" s="432"/>
+      <c r="AD32" s="480"/>
       <c r="AI32" s="230" t="s">
         <v>76</v>
       </c>
@@ -14676,11 +14680,11 @@
         <v>80</v>
       </c>
       <c r="AJ34" s="240">
-        <f t="shared" ref="AJ33:AJ42" si="10">AD20-AD5</f>
+        <f t="shared" ref="AJ34:AJ42" si="10">AD20-AD5</f>
         <v>-4.8291000000000004</v>
       </c>
       <c r="AK34" s="240">
-        <f t="shared" ref="AK33:AK42" si="11">AG20-AG5</f>
+        <f t="shared" ref="AK34:AK42" si="11">AG20-AG5</f>
         <v>-0.45517786187029452</v>
       </c>
       <c r="AL34" s="240">
@@ -15993,46 +15997,46 @@
         <v>100</v>
       </c>
     </row>
-    <row r="51" spans="2:40" ht="15">
-      <c r="AA51" s="437" t="s">
+    <row r="51" spans="2:40">
+      <c r="AA51" s="476" t="s">
         <v>103</v>
       </c>
-      <c r="AB51" s="437"/>
-      <c r="AC51" s="437"/>
-      <c r="AD51" s="437"/>
-      <c r="AE51" s="437"/>
-      <c r="AF51" s="437"/>
-      <c r="AG51" s="437"/>
-      <c r="AH51" s="437"/>
-      <c r="AI51" s="437"/>
-      <c r="AJ51" s="437"/>
-      <c r="AK51" s="437"/>
-      <c r="AL51" s="437"/>
-      <c r="AM51" s="437"/>
-      <c r="AN51" s="437"/>
+      <c r="AB51" s="476"/>
+      <c r="AC51" s="476"/>
+      <c r="AD51" s="476"/>
+      <c r="AE51" s="476"/>
+      <c r="AF51" s="476"/>
+      <c r="AG51" s="476"/>
+      <c r="AH51" s="476"/>
+      <c r="AI51" s="476"/>
+      <c r="AJ51" s="476"/>
+      <c r="AK51" s="476"/>
+      <c r="AL51" s="476"/>
+      <c r="AM51" s="476"/>
+      <c r="AN51" s="476"/>
     </row>
     <row r="52" spans="2:40">
       <c r="AA52" s="56"/>
-      <c r="AB52" s="448" t="s">
+      <c r="AB52" s="477" t="s">
         <v>72</v>
       </c>
-      <c r="AC52" s="448"/>
-      <c r="AD52" s="448"/>
-      <c r="AE52" s="448" t="s">
+      <c r="AC52" s="477"/>
+      <c r="AD52" s="477"/>
+      <c r="AE52" s="477" t="s">
         <v>73</v>
       </c>
-      <c r="AF52" s="448"/>
-      <c r="AG52" s="448"/>
-      <c r="AH52" s="448" t="s">
+      <c r="AF52" s="477"/>
+      <c r="AG52" s="477"/>
+      <c r="AH52" s="477" t="s">
         <v>74</v>
       </c>
-      <c r="AI52" s="448"/>
-      <c r="AJ52" s="448"/>
-      <c r="AK52" s="448" t="s">
+      <c r="AI52" s="477"/>
+      <c r="AJ52" s="477"/>
+      <c r="AK52" s="477" t="s">
         <v>75</v>
       </c>
-      <c r="AL52" s="448"/>
-      <c r="AM52" s="448"/>
+      <c r="AL52" s="477"/>
+      <c r="AM52" s="477"/>
       <c r="AN52" s="56"/>
     </row>
     <row r="53" spans="2:40" ht="15">
@@ -16127,34 +16131,34 @@
       </c>
     </row>
     <row r="55" spans="2:40" ht="15">
-      <c r="B55" s="445" t="s">
+      <c r="B55" s="473" t="s">
         <v>1</v>
       </c>
-      <c r="C55" s="446"/>
-      <c r="D55" s="446"/>
-      <c r="E55" s="446"/>
-      <c r="F55" s="447"/>
-      <c r="G55" s="445" t="s">
+      <c r="C55" s="474"/>
+      <c r="D55" s="474"/>
+      <c r="E55" s="474"/>
+      <c r="F55" s="475"/>
+      <c r="G55" s="473" t="s">
         <v>2</v>
       </c>
-      <c r="H55" s="446"/>
-      <c r="I55" s="446"/>
-      <c r="J55" s="446"/>
-      <c r="K55" s="447"/>
-      <c r="L55" s="445" t="s">
+      <c r="H55" s="474"/>
+      <c r="I55" s="474"/>
+      <c r="J55" s="474"/>
+      <c r="K55" s="475"/>
+      <c r="L55" s="473" t="s">
         <v>3</v>
       </c>
-      <c r="M55" s="446"/>
-      <c r="N55" s="446"/>
-      <c r="O55" s="446"/>
-      <c r="P55" s="447"/>
-      <c r="Q55" s="445" t="s">
+      <c r="M55" s="474"/>
+      <c r="N55" s="474"/>
+      <c r="O55" s="474"/>
+      <c r="P55" s="475"/>
+      <c r="Q55" s="473" t="s">
         <v>4</v>
       </c>
-      <c r="R55" s="446"/>
-      <c r="S55" s="446"/>
-      <c r="T55" s="446"/>
-      <c r="U55" s="447"/>
+      <c r="R55" s="474"/>
+      <c r="S55" s="474"/>
+      <c r="T55" s="474"/>
+      <c r="U55" s="475"/>
       <c r="AA55" s="218" t="s">
         <v>80</v>
       </c>
@@ -17365,20 +17369,20 @@
     </row>
     <row r="69" spans="2:21" ht="15" thickBot="1"/>
     <row r="70" spans="2:21">
-      <c r="B70" s="439" t="s">
+      <c r="B70" s="445" t="s">
         <v>5</v>
       </c>
-      <c r="C70" s="440"/>
-      <c r="D70" s="440"/>
-      <c r="E70" s="440"/>
-      <c r="F70" s="441"/>
-      <c r="G70" s="439" t="s">
+      <c r="C70" s="446"/>
+      <c r="D70" s="446"/>
+      <c r="E70" s="446"/>
+      <c r="F70" s="447"/>
+      <c r="G70" s="445" t="s">
         <v>6</v>
       </c>
-      <c r="H70" s="440"/>
-      <c r="I70" s="440"/>
-      <c r="J70" s="440"/>
-      <c r="K70" s="441"/>
+      <c r="H70" s="446"/>
+      <c r="I70" s="446"/>
+      <c r="J70" s="446"/>
+      <c r="K70" s="447"/>
     </row>
     <row r="71" spans="2:21" ht="15" thickBot="1">
       <c r="B71" s="150" t="s">
@@ -17786,20 +17790,20 @@
     </row>
     <row r="84" spans="2:11" ht="15" thickBot="1"/>
     <row r="85" spans="2:11">
-      <c r="B85" s="442" t="s">
+      <c r="B85" s="470" t="s">
         <v>7</v>
       </c>
-      <c r="C85" s="443"/>
-      <c r="D85" s="443"/>
-      <c r="E85" s="443"/>
-      <c r="F85" s="444"/>
-      <c r="G85" s="442" t="s">
+      <c r="C85" s="471"/>
+      <c r="D85" s="471"/>
+      <c r="E85" s="471"/>
+      <c r="F85" s="472"/>
+      <c r="G85" s="470" t="s">
         <v>8</v>
       </c>
-      <c r="H85" s="443"/>
-      <c r="I85" s="443"/>
-      <c r="J85" s="443"/>
-      <c r="K85" s="444"/>
+      <c r="H85" s="471"/>
+      <c r="I85" s="471"/>
+      <c r="J85" s="471"/>
+      <c r="K85" s="472"/>
     </row>
     <row r="86" spans="2:11" ht="15" thickBot="1">
       <c r="B86" s="173" t="s">
@@ -18209,34 +18213,34 @@
     </row>
     <row r="99" spans="2:21" ht="15" thickBot="1"/>
     <row r="100" spans="2:21">
-      <c r="B100" s="449" t="s">
+      <c r="B100" s="457" t="s">
         <v>9</v>
       </c>
-      <c r="C100" s="450"/>
-      <c r="D100" s="450"/>
-      <c r="E100" s="450"/>
-      <c r="F100" s="451"/>
-      <c r="G100" s="449" t="s">
+      <c r="C100" s="458"/>
+      <c r="D100" s="458"/>
+      <c r="E100" s="458"/>
+      <c r="F100" s="459"/>
+      <c r="G100" s="457" t="s">
         <v>10</v>
       </c>
-      <c r="H100" s="450"/>
-      <c r="I100" s="450"/>
-      <c r="J100" s="450"/>
-      <c r="K100" s="451"/>
-      <c r="L100" s="452" t="s">
+      <c r="H100" s="458"/>
+      <c r="I100" s="458"/>
+      <c r="J100" s="458"/>
+      <c r="K100" s="459"/>
+      <c r="L100" s="460" t="s">
         <v>11</v>
       </c>
-      <c r="M100" s="453"/>
-      <c r="N100" s="453"/>
-      <c r="O100" s="453"/>
-      <c r="P100" s="454"/>
-      <c r="Q100" s="449" t="s">
+      <c r="M100" s="461"/>
+      <c r="N100" s="461"/>
+      <c r="O100" s="461"/>
+      <c r="P100" s="462"/>
+      <c r="Q100" s="457" t="s">
         <v>12</v>
       </c>
-      <c r="R100" s="450"/>
-      <c r="S100" s="450"/>
-      <c r="T100" s="450"/>
-      <c r="U100" s="451"/>
+      <c r="R100" s="458"/>
+      <c r="S100" s="458"/>
+      <c r="T100" s="458"/>
+      <c r="U100" s="459"/>
     </row>
     <row r="101" spans="2:21" ht="15" thickBot="1">
       <c r="B101" s="183" t="s">
@@ -19024,34 +19028,34 @@
     </row>
     <row r="114" spans="2:21" ht="15" thickBot="1"/>
     <row r="115" spans="2:21">
-      <c r="B115" s="455" t="s">
+      <c r="B115" s="463" t="s">
         <v>13</v>
       </c>
-      <c r="C115" s="456"/>
-      <c r="D115" s="456"/>
-      <c r="E115" s="456"/>
-      <c r="F115" s="457"/>
-      <c r="G115" s="455" t="s">
+      <c r="C115" s="464"/>
+      <c r="D115" s="464"/>
+      <c r="E115" s="464"/>
+      <c r="F115" s="465"/>
+      <c r="G115" s="463" t="s">
         <v>14</v>
       </c>
-      <c r="H115" s="456"/>
-      <c r="I115" s="456"/>
-      <c r="J115" s="456"/>
-      <c r="K115" s="457"/>
-      <c r="L115" s="458" t="s">
+      <c r="H115" s="464"/>
+      <c r="I115" s="464"/>
+      <c r="J115" s="464"/>
+      <c r="K115" s="465"/>
+      <c r="L115" s="466" t="s">
         <v>15</v>
       </c>
-      <c r="M115" s="459"/>
-      <c r="N115" s="459"/>
-      <c r="O115" s="459"/>
-      <c r="P115" s="460"/>
-      <c r="Q115" s="455" t="s">
+      <c r="M115" s="467"/>
+      <c r="N115" s="467"/>
+      <c r="O115" s="467"/>
+      <c r="P115" s="468"/>
+      <c r="Q115" s="463" t="s">
         <v>16</v>
       </c>
-      <c r="R115" s="456"/>
-      <c r="S115" s="456"/>
-      <c r="T115" s="456"/>
-      <c r="U115" s="457"/>
+      <c r="R115" s="464"/>
+      <c r="S115" s="464"/>
+      <c r="T115" s="464"/>
+      <c r="U115" s="465"/>
     </row>
     <row r="116" spans="2:21" ht="15" thickBot="1">
       <c r="B116" s="193" t="s">
@@ -19839,34 +19843,34 @@
     </row>
     <row r="129" spans="2:21" ht="15" thickBot="1"/>
     <row r="130" spans="2:21">
-      <c r="B130" s="439" t="s">
+      <c r="B130" s="445" t="s">
         <v>17</v>
       </c>
-      <c r="C130" s="440"/>
-      <c r="D130" s="440"/>
-      <c r="E130" s="440"/>
-      <c r="F130" s="441"/>
-      <c r="G130" s="439" t="s">
+      <c r="C130" s="446"/>
+      <c r="D130" s="446"/>
+      <c r="E130" s="446"/>
+      <c r="F130" s="447"/>
+      <c r="G130" s="445" t="s">
         <v>18</v>
       </c>
-      <c r="H130" s="440"/>
-      <c r="I130" s="440"/>
-      <c r="J130" s="440"/>
-      <c r="K130" s="441"/>
-      <c r="L130" s="461" t="s">
+      <c r="H130" s="446"/>
+      <c r="I130" s="446"/>
+      <c r="J130" s="446"/>
+      <c r="K130" s="447"/>
+      <c r="L130" s="448" t="s">
         <v>19</v>
       </c>
-      <c r="M130" s="462"/>
-      <c r="N130" s="462"/>
-      <c r="O130" s="462"/>
-      <c r="P130" s="463"/>
-      <c r="Q130" s="439" t="s">
+      <c r="M130" s="449"/>
+      <c r="N130" s="449"/>
+      <c r="O130" s="449"/>
+      <c r="P130" s="450"/>
+      <c r="Q130" s="445" t="s">
         <v>20</v>
       </c>
-      <c r="R130" s="440"/>
-      <c r="S130" s="440"/>
-      <c r="T130" s="440"/>
-      <c r="U130" s="441"/>
+      <c r="R130" s="446"/>
+      <c r="S130" s="446"/>
+      <c r="T130" s="446"/>
+      <c r="U130" s="447"/>
     </row>
     <row r="131" spans="2:21" ht="15" thickBot="1">
       <c r="B131" s="150" t="s">
@@ -20654,27 +20658,27 @@
     </row>
     <row r="144" spans="2:21" ht="15" thickBot="1"/>
     <row r="145" spans="2:16">
-      <c r="B145" s="464" t="s">
+      <c r="B145" s="451" t="s">
         <v>21</v>
       </c>
-      <c r="C145" s="465"/>
-      <c r="D145" s="465"/>
-      <c r="E145" s="465"/>
-      <c r="F145" s="466"/>
-      <c r="G145" s="464" t="s">
+      <c r="C145" s="452"/>
+      <c r="D145" s="452"/>
+      <c r="E145" s="452"/>
+      <c r="F145" s="453"/>
+      <c r="G145" s="451" t="s">
         <v>22</v>
       </c>
-      <c r="H145" s="465"/>
-      <c r="I145" s="465"/>
-      <c r="J145" s="465"/>
-      <c r="K145" s="466"/>
-      <c r="L145" s="467" t="s">
+      <c r="H145" s="452"/>
+      <c r="I145" s="452"/>
+      <c r="J145" s="452"/>
+      <c r="K145" s="453"/>
+      <c r="L145" s="454" t="s">
         <v>23</v>
       </c>
-      <c r="M145" s="468"/>
-      <c r="N145" s="468"/>
-      <c r="O145" s="468"/>
-      <c r="P145" s="469"/>
+      <c r="M145" s="455"/>
+      <c r="N145" s="455"/>
+      <c r="O145" s="455"/>
+      <c r="P145" s="456"/>
     </row>
     <row r="146" spans="2:16" ht="15" thickBot="1">
       <c r="B146" s="203" t="s">
@@ -21273,36 +21277,6 @@
     </row>
   </sheetData>
   <mergeCells count="46">
-    <mergeCell ref="B130:F130"/>
-    <mergeCell ref="G130:K130"/>
-    <mergeCell ref="L130:P130"/>
-    <mergeCell ref="Q130:U130"/>
-    <mergeCell ref="B145:F145"/>
-    <mergeCell ref="G145:K145"/>
-    <mergeCell ref="L145:P145"/>
-    <mergeCell ref="B100:F100"/>
-    <mergeCell ref="G100:K100"/>
-    <mergeCell ref="L100:P100"/>
-    <mergeCell ref="Q100:U100"/>
-    <mergeCell ref="B115:F115"/>
-    <mergeCell ref="G115:K115"/>
-    <mergeCell ref="L115:P115"/>
-    <mergeCell ref="Q115:U115"/>
-    <mergeCell ref="AH16:AH17"/>
-    <mergeCell ref="AI16:AI17"/>
-    <mergeCell ref="B70:F70"/>
-    <mergeCell ref="G70:K70"/>
-    <mergeCell ref="B85:F85"/>
-    <mergeCell ref="G85:K85"/>
-    <mergeCell ref="B55:F55"/>
-    <mergeCell ref="G55:K55"/>
-    <mergeCell ref="L55:P55"/>
-    <mergeCell ref="Q55:U55"/>
-    <mergeCell ref="AA51:AN51"/>
-    <mergeCell ref="AB52:AD52"/>
-    <mergeCell ref="AE52:AG52"/>
-    <mergeCell ref="AH52:AJ52"/>
-    <mergeCell ref="AK52:AM52"/>
     <mergeCell ref="AL1:AL2"/>
     <mergeCell ref="AL16:AL17"/>
     <mergeCell ref="AK16:AK17"/>
@@ -21319,6 +21293,36 @@
     <mergeCell ref="AH1:AH2"/>
     <mergeCell ref="AI1:AI2"/>
     <mergeCell ref="AG16:AG17"/>
+    <mergeCell ref="AH16:AH17"/>
+    <mergeCell ref="AI16:AI17"/>
+    <mergeCell ref="B70:F70"/>
+    <mergeCell ref="G70:K70"/>
+    <mergeCell ref="B85:F85"/>
+    <mergeCell ref="G85:K85"/>
+    <mergeCell ref="B55:F55"/>
+    <mergeCell ref="G55:K55"/>
+    <mergeCell ref="L55:P55"/>
+    <mergeCell ref="Q55:U55"/>
+    <mergeCell ref="AA51:AN51"/>
+    <mergeCell ref="AB52:AD52"/>
+    <mergeCell ref="AE52:AG52"/>
+    <mergeCell ref="AH52:AJ52"/>
+    <mergeCell ref="AK52:AM52"/>
+    <mergeCell ref="B100:F100"/>
+    <mergeCell ref="G100:K100"/>
+    <mergeCell ref="L100:P100"/>
+    <mergeCell ref="Q100:U100"/>
+    <mergeCell ref="B115:F115"/>
+    <mergeCell ref="G115:K115"/>
+    <mergeCell ref="L115:P115"/>
+    <mergeCell ref="Q115:U115"/>
+    <mergeCell ref="B130:F130"/>
+    <mergeCell ref="G130:K130"/>
+    <mergeCell ref="L130:P130"/>
+    <mergeCell ref="Q130:U130"/>
+    <mergeCell ref="B145:F145"/>
+    <mergeCell ref="G145:K145"/>
+    <mergeCell ref="L145:P145"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -21330,7 +21334,7 @@
   <dimension ref="B1:BA158"/>
   <sheetViews>
     <sheetView topLeftCell="W1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AN42" sqref="AN42"/>
+      <selection activeCell="AK48" sqref="AK48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -21353,22 +21357,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:53">
-      <c r="AG1" s="436" t="s">
+      <c r="AG1" s="469" t="s">
         <v>56</v>
       </c>
-      <c r="AH1" s="436" t="s">
+      <c r="AH1" s="469" t="s">
         <v>57</v>
       </c>
-      <c r="AI1" s="436" t="s">
+      <c r="AI1" s="469" t="s">
         <v>52</v>
       </c>
-      <c r="AJ1" s="436" t="s">
+      <c r="AJ1" s="469" t="s">
         <v>56</v>
       </c>
-      <c r="AK1" s="436" t="s">
+      <c r="AK1" s="469" t="s">
         <v>57</v>
       </c>
-      <c r="AL1" s="436" t="s">
+      <c r="AL1" s="469" t="s">
         <v>52</v>
       </c>
     </row>
@@ -21445,23 +21449,23 @@
       <c r="Y2" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="AB2" s="433" t="s">
+      <c r="AB2" s="481" t="s">
         <v>25</v>
       </c>
-      <c r="AC2" s="434"/>
-      <c r="AD2" s="437" t="s">
+      <c r="AC2" s="482"/>
+      <c r="AD2" s="476" t="s">
         <v>58</v>
       </c>
-      <c r="AE2" s="437"/>
+      <c r="AE2" s="476"/>
       <c r="AF2" s="429" t="s">
         <v>104</v>
       </c>
-      <c r="AG2" s="436"/>
-      <c r="AH2" s="436"/>
-      <c r="AI2" s="436"/>
-      <c r="AJ2" s="436"/>
-      <c r="AK2" s="436"/>
-      <c r="AL2" s="436"/>
+      <c r="AG2" s="469"/>
+      <c r="AH2" s="469"/>
+      <c r="AI2" s="469"/>
+      <c r="AJ2" s="469"/>
+      <c r="AK2" s="469"/>
+      <c r="AL2" s="469"/>
     </row>
     <row r="3" spans="2:53" ht="15">
       <c r="B3" s="14">
@@ -21657,7 +21661,7 @@
         <f>SUM(C60:C63)</f>
         <v>7.529399999999999</v>
       </c>
-      <c r="AF4" s="483">
+      <c r="AF4" s="433">
         <v>6.2739000000000003</v>
       </c>
       <c r="AG4" s="213">
@@ -21881,7 +21885,7 @@
       <c r="AB6" s="62">
         <v>10.304</v>
       </c>
-      <c r="AC6" s="482">
+      <c r="AC6" s="432">
         <v>-0.3029856615539851</v>
       </c>
       <c r="AD6" s="262">
@@ -21892,7 +21896,7 @@
         <f>SUM(C75:C78)</f>
         <v>7.0016999999999996</v>
       </c>
-      <c r="AF6" s="484">
+      <c r="AF6" s="434">
         <v>4.8148000000000017</v>
       </c>
       <c r="AG6" s="213">
@@ -22237,7 +22241,7 @@
         <f>SUM(R105:R108)</f>
         <v>8.2335999999999991</v>
       </c>
-      <c r="AF9" s="485">
+      <c r="AF9" s="435">
         <v>5.7997999999999958</v>
       </c>
       <c r="AG9" s="213">
@@ -22352,7 +22356,7 @@
         <f>SUM(R120:R123)</f>
         <v>6.8244000000000007</v>
       </c>
-      <c r="AF10" s="486">
+      <c r="AF10" s="436">
         <v>4.7938000000000009</v>
       </c>
       <c r="AG10" s="213">
@@ -22467,7 +22471,7 @@
         <f>SUM(C135:C138)</f>
         <v>7.5085999999999995</v>
       </c>
-      <c r="AF11" s="487">
+      <c r="AF11" s="437">
         <v>5.7195999999999998</v>
       </c>
       <c r="AG11" s="213">
@@ -22582,7 +22586,7 @@
         <f>SUM(R135:R138)</f>
         <v>8.2502999999999993</v>
       </c>
-      <c r="AF12" s="487">
+      <c r="AF12" s="437">
         <v>7.186300000000001</v>
       </c>
       <c r="AG12" s="213">
@@ -22697,7 +22701,7 @@
         <f>SUM(C150:C153)</f>
         <v>9.6692</v>
       </c>
-      <c r="AF13" s="488">
+      <c r="AF13" s="438">
         <v>7.9821999999999989</v>
       </c>
       <c r="AG13" s="213">
@@ -22812,7 +22816,7 @@
         <f>SUM(M150:M153)</f>
         <v>9.2515999999999998</v>
       </c>
-      <c r="AF14" s="489">
+      <c r="AF14" s="439">
         <v>6.5748000000000006</v>
       </c>
       <c r="AG14" s="213">
@@ -22910,22 +22914,22 @@
       <c r="Y15" s="380">
         <v>1.0235026535253984</v>
       </c>
-      <c r="AG15" s="436" t="s">
+      <c r="AG15" s="469" t="s">
         <v>56</v>
       </c>
-      <c r="AH15" s="436" t="s">
+      <c r="AH15" s="469" t="s">
         <v>57</v>
       </c>
-      <c r="AI15" s="436" t="s">
+      <c r="AI15" s="469" t="s">
         <v>52</v>
       </c>
-      <c r="AJ15" s="436" t="s">
+      <c r="AJ15" s="469" t="s">
         <v>56</v>
       </c>
-      <c r="AK15" s="436" t="s">
+      <c r="AK15" s="469" t="s">
         <v>57</v>
       </c>
-      <c r="AL15" s="436" t="s">
+      <c r="AL15" s="469" t="s">
         <v>52</v>
       </c>
     </row>
@@ -23000,23 +23004,23 @@
       <c r="Y16" s="380">
         <v>1.0708870356330553</v>
       </c>
-      <c r="AB16" s="433" t="s">
+      <c r="AB16" s="481" t="s">
         <v>40</v>
       </c>
-      <c r="AC16" s="435"/>
-      <c r="AD16" s="437" t="s">
+      <c r="AC16" s="483"/>
+      <c r="AD16" s="476" t="s">
         <v>58</v>
       </c>
-      <c r="AE16" s="437"/>
+      <c r="AE16" s="476"/>
       <c r="AF16" s="429" t="s">
         <v>104</v>
       </c>
-      <c r="AG16" s="436"/>
-      <c r="AH16" s="436"/>
-      <c r="AI16" s="436"/>
-      <c r="AJ16" s="436"/>
-      <c r="AK16" s="436"/>
-      <c r="AL16" s="436"/>
+      <c r="AG16" s="469"/>
+      <c r="AH16" s="469"/>
+      <c r="AI16" s="469"/>
+      <c r="AJ16" s="469"/>
+      <c r="AK16" s="469"/>
+      <c r="AL16" s="469"/>
     </row>
     <row r="17" spans="2:40" ht="14.45" customHeight="1">
       <c r="B17" s="28">
@@ -23212,7 +23216,7 @@
         <f>SUM(H60:H63)</f>
         <v>8.8132999999999999</v>
       </c>
-      <c r="AF18" s="483">
+      <c r="AF18" s="433">
         <v>7.254999999999999</v>
       </c>
       <c r="AG18" s="88">
@@ -23431,7 +23435,7 @@
       <c r="AB20" s="62">
         <v>15.135</v>
       </c>
-      <c r="AC20" s="482">
+      <c r="AC20" s="432">
         <v>-0.3029856615539851</v>
       </c>
       <c r="AD20" s="216">
@@ -23442,7 +23446,7 @@
         <f>SUM(H75:H78)</f>
         <v>6.6124999999999998</v>
       </c>
-      <c r="AF20" s="484">
+      <c r="AF20" s="434">
         <v>5.5904000000000025</v>
       </c>
       <c r="AG20" s="88">
@@ -23557,7 +23561,7 @@
         <f>SUM(C90:C93)</f>
         <v>3.1219000000000001</v>
       </c>
-      <c r="AF21" s="490">
+      <c r="AF21" s="440">
         <v>2.6214</v>
       </c>
       <c r="AG21" s="88">
@@ -23672,7 +23676,7 @@
         <f>SUM(H105:H108)</f>
         <v>8.4920000000000009</v>
       </c>
-      <c r="AF22" s="491">
+      <c r="AF22" s="441">
         <v>7.4188999999999989</v>
       </c>
       <c r="AG22" s="88">
@@ -24017,7 +24021,7 @@
         <f>SUM(M120:M123)</f>
         <v>5.5735000000000001</v>
       </c>
-      <c r="AF25" s="492">
+      <c r="AF25" s="442">
         <v>5.7463999999999995</v>
       </c>
       <c r="AG25" s="88">
@@ -24247,7 +24251,7 @@
         <f>SUM(M135:M138)</f>
         <v>6.3197999999999999</v>
       </c>
-      <c r="AF27" s="493">
+      <c r="AF27" s="443">
         <v>6.9350000000000014</v>
       </c>
       <c r="AG27" s="88">
@@ -24362,7 +24366,7 @@
         <f>SUM(H150:H153)</f>
         <v>9.8343000000000007</v>
       </c>
-      <c r="AF28" s="494">
+      <c r="AF28" s="444">
         <v>8.6735999999999969</v>
       </c>
       <c r="AG28" s="88">
@@ -24605,14 +24609,14 @@
       <c r="Y31" s="380">
         <v>6.6148597422289619</v>
       </c>
-      <c r="AA31" s="431" t="s">
+      <c r="AA31" s="479" t="s">
         <v>25</v>
       </c>
-      <c r="AB31" s="431"/>
-      <c r="AC31" s="432" t="s">
+      <c r="AB31" s="479"/>
+      <c r="AC31" s="480" t="s">
         <v>40</v>
       </c>
-      <c r="AD31" s="432"/>
+      <c r="AD31" s="480"/>
       <c r="AJ31" s="230" t="s">
         <v>76</v>
       </c>
@@ -24816,7 +24820,7 @@
         <v>8.8132999999999999</v>
       </c>
       <c r="AD33" s="87">
-        <f>AG18</f>
+        <f t="shared" ref="AD33:AD43" si="9">AG18</f>
         <v>2.6834120292299035</v>
       </c>
       <c r="AJ33" s="231" t="s">
@@ -24915,15 +24919,15 @@
         <v>8.8132999999999999</v>
       </c>
       <c r="AB34" s="86">
-        <f t="shared" ref="AB33:AB43" si="9">AG5</f>
+        <f t="shared" ref="AB34:AB42" si="10">AG5</f>
         <v>1.5015923261390882</v>
       </c>
       <c r="AC34" s="66">
-        <f t="shared" ref="AC34:AC43" si="10">AE19</f>
+        <f t="shared" ref="AC34:AC43" si="11">AE19</f>
         <v>11.34998</v>
       </c>
       <c r="AD34" s="87">
-        <f>AG19</f>
+        <f t="shared" si="9"/>
         <v>2.1372765808871073</v>
       </c>
       <c r="AJ34" s="232" t="s">
@@ -25022,15 +25026,15 @@
         <v>7.0016999999999996</v>
       </c>
       <c r="AB35" s="86">
+        <f t="shared" si="10"/>
+        <v>1.4248532844281436</v>
+      </c>
+      <c r="AC35" s="66">
+        <f t="shared" si="11"/>
+        <v>6.6124999999999998</v>
+      </c>
+      <c r="AD35" s="87">
         <f t="shared" si="9"/>
-        <v>1.4248532844281436</v>
-      </c>
-      <c r="AC35" s="66">
-        <f t="shared" si="10"/>
-        <v>6.6124999999999998</v>
-      </c>
-      <c r="AD35" s="87">
-        <f>AG20</f>
         <v>1.3819777993151134</v>
       </c>
       <c r="AJ35" s="233" t="s">
@@ -25129,15 +25133,15 @@
         <v>11.661999999999999</v>
       </c>
       <c r="AB36" s="86">
+        <f t="shared" si="10"/>
+        <v>2.1933442953020137</v>
+      </c>
+      <c r="AC36" s="66">
+        <f t="shared" si="11"/>
+        <v>3.1219000000000001</v>
+      </c>
+      <c r="AD36" s="87">
         <f t="shared" si="9"/>
-        <v>2.1933442953020137</v>
-      </c>
-      <c r="AC36" s="66">
-        <f t="shared" si="10"/>
-        <v>3.1219000000000001</v>
-      </c>
-      <c r="AD36" s="87">
-        <f>AG21</f>
         <v>0.22430094050296454</v>
       </c>
       <c r="AJ36" s="234" t="s">
@@ -25236,15 +25240,15 @@
         <v>10.2044</v>
       </c>
       <c r="AB37" s="86">
+        <f t="shared" si="10"/>
+        <v>1.4338855542216893</v>
+      </c>
+      <c r="AC37" s="66">
+        <f t="shared" si="11"/>
+        <v>8.4920000000000009</v>
+      </c>
+      <c r="AD37" s="87">
         <f t="shared" si="9"/>
-        <v>1.4338855542216893</v>
-      </c>
-      <c r="AC37" s="66">
-        <f t="shared" si="10"/>
-        <v>8.4920000000000009</v>
-      </c>
-      <c r="AD37" s="87">
-        <f>AG22</f>
         <v>1.5524268675721558</v>
       </c>
       <c r="AJ37" s="234" t="s">
@@ -25343,15 +25347,15 @@
         <v>8.2335999999999991</v>
       </c>
       <c r="AB38" s="86">
+        <f t="shared" si="10"/>
+        <v>0.18830519480519459</v>
+      </c>
+      <c r="AC38" s="66">
+        <f t="shared" si="11"/>
+        <v>5.7622000000000009</v>
+      </c>
+      <c r="AD38" s="87">
         <f t="shared" si="9"/>
-        <v>0.18830519480519459</v>
-      </c>
-      <c r="AC38" s="66">
-        <f t="shared" si="10"/>
-        <v>5.7622000000000009</v>
-      </c>
-      <c r="AD38" s="87">
-        <f>AG23</f>
         <v>0.39358079181663208</v>
       </c>
       <c r="AJ38" s="235" t="s">
@@ -25362,11 +25366,11 @@
         <v>-5.5202999999999998</v>
       </c>
       <c r="AL38" s="240">
-        <f t="shared" ref="AL38:AM40" si="11">AG25-AG10</f>
+        <f t="shared" ref="AL38:AM40" si="12">AG25-AG10</f>
         <v>0.25186380023202659</v>
       </c>
       <c r="AM38" s="240">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.65548799899290877</v>
       </c>
       <c r="AN38" s="240">
@@ -25450,15 +25454,15 @@
         <v>6.8244000000000007</v>
       </c>
       <c r="AB39" s="86">
+        <f t="shared" si="10"/>
+        <v>1.0619606931600436</v>
+      </c>
+      <c r="AC39" s="66">
+        <f t="shared" si="11"/>
+        <v>11.0939</v>
+      </c>
+      <c r="AD39" s="87">
         <f t="shared" si="9"/>
-        <v>1.0619606931600436</v>
-      </c>
-      <c r="AC39" s="66">
-        <f t="shared" si="10"/>
-        <v>11.0939</v>
-      </c>
-      <c r="AD39" s="87">
-        <f>AG24</f>
         <v>1.1808994277400584</v>
       </c>
       <c r="AJ39" s="236" t="s">
@@ -25469,11 +25473,11 @@
         <v>-2.0448999999999997</v>
       </c>
       <c r="AL39" s="240">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1.849413921397858</v>
       </c>
       <c r="AM39" s="240">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.63760360773591351</v>
       </c>
       <c r="AN39" s="240">
@@ -25557,15 +25561,15 @@
         <v>7.5085999999999995</v>
       </c>
       <c r="AB40" s="86">
+        <f t="shared" si="10"/>
+        <v>1.1471216953218717</v>
+      </c>
+      <c r="AC40" s="66">
+        <f t="shared" si="11"/>
+        <v>5.5735000000000001</v>
+      </c>
+      <c r="AD40" s="87">
         <f t="shared" si="9"/>
-        <v>1.1471216953218717</v>
-      </c>
-      <c r="AC40" s="66">
-        <f t="shared" si="10"/>
-        <v>5.5735000000000001</v>
-      </c>
-      <c r="AD40" s="87">
-        <f>AG25</f>
         <v>1.3138244933920702</v>
       </c>
       <c r="AJ40" s="236" t="s">
@@ -25576,11 +25580,11 @@
         <v>-0.77380000000000015</v>
       </c>
       <c r="AL40" s="240">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>-0.87190683761703458</v>
       </c>
       <c r="AM40" s="240">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.51081309197247027</v>
       </c>
       <c r="AN40" s="240">
@@ -25664,15 +25668,15 @@
         <v>8.2502999999999993</v>
       </c>
       <c r="AB41" s="86">
+        <f t="shared" si="10"/>
+        <v>1.2975845869776486</v>
+      </c>
+      <c r="AC41" s="66">
+        <f t="shared" si="11"/>
+        <v>8.8879999999999999</v>
+      </c>
+      <c r="AD41" s="87">
         <f t="shared" si="9"/>
-        <v>1.2975845869776486</v>
-      </c>
-      <c r="AC41" s="66">
-        <f t="shared" si="10"/>
-        <v>8.8879999999999999</v>
-      </c>
-      <c r="AD41" s="87">
-        <f>AG26</f>
         <v>2.9965356167197297</v>
       </c>
       <c r="AJ41" s="237" t="s">
@@ -25771,15 +25775,15 @@
         <v>9.6692</v>
       </c>
       <c r="AB42" s="86">
+        <f t="shared" si="10"/>
+        <v>0.16300764991896269</v>
+      </c>
+      <c r="AC42" s="66">
+        <f t="shared" si="11"/>
+        <v>6.3197999999999999</v>
+      </c>
+      <c r="AD42" s="87">
         <f t="shared" si="9"/>
-        <v>0.16300764991896269</v>
-      </c>
-      <c r="AC42" s="66">
-        <f t="shared" si="10"/>
-        <v>6.3197999999999999</v>
-      </c>
-      <c r="AD42" s="87">
-        <f>AG27</f>
         <v>0.42567774936061398</v>
       </c>
     </row>
@@ -25863,11 +25867,11 @@
         <v>2.2325159590598944</v>
       </c>
       <c r="AC43" s="66">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>9.8343000000000007</v>
       </c>
       <c r="AD43" s="87">
-        <f>AG28</f>
+        <f t="shared" si="9"/>
         <v>1.3266062144692778</v>
       </c>
     </row>
@@ -26169,34 +26173,34 @@
     </row>
     <row r="54" spans="2:21" ht="15" thickBot="1"/>
     <row r="55" spans="2:21">
-      <c r="B55" s="470" t="s">
+      <c r="B55" s="485" t="s">
         <v>1</v>
       </c>
-      <c r="C55" s="471"/>
-      <c r="D55" s="471"/>
-      <c r="E55" s="471"/>
-      <c r="F55" s="472"/>
-      <c r="G55" s="470" t="s">
+      <c r="C55" s="486"/>
+      <c r="D55" s="486"/>
+      <c r="E55" s="486"/>
+      <c r="F55" s="487"/>
+      <c r="G55" s="485" t="s">
         <v>2</v>
       </c>
-      <c r="H55" s="471"/>
-      <c r="I55" s="471"/>
-      <c r="J55" s="471"/>
-      <c r="K55" s="472"/>
-      <c r="L55" s="470" t="s">
+      <c r="H55" s="486"/>
+      <c r="I55" s="486"/>
+      <c r="J55" s="486"/>
+      <c r="K55" s="487"/>
+      <c r="L55" s="485" t="s">
         <v>3</v>
       </c>
-      <c r="M55" s="471"/>
-      <c r="N55" s="471"/>
-      <c r="O55" s="471"/>
-      <c r="P55" s="472"/>
-      <c r="Q55" s="470" t="s">
+      <c r="M55" s="486"/>
+      <c r="N55" s="486"/>
+      <c r="O55" s="486"/>
+      <c r="P55" s="487"/>
+      <c r="Q55" s="485" t="s">
         <v>4</v>
       </c>
-      <c r="R55" s="471"/>
-      <c r="S55" s="471"/>
-      <c r="T55" s="471"/>
-      <c r="U55" s="472"/>
+      <c r="R55" s="486"/>
+      <c r="S55" s="486"/>
+      <c r="T55" s="486"/>
+      <c r="U55" s="487"/>
     </row>
     <row r="56" spans="2:21" ht="15" thickBot="1">
       <c r="B56" s="92" t="s">
@@ -26984,20 +26988,20 @@
     </row>
     <row r="69" spans="2:21" ht="15" thickBot="1"/>
     <row r="70" spans="2:21">
-      <c r="B70" s="461" t="s">
+      <c r="B70" s="448" t="s">
         <v>95</v>
       </c>
-      <c r="C70" s="462"/>
-      <c r="D70" s="462"/>
-      <c r="E70" s="462"/>
-      <c r="F70" s="463"/>
-      <c r="G70" s="461" t="s">
+      <c r="C70" s="449"/>
+      <c r="D70" s="449"/>
+      <c r="E70" s="449"/>
+      <c r="F70" s="450"/>
+      <c r="G70" s="448" t="s">
         <v>6</v>
       </c>
-      <c r="H70" s="462"/>
-      <c r="I70" s="462"/>
-      <c r="J70" s="462"/>
-      <c r="K70" s="463"/>
+      <c r="H70" s="449"/>
+      <c r="I70" s="449"/>
+      <c r="J70" s="449"/>
+      <c r="K70" s="450"/>
     </row>
     <row r="71" spans="2:21" ht="15" thickBot="1">
       <c r="B71" s="150" t="s">
@@ -27405,20 +27409,20 @@
     </row>
     <row r="84" spans="2:11" ht="15" thickBot="1"/>
     <row r="85" spans="2:11">
-      <c r="B85" s="473" t="s">
+      <c r="B85" s="488" t="s">
         <v>7</v>
       </c>
-      <c r="C85" s="474"/>
-      <c r="D85" s="474"/>
-      <c r="E85" s="474"/>
-      <c r="F85" s="475"/>
-      <c r="G85" s="473" t="s">
+      <c r="C85" s="489"/>
+      <c r="D85" s="489"/>
+      <c r="E85" s="489"/>
+      <c r="F85" s="490"/>
+      <c r="G85" s="488" t="s">
         <v>8</v>
       </c>
-      <c r="H85" s="474"/>
-      <c r="I85" s="474"/>
-      <c r="J85" s="474"/>
-      <c r="K85" s="475"/>
+      <c r="H85" s="489"/>
+      <c r="I85" s="489"/>
+      <c r="J85" s="489"/>
+      <c r="K85" s="490"/>
     </row>
     <row r="86" spans="2:11" ht="15" thickBot="1">
       <c r="B86" s="173" t="s">
@@ -27828,34 +27832,34 @@
     </row>
     <row r="99" spans="2:21" ht="15" thickBot="1"/>
     <row r="100" spans="2:21">
-      <c r="B100" s="452" t="s">
+      <c r="B100" s="460" t="s">
         <v>9</v>
       </c>
-      <c r="C100" s="453"/>
-      <c r="D100" s="453"/>
-      <c r="E100" s="453"/>
-      <c r="F100" s="454"/>
-      <c r="G100" s="452" t="s">
+      <c r="C100" s="461"/>
+      <c r="D100" s="461"/>
+      <c r="E100" s="461"/>
+      <c r="F100" s="462"/>
+      <c r="G100" s="460" t="s">
         <v>10</v>
       </c>
-      <c r="H100" s="453"/>
-      <c r="I100" s="453"/>
-      <c r="J100" s="453"/>
-      <c r="K100" s="454"/>
-      <c r="L100" s="452" t="s">
+      <c r="H100" s="461"/>
+      <c r="I100" s="461"/>
+      <c r="J100" s="461"/>
+      <c r="K100" s="462"/>
+      <c r="L100" s="460" t="s">
         <v>11</v>
       </c>
-      <c r="M100" s="453"/>
-      <c r="N100" s="453"/>
-      <c r="O100" s="453"/>
-      <c r="P100" s="454"/>
-      <c r="Q100" s="452" t="s">
+      <c r="M100" s="461"/>
+      <c r="N100" s="461"/>
+      <c r="O100" s="461"/>
+      <c r="P100" s="462"/>
+      <c r="Q100" s="460" t="s">
         <v>12</v>
       </c>
-      <c r="R100" s="453"/>
-      <c r="S100" s="453"/>
-      <c r="T100" s="453"/>
-      <c r="U100" s="454"/>
+      <c r="R100" s="461"/>
+      <c r="S100" s="461"/>
+      <c r="T100" s="461"/>
+      <c r="U100" s="462"/>
     </row>
     <row r="101" spans="2:21" ht="15" thickBot="1">
       <c r="B101" s="183" t="s">
@@ -28643,34 +28647,34 @@
     </row>
     <row r="114" spans="2:21" ht="15" thickBot="1"/>
     <row r="115" spans="2:21">
-      <c r="B115" s="455" t="s">
+      <c r="B115" s="463" t="s">
         <v>13</v>
       </c>
-      <c r="C115" s="456"/>
-      <c r="D115" s="456"/>
-      <c r="E115" s="456"/>
-      <c r="F115" s="457"/>
-      <c r="G115" s="458" t="s">
+      <c r="C115" s="464"/>
+      <c r="D115" s="464"/>
+      <c r="E115" s="464"/>
+      <c r="F115" s="465"/>
+      <c r="G115" s="466" t="s">
         <v>14</v>
       </c>
-      <c r="H115" s="459"/>
-      <c r="I115" s="459"/>
-      <c r="J115" s="459"/>
-      <c r="K115" s="460"/>
-      <c r="L115" s="458" t="s">
+      <c r="H115" s="467"/>
+      <c r="I115" s="467"/>
+      <c r="J115" s="467"/>
+      <c r="K115" s="468"/>
+      <c r="L115" s="466" t="s">
         <v>15</v>
       </c>
-      <c r="M115" s="459"/>
-      <c r="N115" s="459"/>
-      <c r="O115" s="459"/>
-      <c r="P115" s="460"/>
-      <c r="Q115" s="458" t="s">
+      <c r="M115" s="467"/>
+      <c r="N115" s="467"/>
+      <c r="O115" s="467"/>
+      <c r="P115" s="468"/>
+      <c r="Q115" s="466" t="s">
         <v>16</v>
       </c>
-      <c r="R115" s="459"/>
-      <c r="S115" s="459"/>
-      <c r="T115" s="459"/>
-      <c r="U115" s="460"/>
+      <c r="R115" s="467"/>
+      <c r="S115" s="467"/>
+      <c r="T115" s="467"/>
+      <c r="U115" s="468"/>
     </row>
     <row r="116" spans="2:21" ht="15" thickBot="1">
       <c r="B116" s="193" t="s">
@@ -29342,34 +29346,34 @@
     </row>
     <row r="129" spans="2:21" ht="15" thickBot="1"/>
     <row r="130" spans="2:21">
-      <c r="B130" s="461" t="s">
+      <c r="B130" s="448" t="s">
         <v>17</v>
       </c>
-      <c r="C130" s="462"/>
-      <c r="D130" s="462"/>
-      <c r="E130" s="462"/>
-      <c r="F130" s="463"/>
-      <c r="G130" s="461" t="s">
+      <c r="C130" s="449"/>
+      <c r="D130" s="449"/>
+      <c r="E130" s="449"/>
+      <c r="F130" s="450"/>
+      <c r="G130" s="448" t="s">
         <v>18</v>
       </c>
-      <c r="H130" s="462"/>
-      <c r="I130" s="462"/>
-      <c r="J130" s="462"/>
-      <c r="K130" s="463"/>
-      <c r="L130" s="461" t="s">
+      <c r="H130" s="449"/>
+      <c r="I130" s="449"/>
+      <c r="J130" s="449"/>
+      <c r="K130" s="450"/>
+      <c r="L130" s="448" t="s">
         <v>19</v>
       </c>
-      <c r="M130" s="462"/>
-      <c r="N130" s="462"/>
-      <c r="O130" s="462"/>
-      <c r="P130" s="463"/>
-      <c r="Q130" s="461" t="s">
+      <c r="M130" s="449"/>
+      <c r="N130" s="449"/>
+      <c r="O130" s="449"/>
+      <c r="P130" s="450"/>
+      <c r="Q130" s="448" t="s">
         <v>20</v>
       </c>
-      <c r="R130" s="462"/>
-      <c r="S130" s="462"/>
-      <c r="T130" s="462"/>
-      <c r="U130" s="463"/>
+      <c r="R130" s="449"/>
+      <c r="S130" s="449"/>
+      <c r="T130" s="449"/>
+      <c r="U130" s="450"/>
     </row>
     <row r="131" spans="2:21" ht="15" thickBot="1">
       <c r="B131" s="150" t="s">
@@ -30157,27 +30161,27 @@
     </row>
     <row r="144" spans="2:21" ht="15" thickBot="1"/>
     <row r="145" spans="2:16">
-      <c r="B145" s="467" t="s">
+      <c r="B145" s="454" t="s">
         <v>21</v>
       </c>
-      <c r="C145" s="468"/>
-      <c r="D145" s="468"/>
-      <c r="E145" s="468"/>
-      <c r="F145" s="469"/>
-      <c r="G145" s="467" t="s">
+      <c r="C145" s="455"/>
+      <c r="D145" s="455"/>
+      <c r="E145" s="455"/>
+      <c r="F145" s="456"/>
+      <c r="G145" s="454" t="s">
         <v>22</v>
       </c>
-      <c r="H145" s="468"/>
-      <c r="I145" s="468"/>
-      <c r="J145" s="468"/>
-      <c r="K145" s="469"/>
-      <c r="L145" s="467" t="s">
+      <c r="H145" s="455"/>
+      <c r="I145" s="455"/>
+      <c r="J145" s="455"/>
+      <c r="K145" s="456"/>
+      <c r="L145" s="454" t="s">
         <v>23</v>
       </c>
-      <c r="M145" s="468"/>
-      <c r="N145" s="468"/>
-      <c r="O145" s="468"/>
-      <c r="P145" s="469"/>
+      <c r="M145" s="455"/>
+      <c r="N145" s="455"/>
+      <c r="O145" s="455"/>
+      <c r="P145" s="456"/>
     </row>
     <row r="146" spans="2:16" ht="15" thickBot="1">
       <c r="B146" s="203" t="s">
@@ -30776,17 +30780,24 @@
     </row>
   </sheetData>
   <mergeCells count="41">
-    <mergeCell ref="B145:F145"/>
-    <mergeCell ref="G145:K145"/>
-    <mergeCell ref="L145:P145"/>
-    <mergeCell ref="B115:F115"/>
-    <mergeCell ref="G115:K115"/>
-    <mergeCell ref="L115:P115"/>
-    <mergeCell ref="Q115:U115"/>
-    <mergeCell ref="B130:F130"/>
-    <mergeCell ref="G130:K130"/>
-    <mergeCell ref="L130:P130"/>
-    <mergeCell ref="Q130:U130"/>
+    <mergeCell ref="AL1:AL2"/>
+    <mergeCell ref="AB2:AC2"/>
+    <mergeCell ref="AD2:AE2"/>
+    <mergeCell ref="AG1:AG2"/>
+    <mergeCell ref="AH1:AH2"/>
+    <mergeCell ref="AI1:AI2"/>
+    <mergeCell ref="AJ1:AJ2"/>
+    <mergeCell ref="AK1:AK2"/>
+    <mergeCell ref="AK15:AK16"/>
+    <mergeCell ref="AL15:AL16"/>
+    <mergeCell ref="AB16:AC16"/>
+    <mergeCell ref="AD16:AE16"/>
+    <mergeCell ref="AA31:AB31"/>
+    <mergeCell ref="AC31:AD31"/>
+    <mergeCell ref="AJ15:AJ16"/>
+    <mergeCell ref="AG15:AG16"/>
+    <mergeCell ref="AH15:AH16"/>
+    <mergeCell ref="AI15:AI16"/>
     <mergeCell ref="Q100:U100"/>
     <mergeCell ref="B55:F55"/>
     <mergeCell ref="G55:K55"/>
@@ -30799,24 +30810,17 @@
     <mergeCell ref="B100:F100"/>
     <mergeCell ref="G100:K100"/>
     <mergeCell ref="L100:P100"/>
-    <mergeCell ref="AK15:AK16"/>
-    <mergeCell ref="AL15:AL16"/>
-    <mergeCell ref="AB16:AC16"/>
-    <mergeCell ref="AD16:AE16"/>
-    <mergeCell ref="AA31:AB31"/>
-    <mergeCell ref="AC31:AD31"/>
-    <mergeCell ref="AJ15:AJ16"/>
-    <mergeCell ref="AG15:AG16"/>
-    <mergeCell ref="AH15:AH16"/>
-    <mergeCell ref="AI15:AI16"/>
-    <mergeCell ref="AL1:AL2"/>
-    <mergeCell ref="AB2:AC2"/>
-    <mergeCell ref="AD2:AE2"/>
-    <mergeCell ref="AG1:AG2"/>
-    <mergeCell ref="AH1:AH2"/>
-    <mergeCell ref="AI1:AI2"/>
-    <mergeCell ref="AJ1:AJ2"/>
-    <mergeCell ref="AK1:AK2"/>
+    <mergeCell ref="Q115:U115"/>
+    <mergeCell ref="B130:F130"/>
+    <mergeCell ref="G130:K130"/>
+    <mergeCell ref="L130:P130"/>
+    <mergeCell ref="Q130:U130"/>
+    <mergeCell ref="B145:F145"/>
+    <mergeCell ref="G145:K145"/>
+    <mergeCell ref="L145:P145"/>
+    <mergeCell ref="B115:F115"/>
+    <mergeCell ref="G115:K115"/>
+    <mergeCell ref="L115:P115"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -30827,8 +30831,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1F56B83-6FD0-4F97-A83F-B325F07CC791}">
   <dimension ref="A1:N40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M44" sqref="M44"/>
+    <sheetView tabSelected="1" topLeftCell="E23" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="X5" sqref="X5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -30846,46 +30850,46 @@
     <col min="14" max="14" width="12.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15.75" thickBot="1">
-      <c r="A1" s="437" t="s">
+    <row r="1" spans="1:14" ht="15" thickBot="1">
+      <c r="A1" s="476" t="s">
         <v>96</v>
       </c>
-      <c r="B1" s="479"/>
-      <c r="C1" s="479"/>
-      <c r="D1" s="479"/>
-      <c r="E1" s="479"/>
-      <c r="F1" s="479"/>
-      <c r="G1" s="479"/>
-      <c r="H1" s="479"/>
-      <c r="I1" s="479"/>
-      <c r="J1" s="479"/>
-      <c r="K1" s="479"/>
-      <c r="L1" s="479"/>
-      <c r="M1" s="479"/>
-      <c r="N1" s="437"/>
-    </row>
-    <row r="2" spans="1:14" ht="15">
+      <c r="B1" s="491"/>
+      <c r="C1" s="491"/>
+      <c r="D1" s="491"/>
+      <c r="E1" s="491"/>
+      <c r="F1" s="491"/>
+      <c r="G1" s="491"/>
+      <c r="H1" s="491"/>
+      <c r="I1" s="491"/>
+      <c r="J1" s="491"/>
+      <c r="K1" s="491"/>
+      <c r="L1" s="491"/>
+      <c r="M1" s="491"/>
+      <c r="N1" s="476"/>
+    </row>
+    <row r="2" spans="1:14">
       <c r="A2" s="229"/>
-      <c r="B2" s="476" t="s">
-        <v>72</v>
-      </c>
-      <c r="C2" s="477"/>
-      <c r="D2" s="478"/>
-      <c r="E2" s="476" t="s">
-        <v>73</v>
-      </c>
-      <c r="F2" s="477"/>
-      <c r="G2" s="478"/>
-      <c r="H2" s="476" t="s">
-        <v>74</v>
-      </c>
-      <c r="I2" s="477"/>
-      <c r="J2" s="478"/>
-      <c r="K2" s="476" t="s">
+      <c r="B2" s="492" t="s">
+        <v>111</v>
+      </c>
+      <c r="C2" s="493"/>
+      <c r="D2" s="494"/>
+      <c r="E2" s="492" t="s">
+        <v>108</v>
+      </c>
+      <c r="F2" s="493"/>
+      <c r="G2" s="494"/>
+      <c r="H2" s="492" t="s">
+        <v>110</v>
+      </c>
+      <c r="I2" s="493"/>
+      <c r="J2" s="494"/>
+      <c r="K2" s="492" t="s">
         <v>75</v>
       </c>
-      <c r="L2" s="477"/>
-      <c r="M2" s="478"/>
+      <c r="L2" s="493"/>
+      <c r="M2" s="494"/>
       <c r="N2" s="246"/>
     </row>
     <row r="3" spans="1:14" ht="15">
@@ -31504,46 +31508,46 @@
         <v>-3.2730377491297959E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="15.75" thickBot="1">
-      <c r="A16" s="437" t="s">
+    <row r="16" spans="1:14" ht="15" thickBot="1">
+      <c r="A16" s="476" t="s">
         <v>106</v>
       </c>
-      <c r="B16" s="479"/>
-      <c r="C16" s="479"/>
-      <c r="D16" s="479"/>
-      <c r="E16" s="479"/>
-      <c r="F16" s="479"/>
-      <c r="G16" s="479"/>
-      <c r="H16" s="479"/>
-      <c r="I16" s="479"/>
-      <c r="J16" s="479"/>
-      <c r="K16" s="479"/>
-      <c r="L16" s="479"/>
-      <c r="M16" s="479"/>
-      <c r="N16" s="437"/>
-    </row>
-    <row r="17" spans="1:14" ht="15">
+      <c r="B16" s="491"/>
+      <c r="C16" s="491"/>
+      <c r="D16" s="491"/>
+      <c r="E16" s="491"/>
+      <c r="F16" s="491"/>
+      <c r="G16" s="491"/>
+      <c r="H16" s="491"/>
+      <c r="I16" s="491"/>
+      <c r="J16" s="491"/>
+      <c r="K16" s="491"/>
+      <c r="L16" s="491"/>
+      <c r="M16" s="491"/>
+      <c r="N16" s="476"/>
+    </row>
+    <row r="17" spans="1:14">
       <c r="A17" s="229"/>
-      <c r="B17" s="476" t="s">
-        <v>72</v>
-      </c>
-      <c r="C17" s="477"/>
-      <c r="D17" s="478"/>
-      <c r="E17" s="476" t="s">
-        <v>73</v>
-      </c>
-      <c r="F17" s="477"/>
-      <c r="G17" s="478"/>
-      <c r="H17" s="476" t="s">
-        <v>74</v>
-      </c>
-      <c r="I17" s="477"/>
-      <c r="J17" s="478"/>
-      <c r="K17" s="476" t="s">
+      <c r="B17" s="492" t="s">
+        <v>111</v>
+      </c>
+      <c r="C17" s="493"/>
+      <c r="D17" s="494"/>
+      <c r="E17" s="492" t="s">
+        <v>109</v>
+      </c>
+      <c r="F17" s="493"/>
+      <c r="G17" s="494"/>
+      <c r="H17" s="492" t="s">
+        <v>110</v>
+      </c>
+      <c r="I17" s="493"/>
+      <c r="J17" s="494"/>
+      <c r="K17" s="492" t="s">
         <v>75</v>
       </c>
-      <c r="L17" s="477"/>
-      <c r="M17" s="478"/>
+      <c r="L17" s="493"/>
+      <c r="M17" s="494"/>
       <c r="N17" s="246"/>
     </row>
     <row r="18" spans="1:14" ht="15">
@@ -31634,7 +31638,7 @@
       <c r="L19" s="86">
         <v>0.20310881995133825</v>
       </c>
-      <c r="M19" s="480">
+      <c r="M19" s="430">
         <f>K19/L19</f>
         <v>0.18061966240201743</v>
       </c>
@@ -31686,7 +31690,7 @@
       <c r="L20" s="86">
         <v>0.24768143380032806</v>
       </c>
-      <c r="M20" s="480">
+      <c r="M20" s="430">
         <f t="shared" ref="M20:M27" si="7">K20/L20</f>
         <v>0.45650263746076064</v>
       </c>
@@ -31738,11 +31742,11 @@
       <c r="L21" s="220">
         <v>0.18703707902634226</v>
       </c>
-      <c r="M21" s="480">
+      <c r="M21" s="430">
         <f t="shared" si="7"/>
         <v>0.25528328492852753</v>
       </c>
-      <c r="N21" s="482">
+      <c r="N21" s="432">
         <v>-0.32001589401318498</v>
       </c>
     </row>
@@ -31790,7 +31794,7 @@
       <c r="L22" s="87">
         <v>0.45884337735094055</v>
       </c>
-      <c r="M22" s="480">
+      <c r="M22" s="430">
         <f t="shared" si="7"/>
         <v>-0.2142122573951242</v>
       </c>
@@ -31842,7 +31846,7 @@
       <c r="L23" s="87">
         <v>0.53364981622151375</v>
       </c>
-      <c r="M23" s="480">
+      <c r="M23" s="430">
         <f t="shared" si="7"/>
         <v>-0.12091619396052283</v>
       </c>
@@ -31894,7 +31898,7 @@
       <c r="L24" s="226">
         <v>0.23523687411480473</v>
       </c>
-      <c r="M24" s="480">
+      <c r="M24" s="430">
         <f t="shared" si="7"/>
         <v>0.19235164956740658</v>
       </c>
@@ -31946,7 +31950,7 @@
       <c r="L25" s="221">
         <v>0.27809010795681738</v>
       </c>
-      <c r="M25" s="480">
+      <c r="M25" s="430">
         <f t="shared" si="7"/>
         <v>6.9338931211544927E-2</v>
       </c>
@@ -31998,7 +32002,7 @@
       <c r="L26" s="221">
         <v>0.3598969808875932</v>
       </c>
-      <c r="M26" s="480">
+      <c r="M26" s="430">
         <f t="shared" si="7"/>
         <v>0.30506992688237528</v>
       </c>
@@ -32050,7 +32054,7 @@
       <c r="L27" s="245">
         <v>0.28163472327520855</v>
       </c>
-      <c r="M27" s="481">
+      <c r="M27" s="431">
         <f t="shared" si="7"/>
         <v>0.73881089123312471</v>
       </c>
@@ -32058,46 +32062,46 @@
         <v>-4.9570413884485784E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:14" ht="15.75" thickBot="1">
-      <c r="A30" s="437" t="s">
+    <row r="30" spans="1:14" ht="15" thickBot="1">
+      <c r="A30" s="476" t="s">
         <v>107</v>
       </c>
-      <c r="B30" s="479"/>
-      <c r="C30" s="479"/>
-      <c r="D30" s="479"/>
-      <c r="E30" s="479"/>
-      <c r="F30" s="479"/>
-      <c r="G30" s="479"/>
-      <c r="H30" s="479"/>
-      <c r="I30" s="479"/>
-      <c r="J30" s="479"/>
-      <c r="K30" s="479"/>
-      <c r="L30" s="479"/>
-      <c r="M30" s="479"/>
-      <c r="N30" s="437"/>
-    </row>
-    <row r="31" spans="1:14" ht="15">
+      <c r="B30" s="491"/>
+      <c r="C30" s="491"/>
+      <c r="D30" s="491"/>
+      <c r="E30" s="491"/>
+      <c r="F30" s="491"/>
+      <c r="G30" s="491"/>
+      <c r="H30" s="491"/>
+      <c r="I30" s="491"/>
+      <c r="J30" s="491"/>
+      <c r="K30" s="491"/>
+      <c r="L30" s="491"/>
+      <c r="M30" s="491"/>
+      <c r="N30" s="476"/>
+    </row>
+    <row r="31" spans="1:14">
       <c r="A31" s="229"/>
-      <c r="B31" s="476" t="s">
-        <v>72</v>
-      </c>
-      <c r="C31" s="477"/>
-      <c r="D31" s="478"/>
-      <c r="E31" s="476" t="s">
-        <v>73</v>
-      </c>
-      <c r="F31" s="477"/>
-      <c r="G31" s="478"/>
-      <c r="H31" s="476" t="s">
-        <v>74</v>
-      </c>
-      <c r="I31" s="477"/>
-      <c r="J31" s="478"/>
-      <c r="K31" s="476" t="s">
+      <c r="B31" s="492" t="s">
+        <v>111</v>
+      </c>
+      <c r="C31" s="493"/>
+      <c r="D31" s="494"/>
+      <c r="E31" s="492" t="s">
+        <v>109</v>
+      </c>
+      <c r="F31" s="493"/>
+      <c r="G31" s="494"/>
+      <c r="H31" s="492" t="s">
+        <v>110</v>
+      </c>
+      <c r="I31" s="493"/>
+      <c r="J31" s="494"/>
+      <c r="K31" s="492" t="s">
         <v>75</v>
       </c>
-      <c r="L31" s="477"/>
-      <c r="M31" s="478"/>
+      <c r="L31" s="493"/>
+      <c r="M31" s="494"/>
       <c r="N31" s="246"/>
     </row>
     <row r="32" spans="1:14" ht="15">
@@ -32181,7 +32185,7 @@
       <c r="L33" s="86">
         <v>0.20310881995133825</v>
       </c>
-      <c r="M33" s="480">
+      <c r="M33" s="430">
         <v>0.18061966240201743</v>
       </c>
       <c r="N33" s="388">
@@ -32225,10 +32229,10 @@
       <c r="L34" s="220">
         <v>0.18703707902634226</v>
       </c>
-      <c r="M34" s="480">
+      <c r="M34" s="430">
         <v>0.25528328492852753</v>
       </c>
-      <c r="N34" s="482">
+      <c r="N34" s="432">
         <v>-0.32001589401318498</v>
       </c>
     </row>
@@ -32269,7 +32273,7 @@
       <c r="L35" s="87">
         <v>0.45884337735094055</v>
       </c>
-      <c r="M35" s="480">
+      <c r="M35" s="430">
         <v>-0.2142122573951242</v>
       </c>
       <c r="N35" s="390">
@@ -32313,7 +32317,7 @@
       <c r="L36" s="87">
         <v>0.53364981622151375</v>
       </c>
-      <c r="M36" s="480">
+      <c r="M36" s="430">
         <v>-0.12091619396052283</v>
       </c>
       <c r="N36" s="390">
@@ -32357,7 +32361,7 @@
       <c r="L37" s="226">
         <v>0.23523687411480473</v>
       </c>
-      <c r="M37" s="480">
+      <c r="M37" s="430">
         <v>0.19235164956740658</v>
       </c>
       <c r="N37" s="226">
@@ -32401,7 +32405,7 @@
       <c r="L38" s="221">
         <v>0.27809010795681738</v>
       </c>
-      <c r="M38" s="480">
+      <c r="M38" s="430">
         <v>6.9338931211544927E-2</v>
       </c>
       <c r="N38" s="389">
@@ -32445,7 +32449,7 @@
       <c r="L39" s="221">
         <v>0.3598969808875932</v>
       </c>
-      <c r="M39" s="480">
+      <c r="M39" s="430">
         <v>0.30506992688237528</v>
       </c>
       <c r="N39" s="389">
@@ -32489,7 +32493,7 @@
       <c r="L40" s="245">
         <v>0.28163472327520855</v>
       </c>
-      <c r="M40" s="481">
+      <c r="M40" s="431">
         <v>0.73881089123312471</v>
       </c>
       <c r="N40" s="391">
@@ -32498,11 +32502,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="A30:N30"/>
-    <mergeCell ref="B31:D31"/>
-    <mergeCell ref="E31:G31"/>
-    <mergeCell ref="H31:J31"/>
-    <mergeCell ref="K31:M31"/>
     <mergeCell ref="B17:D17"/>
     <mergeCell ref="E17:G17"/>
     <mergeCell ref="H17:J17"/>
@@ -32513,6 +32512,11 @@
     <mergeCell ref="H2:J2"/>
     <mergeCell ref="K2:M2"/>
     <mergeCell ref="A16:N16"/>
+    <mergeCell ref="A30:N30"/>
+    <mergeCell ref="B31:D31"/>
+    <mergeCell ref="E31:G31"/>
+    <mergeCell ref="H31:J31"/>
+    <mergeCell ref="K31:M31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
LOI analysis with different GSD
</commit_message>
<xml_diff>
--- a/GSD/baskets_new_sizes/basketGSD_hypflux_NEW_SIZES.xlsx
+++ b/GSD/baskets_new_sizes/basketGSD_hypflux_NEW_SIZES.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\huck4481\Documents\GitHub\La_Jara\GSD\baskets_new_sizes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1F7AC3F-710B-4DB0-84EB-CC2007DED5D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04C664CC-530D-4E1A-B265-28E4F4E46996}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{FF2C68C4-0230-4397-BD30-01ABAA0FCBBF}"/>
+    <workbookView xWindow="-25320" yWindow="195" windowWidth="25440" windowHeight="15390" xr2:uid="{FF2C68C4-0230-4397-BD30-01ABAA0FCBBF}"/>
   </bookViews>
   <sheets>
     <sheet name="Spring Weights" sheetId="1" r:id="rId1"/>
@@ -35,6 +35,28 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -385,7 +407,7 @@
     <numFmt numFmtId="165" formatCode="0.0000"/>
     <numFmt numFmtId="166" formatCode="0.00000"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1244,7 +1266,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="495">
+  <cellXfs count="496">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2572,126 +2594,126 @@
     <xf numFmtId="2" fontId="3" fillId="26" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="31" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="31" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="31" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="31" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="31" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="31" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="38" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="38" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="38" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="38" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="38" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="38" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="29" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="29" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="29" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="29" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="29" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="29" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="36" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="36" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="36" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="36" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="36" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="36" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="28" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="30" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="30" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="30" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="28" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="31" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="31" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="31" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="30" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="30" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="30" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="29" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="29" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="29" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="29" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="29" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="29" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="31" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="31" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="31" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="30" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2710,18 +2732,19 @@
     <xf numFmtId="0" fontId="0" fillId="33" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -11013,49 +11036,49 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{695C6E5A-89DB-4EF6-9D1B-F4A1EC0E0EDD}">
   <dimension ref="B1:AN158"/>
   <sheetViews>
-    <sheetView topLeftCell="U1" zoomScale="76" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AJ11" sqref="AJ11"/>
+    <sheetView tabSelected="1" topLeftCell="U1" zoomScale="76" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AK28" sqref="AK28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="15.75" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" customWidth="1"/>
     <col min="27" max="27" width="18" customWidth="1"/>
-    <col min="28" max="28" width="22.5" customWidth="1"/>
+    <col min="28" max="28" width="22.42578125" customWidth="1"/>
     <col min="29" max="29" width="19" customWidth="1"/>
-    <col min="30" max="30" width="18.625" customWidth="1"/>
-    <col min="31" max="31" width="16.75" customWidth="1"/>
-    <col min="32" max="32" width="19.125" customWidth="1"/>
-    <col min="33" max="33" width="20.875" customWidth="1"/>
-    <col min="34" max="34" width="17.375" customWidth="1"/>
-    <col min="35" max="35" width="20.25" customWidth="1"/>
-    <col min="36" max="36" width="18.25" customWidth="1"/>
+    <col min="30" max="30" width="18.5703125" customWidth="1"/>
+    <col min="31" max="31" width="16.7109375" customWidth="1"/>
+    <col min="32" max="32" width="19.140625" customWidth="1"/>
+    <col min="33" max="33" width="20.85546875" customWidth="1"/>
+    <col min="34" max="34" width="17.42578125" customWidth="1"/>
+    <col min="35" max="35" width="20.28515625" customWidth="1"/>
+    <col min="36" max="36" width="18.28515625" customWidth="1"/>
     <col min="37" max="37" width="17" customWidth="1"/>
-    <col min="38" max="38" width="14.5" customWidth="1"/>
-    <col min="39" max="39" width="14.625" customWidth="1"/>
+    <col min="38" max="38" width="14.42578125" customWidth="1"/>
+    <col min="39" max="39" width="14.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:38" ht="14.45" customHeight="1">
-      <c r="AG1" s="469" t="s">
+    <row r="1" spans="2:40" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AG1" s="451" t="s">
         <v>56</v>
       </c>
-      <c r="AH1" s="469" t="s">
+      <c r="AH1" s="451" t="s">
         <v>57</v>
       </c>
-      <c r="AI1" s="469" t="s">
+      <c r="AI1" s="451" t="s">
         <v>52</v>
       </c>
-      <c r="AJ1" s="469" t="s">
+      <c r="AJ1" s="451" t="s">
         <v>56</v>
       </c>
-      <c r="AK1" s="478" t="s">
+      <c r="AK1" s="445" t="s">
         <v>57</v>
       </c>
-      <c r="AL1" s="478" t="s">
+      <c r="AL1" s="445" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="2:38" ht="15.75" thickBot="1">
+    <row r="2" spans="2:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -11128,25 +11151,25 @@
       <c r="Y2" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="AB2" s="481" t="s">
+      <c r="AB2" s="448" t="s">
         <v>25</v>
       </c>
-      <c r="AC2" s="482"/>
-      <c r="AD2" s="476" t="s">
+      <c r="AC2" s="449"/>
+      <c r="AD2" s="452" t="s">
         <v>58</v>
       </c>
-      <c r="AE2" s="476"/>
+      <c r="AE2" s="452"/>
       <c r="AF2" s="97" t="s">
         <v>104</v>
       </c>
-      <c r="AG2" s="484"/>
-      <c r="AH2" s="469"/>
-      <c r="AI2" s="469"/>
-      <c r="AJ2" s="469"/>
-      <c r="AK2" s="478"/>
-      <c r="AL2" s="478"/>
-    </row>
-    <row r="3" spans="2:38" ht="15">
+      <c r="AG2" s="453"/>
+      <c r="AH2" s="451"/>
+      <c r="AI2" s="451"/>
+      <c r="AJ2" s="451"/>
+      <c r="AK2" s="445"/>
+      <c r="AL2" s="445"/>
+    </row>
+    <row r="3" spans="2:40" x14ac:dyDescent="0.25">
       <c r="B3" s="14">
         <v>0.37</v>
       </c>
@@ -11254,7 +11277,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="4" spans="2:38" ht="15">
+    <row r="4" spans="2:40" x14ac:dyDescent="0.25">
       <c r="B4" s="28">
         <v>0.44</v>
       </c>
@@ -11370,8 +11393,12 @@
       <c r="AL4" s="85">
         <v>4.4862982062414796</v>
       </c>
-    </row>
-    <row r="5" spans="2:38" ht="15">
+      <c r="AN4" s="495" cm="1">
+        <f t="array" ref="AN4">SUM(AD4:AE4+AH4:AI4)</f>
+        <v>48.180706785417371</v>
+      </c>
+    </row>
+    <row r="5" spans="2:40" x14ac:dyDescent="0.25">
       <c r="B5" s="28">
         <v>0.52</v>
       </c>
@@ -11487,8 +11514,12 @@
       <c r="AL5" s="85">
         <v>4.6747701009495621</v>
       </c>
-    </row>
-    <row r="6" spans="2:38" ht="15">
+      <c r="AN5" s="495" cm="1">
+        <f t="array" ref="AN5">SUM(AD5:AE5+AH5:AI5)</f>
+        <v>28.887846869065235</v>
+      </c>
+    </row>
+    <row r="6" spans="2:40" x14ac:dyDescent="0.25">
       <c r="B6" s="28">
         <v>0.61</v>
       </c>
@@ -11604,8 +11635,12 @@
       <c r="AL6" s="85">
         <v>4.5354006526071435</v>
       </c>
-    </row>
-    <row r="7" spans="2:38" ht="15">
+      <c r="AN6" s="495" cm="1">
+        <f t="array" ref="AN6">SUM(AD6:AE6+AH6:AI6)</f>
+        <v>48.912455571250248</v>
+      </c>
+    </row>
+    <row r="7" spans="2:40" x14ac:dyDescent="0.25">
       <c r="B7" s="28">
         <v>0.72</v>
       </c>
@@ -11721,8 +11756,12 @@
       <c r="AL7" s="85">
         <v>4.7942747635056886</v>
       </c>
-    </row>
-    <row r="8" spans="2:38" ht="15">
+      <c r="AN7" s="495" cm="1">
+        <f t="array" ref="AN7">SUM(AD7:AE7+AH7:AI7)</f>
+        <v>39.847631152605949</v>
+      </c>
+    </row>
+    <row r="8" spans="2:40" x14ac:dyDescent="0.25">
       <c r="B8" s="28">
         <v>0.85</v>
       </c>
@@ -11838,8 +11877,12 @@
       <c r="AL8" s="85">
         <v>5.2577078294667103</v>
       </c>
-    </row>
-    <row r="9" spans="2:38" ht="15">
+      <c r="AN8" s="495" cm="1">
+        <f t="array" ref="AN8">SUM(AD8:AE8+AH8:AI8)</f>
+        <v>58.127101424893439</v>
+      </c>
+    </row>
+    <row r="9" spans="2:40" x14ac:dyDescent="0.25">
       <c r="B9" s="28">
         <v>1.01</v>
       </c>
@@ -11955,8 +11998,12 @@
       <c r="AL9" s="85">
         <v>5.6995853735103816</v>
       </c>
-    </row>
-    <row r="10" spans="2:38" ht="15">
+      <c r="AN9" s="495" cm="1">
+        <f t="array" ref="AN9">SUM(AD9:AE9+AH9:AI9)</f>
+        <v>29.51974094446777</v>
+      </c>
+    </row>
+    <row r="10" spans="2:40" x14ac:dyDescent="0.25">
       <c r="B10" s="28">
         <v>1.19</v>
       </c>
@@ -12072,8 +12119,12 @@
       <c r="AL10" s="85">
         <v>5.7620190171509806</v>
       </c>
-    </row>
-    <row r="11" spans="2:38" ht="15">
+      <c r="AN10" s="495" cm="1">
+        <f t="array" ref="AN10">SUM(AD10:AE10+AH10:AI10)</f>
+        <v>66.459687570129446</v>
+      </c>
+    </row>
+    <row r="11" spans="2:40" x14ac:dyDescent="0.25">
       <c r="B11" s="28">
         <v>1.4</v>
       </c>
@@ -12189,8 +12240,12 @@
       <c r="AL11" s="85">
         <v>5.4028394533867061</v>
       </c>
-    </row>
-    <row r="12" spans="2:38" ht="15">
+      <c r="AN11" s="495" cm="1">
+        <f t="array" ref="AN11">SUM(AD11:AE11+AH11:AI11)</f>
+        <v>33.068215224776033</v>
+      </c>
+    </row>
+    <row r="12" spans="2:40" x14ac:dyDescent="0.25">
       <c r="B12" s="28">
         <v>1.65</v>
       </c>
@@ -12306,8 +12361,12 @@
       <c r="AL12" s="85">
         <v>4.0131920254947007</v>
       </c>
-    </row>
-    <row r="13" spans="2:38" ht="15.75" thickBot="1">
+      <c r="AN12" s="495" cm="1">
+        <f t="array" ref="AN12">SUM(AD12:AE12+AH12:AI12)</f>
+        <v>22.221924752228428</v>
+      </c>
+    </row>
+    <row r="13" spans="2:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="42">
         <v>1.95</v>
       </c>
@@ -12423,8 +12482,12 @@
       <c r="AL13" s="85">
         <v>4.1655882664049999</v>
       </c>
-    </row>
-    <row r="14" spans="2:38" ht="15">
+      <c r="AN13" s="495" cm="1">
+        <f t="array" ref="AN13">SUM(AD13:AE13+AH13:AI13)</f>
+        <v>17.67739723854514</v>
+      </c>
+    </row>
+    <row r="14" spans="2:40" x14ac:dyDescent="0.25">
       <c r="B14" s="28">
         <v>2.2999999999999998</v>
       </c>
@@ -12540,8 +12603,12 @@
       <c r="AL14" s="85">
         <v>4.4084484937594492</v>
       </c>
-    </row>
-    <row r="15" spans="2:38" ht="15">
+      <c r="AN14" s="495" cm="1">
+        <f t="array" ref="AN14">SUM(AD14:AE14+AH14:AI14)</f>
+        <v>25.409342136325719</v>
+      </c>
+    </row>
+    <row r="15" spans="2:40" x14ac:dyDescent="0.25">
       <c r="B15" s="28">
         <v>2.72</v>
       </c>
@@ -12657,8 +12724,12 @@
       <c r="AL15" s="85">
         <v>4.116314199395771</v>
       </c>
-    </row>
-    <row r="16" spans="2:38" ht="14.45" customHeight="1" thickBot="1">
+      <c r="AN15" s="495" cm="1">
+        <f t="array" ref="AN15">SUM(AD15:AE15+AH15:AI15)</f>
+        <v>36.023819541895307</v>
+      </c>
+    </row>
+    <row r="16" spans="2:40" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="28">
         <v>3.2</v>
       </c>
@@ -12731,26 +12802,27 @@
       <c r="Y16" s="41">
         <v>1.1583636475738333</v>
       </c>
-      <c r="AG16" s="469" t="s">
+      <c r="AG16" s="451" t="s">
         <v>56</v>
       </c>
-      <c r="AH16" s="469" t="s">
+      <c r="AH16" s="451" t="s">
         <v>57</v>
       </c>
-      <c r="AI16" s="469" t="s">
+      <c r="AI16" s="451" t="s">
         <v>52</v>
       </c>
-      <c r="AJ16" s="469" t="s">
+      <c r="AJ16" s="451" t="s">
         <v>56</v>
       </c>
-      <c r="AK16" s="478" t="s">
+      <c r="AK16" s="445" t="s">
         <v>57</v>
       </c>
-      <c r="AL16" s="478" t="s">
+      <c r="AL16" s="445" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="17" spans="2:39" ht="14.45" customHeight="1">
+      <c r="AN16" s="495"/>
+    </row>
+    <row r="17" spans="2:40" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="28">
         <v>3.78</v>
       </c>
@@ -12823,25 +12895,26 @@
       <c r="Y17" s="41">
         <v>1.2284974412725813</v>
       </c>
-      <c r="AB17" s="481" t="s">
+      <c r="AB17" s="448" t="s">
         <v>40</v>
       </c>
-      <c r="AC17" s="483"/>
-      <c r="AD17" s="476" t="s">
+      <c r="AC17" s="450"/>
+      <c r="AD17" s="452" t="s">
         <v>58</v>
       </c>
-      <c r="AE17" s="476"/>
+      <c r="AE17" s="452"/>
       <c r="AF17" s="261" t="s">
         <v>104</v>
       </c>
-      <c r="AG17" s="469"/>
-      <c r="AH17" s="469"/>
-      <c r="AI17" s="469"/>
-      <c r="AJ17" s="469"/>
-      <c r="AK17" s="478"/>
-      <c r="AL17" s="478"/>
-    </row>
-    <row r="18" spans="2:39" ht="15">
+      <c r="AG17" s="451"/>
+      <c r="AH17" s="451"/>
+      <c r="AI17" s="451"/>
+      <c r="AJ17" s="451"/>
+      <c r="AK17" s="445"/>
+      <c r="AL17" s="445"/>
+      <c r="AN17" s="495"/>
+    </row>
+    <row r="18" spans="2:40" x14ac:dyDescent="0.25">
       <c r="B18" s="28">
         <v>4.46</v>
       </c>
@@ -12948,8 +13021,9 @@
       <c r="AL18" s="57" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="19" spans="2:39" ht="15">
+      <c r="AN18" s="495"/>
+    </row>
+    <row r="19" spans="2:40" x14ac:dyDescent="0.25">
       <c r="B19" s="28">
         <v>5.27</v>
       </c>
@@ -13065,8 +13139,12 @@
       <c r="AL19" s="85">
         <v>4.5587550186087658</v>
       </c>
-    </row>
-    <row r="20" spans="2:39" ht="15">
+      <c r="AN19" s="495" cm="1">
+        <f t="array" ref="AN19">SUM(AD19:AE19+AH19:AI19)</f>
+        <v>28.846378390799789</v>
+      </c>
+    </row>
+    <row r="20" spans="2:40" x14ac:dyDescent="0.25">
       <c r="B20" s="28">
         <v>6.21</v>
       </c>
@@ -13182,8 +13260,12 @@
       <c r="AL20" s="85">
         <v>3.9878514411911556</v>
       </c>
-    </row>
-    <row r="21" spans="2:39" ht="15">
+      <c r="AN20" s="495" cm="1">
+        <f t="array" ref="AN20">SUM(AD20:AE20+AH20:AI20)</f>
+        <v>14.902324730935526</v>
+      </c>
+    </row>
+    <row r="21" spans="2:40" x14ac:dyDescent="0.25">
       <c r="B21" s="28">
         <v>7.33</v>
       </c>
@@ -13299,8 +13381,12 @@
       <c r="AL21" s="85">
         <v>4.1099541035384686</v>
       </c>
-    </row>
-    <row r="22" spans="2:39" ht="15">
+      <c r="AN21" s="495" cm="1">
+        <f t="array" ref="AN21">SUM(AD21:AE21+AH21:AI21)</f>
+        <v>73.801494687854699</v>
+      </c>
+    </row>
+    <row r="22" spans="2:40" x14ac:dyDescent="0.25">
       <c r="B22" s="28">
         <v>8.65</v>
       </c>
@@ -13416,8 +13502,12 @@
       <c r="AL22" s="85">
         <v>4.9294166633087526</v>
       </c>
-    </row>
-    <row r="23" spans="2:39" ht="15">
+      <c r="AN22" s="495" cm="1">
+        <f t="array" ref="AN22">SUM(AD22:AE22+AH22:AI22)</f>
+        <v>49.675701073636795</v>
+      </c>
+    </row>
+    <row r="23" spans="2:40" x14ac:dyDescent="0.25">
       <c r="B23" s="28">
         <v>10.210000000000001</v>
       </c>
@@ -13533,8 +13623,12 @@
       <c r="AL23" s="85">
         <v>5.1075992693696532</v>
       </c>
-    </row>
-    <row r="24" spans="2:39" ht="15">
+      <c r="AN23" s="495" cm="1">
+        <f t="array" ref="AN23">SUM(AD23:AE23+AH23:AI23)</f>
+        <v>33.295728027070957</v>
+      </c>
+    </row>
+    <row r="24" spans="2:40" x14ac:dyDescent="0.25">
       <c r="B24" s="28">
         <v>12.05</v>
       </c>
@@ -13650,8 +13744,12 @@
       <c r="AL24" s="85">
         <v>4.0737324532326404</v>
       </c>
-    </row>
-    <row r="25" spans="2:39" ht="15">
+      <c r="AN24" s="495" cm="1">
+        <f t="array" ref="AN24">SUM(AD24:AE24+AH24:AI24)</f>
+        <v>24.878892112529908</v>
+      </c>
+    </row>
+    <row r="25" spans="2:40" x14ac:dyDescent="0.25">
       <c r="B25" s="28">
         <v>14.22</v>
       </c>
@@ -13767,8 +13865,12 @@
       <c r="AL25" s="85">
         <v>5.3576987503520641</v>
       </c>
-    </row>
-    <row r="26" spans="2:39" ht="15">
+      <c r="AN25" s="495" cm="1">
+        <f t="array" ref="AN25">SUM(AD25:AE25+AH25:AI25)</f>
+        <v>65.287934787055846</v>
+      </c>
+    </row>
+    <row r="26" spans="2:40" x14ac:dyDescent="0.25">
       <c r="B26" s="28">
         <v>16.78</v>
       </c>
@@ -13884,8 +13986,12 @@
       <c r="AL26" s="85">
         <v>5.1676289024362116</v>
       </c>
-    </row>
-    <row r="27" spans="2:39" ht="15">
+      <c r="AN26" s="495" cm="1">
+        <f t="array" ref="AN26">SUM(AD26:AE26+AH26:AI26)</f>
+        <v>30.923717364063375</v>
+      </c>
+    </row>
+    <row r="27" spans="2:40" x14ac:dyDescent="0.25">
       <c r="B27" s="28">
         <v>19.809999999999999</v>
       </c>
@@ -14001,8 +14107,12 @@
       <c r="AL27" s="85">
         <v>4.2478099958744497</v>
       </c>
-    </row>
-    <row r="28" spans="2:39" ht="15">
+      <c r="AN27" s="495" cm="1">
+        <f t="array" ref="AN27">SUM(AD27:AE27+AH27:AI27)</f>
+        <v>26.182885506373523</v>
+      </c>
+    </row>
+    <row r="28" spans="2:40" x14ac:dyDescent="0.25">
       <c r="B28" s="28">
         <v>23.37</v>
       </c>
@@ -14118,8 +14228,12 @@
       <c r="AL28" s="85">
         <v>3.8645229263535508</v>
       </c>
-    </row>
-    <row r="29" spans="2:39" ht="15.75" thickBot="1">
+      <c r="AN28" s="495" cm="1">
+        <f t="array" ref="AN28">SUM(AD28:AE28+AH28:AI28)</f>
+        <v>15.496677710150983</v>
+      </c>
+    </row>
+    <row r="29" spans="2:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B29" s="28">
         <v>27.58</v>
       </c>
@@ -14235,8 +14349,12 @@
       <c r="AL29" s="85">
         <v>4.1952896284577506</v>
       </c>
-    </row>
-    <row r="30" spans="2:39" ht="15">
+      <c r="AN29" s="495" cm="1">
+        <f t="array" ref="AN29">SUM(AD29:AE29+AH29:AI29)</f>
+        <v>32.100596932897439</v>
+      </c>
+    </row>
+    <row r="30" spans="2:40" x14ac:dyDescent="0.25">
       <c r="B30" s="28">
         <v>32.549999999999997</v>
       </c>
@@ -14310,7 +14428,7 @@
         <v>5.6565602071644365</v>
       </c>
     </row>
-    <row r="31" spans="2:39" ht="15">
+    <row r="31" spans="2:40" x14ac:dyDescent="0.25">
       <c r="B31" s="28">
         <v>38.409999999999997</v>
       </c>
@@ -14385,7 +14503,7 @@
       </c>
       <c r="AG31" s="83"/>
     </row>
-    <row r="32" spans="2:39" ht="15">
+    <row r="32" spans="2:40" x14ac:dyDescent="0.25">
       <c r="B32" s="28">
         <v>45.32</v>
       </c>
@@ -14458,14 +14576,14 @@
       <c r="Y32" s="41">
         <v>6.9971946482520506</v>
       </c>
-      <c r="AA32" s="479" t="s">
+      <c r="AA32" s="446" t="s">
         <v>25</v>
       </c>
-      <c r="AB32" s="479"/>
-      <c r="AC32" s="480" t="s">
+      <c r="AB32" s="446"/>
+      <c r="AC32" s="447" t="s">
         <v>40</v>
       </c>
-      <c r="AD32" s="480"/>
+      <c r="AD32" s="447"/>
       <c r="AI32" s="230" t="s">
         <v>76</v>
       </c>
@@ -14482,7 +14600,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="33" spans="2:39" ht="15.75" thickBot="1">
+    <row r="33" spans="2:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B33" s="28">
         <v>53.48</v>
       </c>
@@ -14587,7 +14705,7 @@
         <v>-3.1232600058148624E-2</v>
       </c>
     </row>
-    <row r="34" spans="2:39" ht="15">
+    <row r="34" spans="2:39" x14ac:dyDescent="0.25">
       <c r="B34" s="14">
         <v>63.11</v>
       </c>
@@ -14696,7 +14814,7 @@
         <v>-8.6593108308677155E-2</v>
       </c>
     </row>
-    <row r="35" spans="2:39" ht="15">
+    <row r="35" spans="2:39" x14ac:dyDescent="0.25">
       <c r="B35" s="28">
         <v>74.48</v>
       </c>
@@ -14805,7 +14923,7 @@
         <v>6.5999564974747599E-2</v>
       </c>
     </row>
-    <row r="36" spans="2:39" ht="15">
+    <row r="36" spans="2:39" x14ac:dyDescent="0.25">
       <c r="B36" s="28">
         <v>87.89</v>
       </c>
@@ -14914,7 +15032,7 @@
         <v>0.11179122774730278</v>
       </c>
     </row>
-    <row r="37" spans="2:39" ht="15">
+    <row r="37" spans="2:39" x14ac:dyDescent="0.25">
       <c r="B37" s="28">
         <v>103.72</v>
       </c>
@@ -15023,7 +15141,7 @@
         <v>-0.17582642709759408</v>
       </c>
     </row>
-    <row r="38" spans="2:39" ht="15">
+    <row r="38" spans="2:39" x14ac:dyDescent="0.25">
       <c r="B38" s="28">
         <v>122.39</v>
       </c>
@@ -15132,7 +15250,7 @@
         <v>-0.11171399488573321</v>
       </c>
     </row>
-    <row r="39" spans="2:39" ht="15">
+    <row r="39" spans="2:39" x14ac:dyDescent="0.25">
       <c r="B39" s="28">
         <v>144.43</v>
       </c>
@@ -15241,7 +15359,7 @@
         <v>-7.121946965890269E-2</v>
       </c>
     </row>
-    <row r="40" spans="2:39" ht="15">
+    <row r="40" spans="2:39" x14ac:dyDescent="0.25">
       <c r="B40" s="28">
         <v>170.44</v>
       </c>
@@ -15350,7 +15468,7 @@
         <v>4.7038602982888728E-2</v>
       </c>
     </row>
-    <row r="41" spans="2:39" ht="15">
+    <row r="41" spans="2:39" x14ac:dyDescent="0.25">
       <c r="B41" s="28">
         <v>201.13</v>
       </c>
@@ -15459,7 +15577,7 @@
         <v>4.5512412826442646E-2</v>
       </c>
     </row>
-    <row r="42" spans="2:39" ht="15">
+    <row r="42" spans="2:39" x14ac:dyDescent="0.25">
       <c r="B42" s="28">
         <v>237.35</v>
       </c>
@@ -15568,7 +15686,7 @@
         <v>1.1007356080440442E-2</v>
       </c>
     </row>
-    <row r="43" spans="2:39" ht="15">
+    <row r="43" spans="2:39" x14ac:dyDescent="0.25">
       <c r="B43" s="28">
         <v>280.08999999999997</v>
       </c>
@@ -15677,7 +15795,7 @@
         <v>-2.1770204424107042E-2</v>
       </c>
     </row>
-    <row r="44" spans="2:39" ht="15">
+    <row r="44" spans="2:39" x14ac:dyDescent="0.25">
       <c r="B44" s="28">
         <v>330.52</v>
       </c>
@@ -15767,7 +15885,7 @@
         <v>0.58440306710255763</v>
       </c>
     </row>
-    <row r="45" spans="2:39" ht="15">
+    <row r="45" spans="2:39" x14ac:dyDescent="0.25">
       <c r="B45" s="28">
         <v>390.04</v>
       </c>
@@ -15849,7 +15967,7 @@
         <v>0.89478045810468942</v>
       </c>
     </row>
-    <row r="46" spans="2:39" ht="15.75" thickBot="1">
+    <row r="46" spans="2:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B46" s="42">
         <v>460.27</v>
       </c>
@@ -15923,7 +16041,7 @@
         <v>0.86202910167087976</v>
       </c>
     </row>
-    <row r="47" spans="2:39" ht="15">
+    <row r="47" spans="2:39" x14ac:dyDescent="0.25">
       <c r="B47" s="1" t="s">
         <v>24</v>
       </c>
@@ -15997,49 +16115,49 @@
         <v>100</v>
       </c>
     </row>
-    <row r="51" spans="2:40">
-      <c r="AA51" s="476" t="s">
+    <row r="51" spans="2:40" x14ac:dyDescent="0.25">
+      <c r="AA51" s="452" t="s">
         <v>103</v>
       </c>
-      <c r="AB51" s="476"/>
-      <c r="AC51" s="476"/>
-      <c r="AD51" s="476"/>
-      <c r="AE51" s="476"/>
-      <c r="AF51" s="476"/>
-      <c r="AG51" s="476"/>
-      <c r="AH51" s="476"/>
-      <c r="AI51" s="476"/>
-      <c r="AJ51" s="476"/>
-      <c r="AK51" s="476"/>
-      <c r="AL51" s="476"/>
-      <c r="AM51" s="476"/>
-      <c r="AN51" s="476"/>
-    </row>
-    <row r="52" spans="2:40">
+      <c r="AB51" s="452"/>
+      <c r="AC51" s="452"/>
+      <c r="AD51" s="452"/>
+      <c r="AE51" s="452"/>
+      <c r="AF51" s="452"/>
+      <c r="AG51" s="452"/>
+      <c r="AH51" s="452"/>
+      <c r="AI51" s="452"/>
+      <c r="AJ51" s="452"/>
+      <c r="AK51" s="452"/>
+      <c r="AL51" s="452"/>
+      <c r="AM51" s="452"/>
+      <c r="AN51" s="452"/>
+    </row>
+    <row r="52" spans="2:40" x14ac:dyDescent="0.25">
       <c r="AA52" s="56"/>
-      <c r="AB52" s="477" t="s">
+      <c r="AB52" s="463" t="s">
         <v>72</v>
       </c>
-      <c r="AC52" s="477"/>
-      <c r="AD52" s="477"/>
-      <c r="AE52" s="477" t="s">
+      <c r="AC52" s="463"/>
+      <c r="AD52" s="463"/>
+      <c r="AE52" s="463" t="s">
         <v>73</v>
       </c>
-      <c r="AF52" s="477"/>
-      <c r="AG52" s="477"/>
-      <c r="AH52" s="477" t="s">
+      <c r="AF52" s="463"/>
+      <c r="AG52" s="463"/>
+      <c r="AH52" s="463" t="s">
         <v>74</v>
       </c>
-      <c r="AI52" s="477"/>
-      <c r="AJ52" s="477"/>
-      <c r="AK52" s="477" t="s">
+      <c r="AI52" s="463"/>
+      <c r="AJ52" s="463"/>
+      <c r="AK52" s="463" t="s">
         <v>75</v>
       </c>
-      <c r="AL52" s="477"/>
-      <c r="AM52" s="477"/>
+      <c r="AL52" s="463"/>
+      <c r="AM52" s="463"/>
       <c r="AN52" s="56"/>
     </row>
-    <row r="53" spans="2:40" ht="15">
+    <row r="53" spans="2:40" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
         <v>94</v>
       </c>
@@ -16086,7 +16204,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="54" spans="2:40" ht="15.75" thickBot="1">
+    <row r="54" spans="2:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="AA54" s="218" t="s">
         <v>79</v>
       </c>
@@ -16130,35 +16248,35 @@
         <v>0.22851828638601948</v>
       </c>
     </row>
-    <row r="55" spans="2:40" ht="15">
-      <c r="B55" s="473" t="s">
+    <row r="55" spans="2:40" x14ac:dyDescent="0.25">
+      <c r="B55" s="460" t="s">
         <v>1</v>
       </c>
-      <c r="C55" s="474"/>
-      <c r="D55" s="474"/>
-      <c r="E55" s="474"/>
-      <c r="F55" s="475"/>
-      <c r="G55" s="473" t="s">
+      <c r="C55" s="461"/>
+      <c r="D55" s="461"/>
+      <c r="E55" s="461"/>
+      <c r="F55" s="462"/>
+      <c r="G55" s="460" t="s">
         <v>2</v>
       </c>
-      <c r="H55" s="474"/>
-      <c r="I55" s="474"/>
-      <c r="J55" s="474"/>
-      <c r="K55" s="475"/>
-      <c r="L55" s="473" t="s">
+      <c r="H55" s="461"/>
+      <c r="I55" s="461"/>
+      <c r="J55" s="461"/>
+      <c r="K55" s="462"/>
+      <c r="L55" s="460" t="s">
         <v>3</v>
       </c>
-      <c r="M55" s="474"/>
-      <c r="N55" s="474"/>
-      <c r="O55" s="474"/>
-      <c r="P55" s="475"/>
-      <c r="Q55" s="473" t="s">
+      <c r="M55" s="461"/>
+      <c r="N55" s="461"/>
+      <c r="O55" s="461"/>
+      <c r="P55" s="462"/>
+      <c r="Q55" s="460" t="s">
         <v>4</v>
       </c>
-      <c r="R55" s="474"/>
-      <c r="S55" s="474"/>
-      <c r="T55" s="474"/>
-      <c r="U55" s="475"/>
+      <c r="R55" s="461"/>
+      <c r="S55" s="461"/>
+      <c r="T55" s="461"/>
+      <c r="U55" s="462"/>
       <c r="AA55" s="218" t="s">
         <v>80</v>
       </c>
@@ -16202,7 +16320,7 @@
         <v>0.22851828638601948</v>
       </c>
     </row>
-    <row r="56" spans="2:40" ht="15.75" thickBot="1">
+    <row r="56" spans="2:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B56" s="92" t="s">
         <v>65</v>
       </c>
@@ -16306,7 +16424,7 @@
         <v>-0.3027637470411495</v>
       </c>
     </row>
-    <row r="57" spans="2:40" ht="15">
+    <row r="57" spans="2:40" x14ac:dyDescent="0.25">
       <c r="B57" s="165">
         <v>5</v>
       </c>
@@ -16410,7 +16528,7 @@
         <v>-9.3318329100743891E-2</v>
       </c>
     </row>
-    <row r="58" spans="2:40" ht="15">
+    <row r="58" spans="2:40" x14ac:dyDescent="0.25">
       <c r="B58" s="168">
         <v>1</v>
       </c>
@@ -16514,7 +16632,7 @@
         <v>5.0766638815107075E-2</v>
       </c>
     </row>
-    <row r="59" spans="2:40" ht="15.75" thickBot="1">
+    <row r="59" spans="2:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B59" s="170">
         <v>0.85</v>
       </c>
@@ -16618,7 +16736,7 @@
         <v>5.0766638815107075E-2</v>
       </c>
     </row>
-    <row r="60" spans="2:40" ht="15">
+    <row r="60" spans="2:40" x14ac:dyDescent="0.25">
       <c r="B60" s="165">
         <v>0.3</v>
       </c>
@@ -16722,7 +16840,7 @@
         <v>-3.8520880931257544E-2</v>
       </c>
     </row>
-    <row r="61" spans="2:40" ht="15">
+    <row r="61" spans="2:40" x14ac:dyDescent="0.25">
       <c r="B61" s="168">
         <v>0.25</v>
       </c>
@@ -16826,7 +16944,7 @@
         <v>-3.8520880931257544E-2</v>
       </c>
     </row>
-    <row r="62" spans="2:40" ht="15">
+    <row r="62" spans="2:40" x14ac:dyDescent="0.25">
       <c r="B62" s="168">
         <v>0.125</v>
       </c>
@@ -16930,7 +17048,7 @@
         <v>-6.340384840026668E-2</v>
       </c>
     </row>
-    <row r="63" spans="2:40" ht="15.75" thickBot="1">
+    <row r="63" spans="2:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B63" s="170">
         <v>6.3E-2</v>
       </c>
@@ -17034,7 +17152,7 @@
         <v>-6.340384840026668E-2</v>
       </c>
     </row>
-    <row r="64" spans="2:40" ht="15">
+    <row r="64" spans="2:40" x14ac:dyDescent="0.25">
       <c r="B64" s="165">
         <v>5.2999999999999999E-2</v>
       </c>
@@ -17138,7 +17256,7 @@
         <v>-3.2730377491297959E-2</v>
       </c>
     </row>
-    <row r="65" spans="2:21">
+    <row r="65" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B65" s="168">
         <v>3.7999999999999999E-2</v>
       </c>
@@ -17200,7 +17318,7 @@
         <v>0.76774197914340903</v>
       </c>
     </row>
-    <row r="66" spans="2:21" ht="15" thickBot="1">
+    <row r="66" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B66" s="170">
         <v>2.5000000000000001E-2</v>
       </c>
@@ -17262,7 +17380,7 @@
         <v>0.25681629007044648</v>
       </c>
     </row>
-    <row r="67" spans="2:21">
+    <row r="67" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B67" s="148" t="s">
         <v>70</v>
       </c>
@@ -17324,7 +17442,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="2:21" ht="15.75" thickBot="1">
+    <row r="68" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B68" s="143" t="s">
         <v>24</v>
       </c>
@@ -17367,24 +17485,24 @@
       <c r="T68" s="146"/>
       <c r="U68" s="147"/>
     </row>
-    <row r="69" spans="2:21" ht="15" thickBot="1"/>
-    <row r="70" spans="2:21">
-      <c r="B70" s="445" t="s">
+    <row r="69" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="70" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B70" s="454" t="s">
         <v>5</v>
       </c>
-      <c r="C70" s="446"/>
-      <c r="D70" s="446"/>
-      <c r="E70" s="446"/>
-      <c r="F70" s="447"/>
-      <c r="G70" s="445" t="s">
+      <c r="C70" s="455"/>
+      <c r="D70" s="455"/>
+      <c r="E70" s="455"/>
+      <c r="F70" s="456"/>
+      <c r="G70" s="454" t="s">
         <v>6</v>
       </c>
-      <c r="H70" s="446"/>
-      <c r="I70" s="446"/>
-      <c r="J70" s="446"/>
-      <c r="K70" s="447"/>
-    </row>
-    <row r="71" spans="2:21" ht="15" thickBot="1">
+      <c r="H70" s="455"/>
+      <c r="I70" s="455"/>
+      <c r="J70" s="455"/>
+      <c r="K70" s="456"/>
+    </row>
+    <row r="71" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B71" s="150" t="s">
         <v>65</v>
       </c>
@@ -17416,7 +17534,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="72" spans="2:21">
+    <row r="72" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B72" s="156">
         <v>5</v>
       </c>
@@ -17448,7 +17566,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="73" spans="2:21">
+    <row r="73" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B73" s="98">
         <v>1</v>
       </c>
@@ -17480,7 +17598,7 @@
         <v>43.638118564681662</v>
       </c>
     </row>
-    <row r="74" spans="2:21" ht="15" thickBot="1">
+    <row r="74" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B74" s="159">
         <v>0.85</v>
       </c>
@@ -17512,7 +17630,7 @@
         <v>34.792354193226231</v>
       </c>
     </row>
-    <row r="75" spans="2:21">
+    <row r="75" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B75" s="156">
         <v>0.3</v>
       </c>
@@ -17544,7 +17662,7 @@
         <v>6.7326227226191264</v>
       </c>
     </row>
-    <row r="76" spans="2:21">
+    <row r="76" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B76" s="98">
         <v>0.25</v>
       </c>
@@ -17576,7 +17694,7 @@
         <v>5.0779560968669699</v>
       </c>
     </row>
-    <row r="77" spans="2:21">
+    <row r="77" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B77" s="98">
         <v>0.125</v>
       </c>
@@ -17608,7 +17726,7 @@
         <v>2.0427035938751033</v>
       </c>
     </row>
-    <row r="78" spans="2:21" ht="15" thickBot="1">
+    <row r="78" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B78" s="159">
         <v>6.3E-2</v>
       </c>
@@ -17640,7 +17758,7 @@
         <v>0.97190567716775433</v>
       </c>
     </row>
-    <row r="79" spans="2:21">
+    <row r="79" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B79" s="156">
         <v>5.2999999999999999E-2</v>
       </c>
@@ -17672,7 +17790,7 @@
         <v>0.8055044899029582</v>
       </c>
     </row>
-    <row r="80" spans="2:21">
+    <row r="80" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B80" s="98">
         <v>3.7999999999999999E-2</v>
       </c>
@@ -17704,7 +17822,7 @@
         <v>0.4286260255362464</v>
       </c>
     </row>
-    <row r="81" spans="2:11">
+    <row r="81" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B81" s="98">
         <v>2.5000000000000001E-2</v>
       </c>
@@ -17736,7 +17854,7 @@
         <v>0.10502941660553233</v>
       </c>
     </row>
-    <row r="82" spans="2:11" ht="15" thickBot="1">
+    <row r="82" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B82" s="159" t="s">
         <v>70</v>
       </c>
@@ -17768,7 +17886,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="2:11" ht="15.75" thickBot="1">
+    <row r="83" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B83" s="160" t="s">
         <v>24</v>
       </c>
@@ -17788,24 +17906,24 @@
       <c r="J83" s="163"/>
       <c r="K83" s="164"/>
     </row>
-    <row r="84" spans="2:11" ht="15" thickBot="1"/>
-    <row r="85" spans="2:11">
-      <c r="B85" s="470" t="s">
+    <row r="84" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="85" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B85" s="457" t="s">
         <v>7</v>
       </c>
-      <c r="C85" s="471"/>
-      <c r="D85" s="471"/>
-      <c r="E85" s="471"/>
-      <c r="F85" s="472"/>
-      <c r="G85" s="470" t="s">
+      <c r="C85" s="458"/>
+      <c r="D85" s="458"/>
+      <c r="E85" s="458"/>
+      <c r="F85" s="459"/>
+      <c r="G85" s="457" t="s">
         <v>8</v>
       </c>
-      <c r="H85" s="471"/>
-      <c r="I85" s="471"/>
-      <c r="J85" s="471"/>
-      <c r="K85" s="472"/>
-    </row>
-    <row r="86" spans="2:11" ht="15" thickBot="1">
+      <c r="H85" s="458"/>
+      <c r="I85" s="458"/>
+      <c r="J85" s="458"/>
+      <c r="K85" s="459"/>
+    </row>
+    <row r="86" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B86" s="173" t="s">
         <v>65</v>
       </c>
@@ -17837,7 +17955,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="87" spans="2:11">
+    <row r="87" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B87" s="179">
         <v>5</v>
       </c>
@@ -17869,7 +17987,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="88" spans="2:11">
+    <row r="88" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B88" s="107">
         <v>1</v>
       </c>
@@ -17901,7 +18019,7 @@
         <v>38.13410958444954</v>
       </c>
     </row>
-    <row r="89" spans="2:11" ht="15" thickBot="1">
+    <row r="89" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B89" s="182">
         <v>0.85</v>
       </c>
@@ -17933,7 +18051,7 @@
         <v>30.354753291890873</v>
       </c>
     </row>
-    <row r="90" spans="2:11">
+    <row r="90" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B90" s="179">
         <v>0.3</v>
       </c>
@@ -17965,7 +18083,7 @@
         <v>6.5023063218227861</v>
       </c>
     </row>
-    <row r="91" spans="2:11">
+    <row r="91" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B91" s="107">
         <v>0.25</v>
       </c>
@@ -17997,7 +18115,7 @@
         <v>5.288683424133751</v>
       </c>
     </row>
-    <row r="92" spans="2:11">
+    <row r="92" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B92" s="107">
         <v>0.125</v>
       </c>
@@ -18029,7 +18147,7 @@
         <v>2.7820248706319859</v>
       </c>
     </row>
-    <row r="93" spans="2:11" ht="15" thickBot="1">
+    <row r="93" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B93" s="182">
         <v>6.3E-2</v>
       </c>
@@ -18061,7 +18179,7 @@
         <v>1.7243913192573501</v>
       </c>
     </row>
-    <row r="94" spans="2:11">
+    <row r="94" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B94" s="176">
         <v>5.2999999999999999E-2</v>
       </c>
@@ -18093,7 +18211,7 @@
         <v>1.5124520751739823</v>
       </c>
     </row>
-    <row r="95" spans="2:11">
+    <row r="95" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B95" s="107">
         <v>3.7999999999999999E-2</v>
       </c>
@@ -18125,7 +18243,7 @@
         <v>1.0370068609529142</v>
       </c>
     </row>
-    <row r="96" spans="2:11">
+    <row r="96" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B96" s="107">
         <v>2.5000000000000001E-2</v>
       </c>
@@ -18157,7 +18275,7 @@
         <v>0.62627788793004413</v>
       </c>
     </row>
-    <row r="97" spans="2:21" ht="15" thickBot="1">
+    <row r="97" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B97" s="109" t="s">
         <v>70</v>
       </c>
@@ -18189,7 +18307,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="2:21" ht="15.75" thickBot="1">
+    <row r="98" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B98" s="111" t="s">
         <v>24</v>
       </c>
@@ -18211,38 +18329,38 @@
       <c r="J98" s="114"/>
       <c r="K98" s="115"/>
     </row>
-    <row r="99" spans="2:21" ht="15" thickBot="1"/>
-    <row r="100" spans="2:21">
-      <c r="B100" s="457" t="s">
+    <row r="99" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="100" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B100" s="464" t="s">
         <v>9</v>
       </c>
-      <c r="C100" s="458"/>
-      <c r="D100" s="458"/>
-      <c r="E100" s="458"/>
-      <c r="F100" s="459"/>
-      <c r="G100" s="457" t="s">
+      <c r="C100" s="465"/>
+      <c r="D100" s="465"/>
+      <c r="E100" s="465"/>
+      <c r="F100" s="466"/>
+      <c r="G100" s="464" t="s">
         <v>10</v>
       </c>
-      <c r="H100" s="458"/>
-      <c r="I100" s="458"/>
-      <c r="J100" s="458"/>
-      <c r="K100" s="459"/>
-      <c r="L100" s="460" t="s">
+      <c r="H100" s="465"/>
+      <c r="I100" s="465"/>
+      <c r="J100" s="465"/>
+      <c r="K100" s="466"/>
+      <c r="L100" s="467" t="s">
         <v>11</v>
       </c>
-      <c r="M100" s="461"/>
-      <c r="N100" s="461"/>
-      <c r="O100" s="461"/>
-      <c r="P100" s="462"/>
-      <c r="Q100" s="457" t="s">
+      <c r="M100" s="468"/>
+      <c r="N100" s="468"/>
+      <c r="O100" s="468"/>
+      <c r="P100" s="469"/>
+      <c r="Q100" s="464" t="s">
         <v>12</v>
       </c>
-      <c r="R100" s="458"/>
-      <c r="S100" s="458"/>
-      <c r="T100" s="458"/>
-      <c r="U100" s="459"/>
-    </row>
-    <row r="101" spans="2:21" ht="15" thickBot="1">
+      <c r="R100" s="465"/>
+      <c r="S100" s="465"/>
+      <c r="T100" s="465"/>
+      <c r="U100" s="466"/>
+    </row>
+    <row r="101" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B101" s="183" t="s">
         <v>65</v>
       </c>
@@ -18304,7 +18422,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="102" spans="2:21">
+    <row r="102" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B102" s="189">
         <v>5</v>
       </c>
@@ -18366,7 +18484,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="103" spans="2:21">
+    <row r="103" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B103" s="116">
         <v>1</v>
       </c>
@@ -18428,7 +18546,7 @@
         <v>57.614897190092236</v>
       </c>
     </row>
-    <row r="104" spans="2:21" ht="15" thickBot="1">
+    <row r="104" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B104" s="192">
         <v>0.85</v>
       </c>
@@ -18490,7 +18608,7 @@
         <v>49.683536269101168</v>
       </c>
     </row>
-    <row r="105" spans="2:21">
+    <row r="105" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B105" s="189">
         <v>0.3</v>
       </c>
@@ -18552,7 +18670,7 @@
         <v>14.041921923228983</v>
       </c>
     </row>
-    <row r="106" spans="2:21">
+    <row r="106" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B106" s="116">
         <v>0.25</v>
       </c>
@@ -18614,7 +18732,7 @@
         <v>11.205899101569443</v>
       </c>
     </row>
-    <row r="107" spans="2:21">
+    <row r="107" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B107" s="116">
         <v>0.125</v>
       </c>
@@ -18676,7 +18794,7 @@
         <v>5.4972198343870105</v>
       </c>
     </row>
-    <row r="108" spans="2:21" ht="15" thickBot="1">
+    <row r="108" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B108" s="192">
         <v>6.3E-2</v>
       </c>
@@ -18738,7 +18856,7 @@
         <v>3.0282586696554006</v>
       </c>
     </row>
-    <row r="109" spans="2:21">
+    <row r="109" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B109" s="186">
         <v>5.2999999999999999E-2</v>
       </c>
@@ -18800,7 +18918,7 @@
         <v>2.4950762233272883</v>
       </c>
     </row>
-    <row r="110" spans="2:21">
+    <row r="110" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B110" s="116">
         <v>3.7999999999999999E-2</v>
       </c>
@@ -18862,7 +18980,7 @@
         <v>1.3938912525435114</v>
       </c>
     </row>
-    <row r="111" spans="2:21">
+    <row r="111" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B111" s="116">
         <v>2.5000000000000001E-2</v>
       </c>
@@ -18924,7 +19042,7 @@
         <v>0.73049622238424661</v>
       </c>
     </row>
-    <row r="112" spans="2:21" ht="15" thickBot="1">
+    <row r="112" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B112" s="118" t="s">
         <v>70</v>
       </c>
@@ -18986,7 +19104,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="2:21" ht="15.75" thickBot="1">
+    <row r="113" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B113" s="120" t="s">
         <v>24</v>
       </c>
@@ -19026,38 +19144,38 @@
       <c r="T113" s="123"/>
       <c r="U113" s="124"/>
     </row>
-    <row r="114" spans="2:21" ht="15" thickBot="1"/>
-    <row r="115" spans="2:21">
-      <c r="B115" s="463" t="s">
+    <row r="114" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="115" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B115" s="470" t="s">
         <v>13</v>
       </c>
-      <c r="C115" s="464"/>
-      <c r="D115" s="464"/>
-      <c r="E115" s="464"/>
-      <c r="F115" s="465"/>
-      <c r="G115" s="463" t="s">
+      <c r="C115" s="471"/>
+      <c r="D115" s="471"/>
+      <c r="E115" s="471"/>
+      <c r="F115" s="472"/>
+      <c r="G115" s="470" t="s">
         <v>14</v>
       </c>
-      <c r="H115" s="464"/>
-      <c r="I115" s="464"/>
-      <c r="J115" s="464"/>
-      <c r="K115" s="465"/>
-      <c r="L115" s="466" t="s">
+      <c r="H115" s="471"/>
+      <c r="I115" s="471"/>
+      <c r="J115" s="471"/>
+      <c r="K115" s="472"/>
+      <c r="L115" s="473" t="s">
         <v>15</v>
       </c>
-      <c r="M115" s="467"/>
-      <c r="N115" s="467"/>
-      <c r="O115" s="467"/>
-      <c r="P115" s="468"/>
-      <c r="Q115" s="463" t="s">
+      <c r="M115" s="474"/>
+      <c r="N115" s="474"/>
+      <c r="O115" s="474"/>
+      <c r="P115" s="475"/>
+      <c r="Q115" s="470" t="s">
         <v>16</v>
       </c>
-      <c r="R115" s="464"/>
-      <c r="S115" s="464"/>
-      <c r="T115" s="464"/>
-      <c r="U115" s="465"/>
-    </row>
-    <row r="116" spans="2:21" ht="15" thickBot="1">
+      <c r="R115" s="471"/>
+      <c r="S115" s="471"/>
+      <c r="T115" s="471"/>
+      <c r="U115" s="472"/>
+    </row>
+    <row r="116" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B116" s="193" t="s">
         <v>65</v>
       </c>
@@ -19119,7 +19237,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="117" spans="2:21">
+    <row r="117" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B117" s="199">
         <v>5</v>
       </c>
@@ -19181,7 +19299,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="118" spans="2:21">
+    <row r="118" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B118" s="125">
         <v>1</v>
       </c>
@@ -19243,7 +19361,7 @@
         <v>39.693418059151178</v>
       </c>
     </row>
-    <row r="119" spans="2:21" ht="15" thickBot="1">
+    <row r="119" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B119" s="202">
         <v>0.85</v>
       </c>
@@ -19305,7 +19423,7 @@
         <v>32.956146544284934</v>
       </c>
     </row>
-    <row r="120" spans="2:21">
+    <row r="120" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B120" s="199">
         <v>0.3</v>
       </c>
@@ -19367,7 +19485,7 @@
         <v>7.1524280222797501</v>
       </c>
     </row>
-    <row r="121" spans="2:21">
+    <row r="121" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B121" s="125">
         <v>0.25</v>
       </c>
@@ -19429,7 +19547,7 @@
         <v>5.7412724562642126</v>
       </c>
     </row>
-    <row r="122" spans="2:21">
+    <row r="122" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B122" s="125">
         <v>0.125</v>
       </c>
@@ -19491,7 +19609,7 @@
         <v>2.6459559111947897</v>
       </c>
     </row>
-    <row r="123" spans="2:21" ht="15" thickBot="1">
+    <row r="123" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B123" s="202">
         <v>6.3E-2</v>
       </c>
@@ -19553,7 +19671,7 @@
         <v>1.5172197379775554</v>
       </c>
     </row>
-    <row r="124" spans="2:21">
+    <row r="124" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B124" s="196">
         <v>5.2999999999999999E-2</v>
       </c>
@@ -19615,7 +19733,7 @@
         <v>1.3223503569467283</v>
       </c>
     </row>
-    <row r="125" spans="2:21">
+    <row r="125" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B125" s="125">
         <v>3.7999999999999999E-2</v>
       </c>
@@ -19677,7 +19795,7 @@
         <v>0.92413901310111157</v>
       </c>
     </row>
-    <row r="126" spans="2:21">
+    <row r="126" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B126" s="125">
         <v>2.5000000000000001E-2</v>
       </c>
@@ -19739,7 +19857,7 @@
         <v>0.5136894955675757</v>
       </c>
     </row>
-    <row r="127" spans="2:21" ht="15" thickBot="1">
+    <row r="127" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B127" s="127" t="s">
         <v>70</v>
       </c>
@@ -19801,7 +19919,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="128" spans="2:21" ht="15.75" thickBot="1">
+    <row r="128" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B128" s="129" t="s">
         <v>24</v>
       </c>
@@ -19841,38 +19959,38 @@
       <c r="T128" s="132"/>
       <c r="U128" s="133"/>
     </row>
-    <row r="129" spans="2:21" ht="15" thickBot="1"/>
-    <row r="130" spans="2:21">
-      <c r="B130" s="445" t="s">
+    <row r="129" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="130" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B130" s="454" t="s">
         <v>17</v>
       </c>
-      <c r="C130" s="446"/>
-      <c r="D130" s="446"/>
-      <c r="E130" s="446"/>
-      <c r="F130" s="447"/>
-      <c r="G130" s="445" t="s">
+      <c r="C130" s="455"/>
+      <c r="D130" s="455"/>
+      <c r="E130" s="455"/>
+      <c r="F130" s="456"/>
+      <c r="G130" s="454" t="s">
         <v>18</v>
       </c>
-      <c r="H130" s="446"/>
-      <c r="I130" s="446"/>
-      <c r="J130" s="446"/>
-      <c r="K130" s="447"/>
-      <c r="L130" s="448" t="s">
+      <c r="H130" s="455"/>
+      <c r="I130" s="455"/>
+      <c r="J130" s="455"/>
+      <c r="K130" s="456"/>
+      <c r="L130" s="476" t="s">
         <v>19</v>
       </c>
-      <c r="M130" s="449"/>
-      <c r="N130" s="449"/>
-      <c r="O130" s="449"/>
-      <c r="P130" s="450"/>
-      <c r="Q130" s="445" t="s">
+      <c r="M130" s="477"/>
+      <c r="N130" s="477"/>
+      <c r="O130" s="477"/>
+      <c r="P130" s="478"/>
+      <c r="Q130" s="454" t="s">
         <v>20</v>
       </c>
-      <c r="R130" s="446"/>
-      <c r="S130" s="446"/>
-      <c r="T130" s="446"/>
-      <c r="U130" s="447"/>
-    </row>
-    <row r="131" spans="2:21" ht="15" thickBot="1">
+      <c r="R130" s="455"/>
+      <c r="S130" s="455"/>
+      <c r="T130" s="455"/>
+      <c r="U130" s="456"/>
+    </row>
+    <row r="131" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B131" s="150" t="s">
         <v>65</v>
       </c>
@@ -19934,7 +20052,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="132" spans="2:21">
+    <row r="132" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B132" s="156">
         <v>5</v>
       </c>
@@ -19996,7 +20114,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="133" spans="2:21">
+    <row r="133" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B133" s="98">
         <v>1</v>
       </c>
@@ -20058,7 +20176,7 @@
         <v>48.409962359728418</v>
       </c>
     </row>
-    <row r="134" spans="2:21" ht="15" thickBot="1">
+    <row r="134" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B134" s="159">
         <v>0.85</v>
       </c>
@@ -20120,7 +20238,7 @@
         <v>39.877581172828641</v>
       </c>
     </row>
-    <row r="135" spans="2:21">
+    <row r="135" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B135" s="156">
         <v>0.3</v>
       </c>
@@ -20182,7 +20300,7 @@
         <v>9.2318335854410662</v>
       </c>
     </row>
-    <row r="136" spans="2:21">
+    <row r="136" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B136" s="98">
         <v>0.25</v>
       </c>
@@ -20244,7 +20362,7 @@
         <v>7.8557943738933602</v>
       </c>
     </row>
-    <row r="137" spans="2:21">
+    <row r="137" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B137" s="98">
         <v>0.125</v>
       </c>
@@ -20306,7 +20424,7 @@
         <v>4.9946646967085258</v>
       </c>
     </row>
-    <row r="138" spans="2:21" ht="15" thickBot="1">
+    <row r="138" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B138" s="159">
         <v>6.3E-2</v>
       </c>
@@ -20368,7 +20486,7 @@
         <v>2.9936328138741288</v>
       </c>
     </row>
-    <row r="139" spans="2:21">
+    <row r="139" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B139" s="153">
         <v>5.2999999999999999E-2</v>
       </c>
@@ -20430,7 +20548,7 @@
         <v>2.3639497660674635</v>
       </c>
     </row>
-    <row r="140" spans="2:21">
+    <row r="140" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B140" s="98">
         <v>3.7999999999999999E-2</v>
       </c>
@@ -20492,7 +20610,7 @@
         <v>1.244122371923396</v>
       </c>
     </row>
-    <row r="141" spans="2:21">
+    <row r="141" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B141" s="98">
         <v>2.5000000000000001E-2</v>
       </c>
@@ -20554,7 +20672,7 @@
         <v>0.28669926478346497</v>
       </c>
     </row>
-    <row r="142" spans="2:21" ht="15" thickBot="1">
+    <row r="142" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B142" s="100" t="s">
         <v>70</v>
       </c>
@@ -20616,7 +20734,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="143" spans="2:21" ht="15.75" thickBot="1">
+    <row r="143" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B143" s="102" t="s">
         <v>24</v>
       </c>
@@ -20656,31 +20774,31 @@
       <c r="T143" s="105"/>
       <c r="U143" s="106"/>
     </row>
-    <row r="144" spans="2:21" ht="15" thickBot="1"/>
-    <row r="145" spans="2:16">
-      <c r="B145" s="451" t="s">
+    <row r="144" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="145" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B145" s="479" t="s">
         <v>21</v>
       </c>
-      <c r="C145" s="452"/>
-      <c r="D145" s="452"/>
-      <c r="E145" s="452"/>
-      <c r="F145" s="453"/>
-      <c r="G145" s="451" t="s">
+      <c r="C145" s="480"/>
+      <c r="D145" s="480"/>
+      <c r="E145" s="480"/>
+      <c r="F145" s="481"/>
+      <c r="G145" s="479" t="s">
         <v>22</v>
       </c>
-      <c r="H145" s="452"/>
-      <c r="I145" s="452"/>
-      <c r="J145" s="452"/>
-      <c r="K145" s="453"/>
-      <c r="L145" s="454" t="s">
+      <c r="H145" s="480"/>
+      <c r="I145" s="480"/>
+      <c r="J145" s="480"/>
+      <c r="K145" s="481"/>
+      <c r="L145" s="482" t="s">
         <v>23</v>
       </c>
-      <c r="M145" s="455"/>
-      <c r="N145" s="455"/>
-      <c r="O145" s="455"/>
-      <c r="P145" s="456"/>
-    </row>
-    <row r="146" spans="2:16" ht="15" thickBot="1">
+      <c r="M145" s="483"/>
+      <c r="N145" s="483"/>
+      <c r="O145" s="483"/>
+      <c r="P145" s="484"/>
+    </row>
+    <row r="146" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B146" s="203" t="s">
         <v>65</v>
       </c>
@@ -20727,7 +20845,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="147" spans="2:16">
+    <row r="147" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B147" s="209">
         <v>5</v>
       </c>
@@ -20774,7 +20892,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="148" spans="2:16">
+    <row r="148" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B148" s="134">
         <v>1</v>
       </c>
@@ -20821,7 +20939,7 @@
         <v>49.636163364076339</v>
       </c>
     </row>
-    <row r="149" spans="2:16" ht="15" thickBot="1">
+    <row r="149" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B149" s="212">
         <v>0.85</v>
       </c>
@@ -20868,7 +20986,7 @@
         <v>39.957252762304812</v>
       </c>
     </row>
-    <row r="150" spans="2:16">
+    <row r="150" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B150" s="209">
         <v>0.3</v>
       </c>
@@ -20915,7 +21033,7 @@
         <v>7.0761231850972592</v>
       </c>
     </row>
-    <row r="151" spans="2:16">
+    <row r="151" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B151" s="134">
         <v>0.25</v>
       </c>
@@ -20962,7 +21080,7 @@
         <v>5.7083827960916835</v>
       </c>
     </row>
-    <row r="152" spans="2:16">
+    <row r="152" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B152" s="134">
         <v>0.125</v>
       </c>
@@ -21009,7 +21127,7 @@
         <v>2.9988699662131353</v>
       </c>
     </row>
-    <row r="153" spans="2:16" ht="15" thickBot="1">
+    <row r="153" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B153" s="212">
         <v>6.3E-2</v>
       </c>
@@ -21056,7 +21174,7 @@
         <v>1.7244429732444502</v>
       </c>
     </row>
-    <row r="154" spans="2:16">
+    <row r="154" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B154" s="206">
         <v>5.2999999999999999E-2</v>
       </c>
@@ -21103,7 +21221,7 @@
         <v>1.4798876814902684</v>
       </c>
     </row>
-    <row r="155" spans="2:16">
+    <row r="155" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B155" s="134">
         <v>3.7999999999999999E-2</v>
       </c>
@@ -21150,7 +21268,7 @@
         <v>0.9605287188384608</v>
       </c>
     </row>
-    <row r="156" spans="2:16">
+    <row r="156" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B156" s="134">
         <v>2.5000000000000001E-2</v>
       </c>
@@ -21197,7 +21315,7 @@
         <v>0.295635101817183</v>
       </c>
     </row>
-    <row r="157" spans="2:16" ht="15" thickBot="1">
+    <row r="157" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B157" s="136" t="s">
         <v>70</v>
       </c>
@@ -21244,7 +21362,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="158" spans="2:16" ht="15.75" thickBot="1">
+    <row r="158" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B158" s="138" t="s">
         <v>24</v>
       </c>
@@ -21277,6 +21395,36 @@
     </row>
   </sheetData>
   <mergeCells count="46">
+    <mergeCell ref="B130:F130"/>
+    <mergeCell ref="G130:K130"/>
+    <mergeCell ref="L130:P130"/>
+    <mergeCell ref="Q130:U130"/>
+    <mergeCell ref="B145:F145"/>
+    <mergeCell ref="G145:K145"/>
+    <mergeCell ref="L145:P145"/>
+    <mergeCell ref="B100:F100"/>
+    <mergeCell ref="G100:K100"/>
+    <mergeCell ref="L100:P100"/>
+    <mergeCell ref="Q100:U100"/>
+    <mergeCell ref="B115:F115"/>
+    <mergeCell ref="G115:K115"/>
+    <mergeCell ref="L115:P115"/>
+    <mergeCell ref="Q115:U115"/>
+    <mergeCell ref="AH16:AH17"/>
+    <mergeCell ref="AI16:AI17"/>
+    <mergeCell ref="B70:F70"/>
+    <mergeCell ref="G70:K70"/>
+    <mergeCell ref="B85:F85"/>
+    <mergeCell ref="G85:K85"/>
+    <mergeCell ref="B55:F55"/>
+    <mergeCell ref="G55:K55"/>
+    <mergeCell ref="L55:P55"/>
+    <mergeCell ref="Q55:U55"/>
+    <mergeCell ref="AA51:AN51"/>
+    <mergeCell ref="AB52:AD52"/>
+    <mergeCell ref="AE52:AG52"/>
+    <mergeCell ref="AH52:AJ52"/>
+    <mergeCell ref="AK52:AM52"/>
     <mergeCell ref="AL1:AL2"/>
     <mergeCell ref="AL16:AL17"/>
     <mergeCell ref="AK16:AK17"/>
@@ -21293,36 +21441,6 @@
     <mergeCell ref="AH1:AH2"/>
     <mergeCell ref="AI1:AI2"/>
     <mergeCell ref="AG16:AG17"/>
-    <mergeCell ref="AH16:AH17"/>
-    <mergeCell ref="AI16:AI17"/>
-    <mergeCell ref="B70:F70"/>
-    <mergeCell ref="G70:K70"/>
-    <mergeCell ref="B85:F85"/>
-    <mergeCell ref="G85:K85"/>
-    <mergeCell ref="B55:F55"/>
-    <mergeCell ref="G55:K55"/>
-    <mergeCell ref="L55:P55"/>
-    <mergeCell ref="Q55:U55"/>
-    <mergeCell ref="AA51:AN51"/>
-    <mergeCell ref="AB52:AD52"/>
-    <mergeCell ref="AE52:AG52"/>
-    <mergeCell ref="AH52:AJ52"/>
-    <mergeCell ref="AK52:AM52"/>
-    <mergeCell ref="B100:F100"/>
-    <mergeCell ref="G100:K100"/>
-    <mergeCell ref="L100:P100"/>
-    <mergeCell ref="Q100:U100"/>
-    <mergeCell ref="B115:F115"/>
-    <mergeCell ref="G115:K115"/>
-    <mergeCell ref="L115:P115"/>
-    <mergeCell ref="Q115:U115"/>
-    <mergeCell ref="B130:F130"/>
-    <mergeCell ref="G130:K130"/>
-    <mergeCell ref="L130:P130"/>
-    <mergeCell ref="Q130:U130"/>
-    <mergeCell ref="B145:F145"/>
-    <mergeCell ref="G145:K145"/>
-    <mergeCell ref="L145:P145"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -21334,49 +21452,49 @@
   <dimension ref="B1:BA158"/>
   <sheetViews>
     <sheetView topLeftCell="W1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AK48" sqref="AK48"/>
+      <selection activeCell="AM17" sqref="AM17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="15.75" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" customWidth="1"/>
     <col min="27" max="27" width="18" customWidth="1"/>
-    <col min="28" max="28" width="22.5" customWidth="1"/>
+    <col min="28" max="28" width="22.42578125" customWidth="1"/>
     <col min="29" max="29" width="19" customWidth="1"/>
-    <col min="30" max="30" width="18.625" customWidth="1"/>
-    <col min="31" max="31" width="16.75" customWidth="1"/>
-    <col min="32" max="32" width="20.5" customWidth="1"/>
-    <col min="33" max="33" width="19.125" customWidth="1"/>
-    <col min="34" max="34" width="20.875" customWidth="1"/>
-    <col min="35" max="35" width="17.375" customWidth="1"/>
-    <col min="36" max="36" width="20.25" customWidth="1"/>
-    <col min="37" max="37" width="18.25" customWidth="1"/>
+    <col min="30" max="30" width="18.5703125" customWidth="1"/>
+    <col min="31" max="31" width="16.7109375" customWidth="1"/>
+    <col min="32" max="32" width="20.42578125" customWidth="1"/>
+    <col min="33" max="33" width="19.140625" customWidth="1"/>
+    <col min="34" max="34" width="20.85546875" customWidth="1"/>
+    <col min="35" max="35" width="17.42578125" customWidth="1"/>
+    <col min="36" max="36" width="20.28515625" customWidth="1"/>
+    <col min="37" max="37" width="18.28515625" customWidth="1"/>
     <col min="38" max="38" width="17" customWidth="1"/>
-    <col min="39" max="39" width="14.5" customWidth="1"/>
-    <col min="40" max="40" width="14.625" customWidth="1"/>
+    <col min="39" max="39" width="14.42578125" customWidth="1"/>
+    <col min="40" max="40" width="14.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:53">
-      <c r="AG1" s="469" t="s">
+    <row r="1" spans="2:53" x14ac:dyDescent="0.25">
+      <c r="AG1" s="451" t="s">
         <v>56</v>
       </c>
-      <c r="AH1" s="469" t="s">
+      <c r="AH1" s="451" t="s">
         <v>57</v>
       </c>
-      <c r="AI1" s="469" t="s">
+      <c r="AI1" s="451" t="s">
         <v>52</v>
       </c>
-      <c r="AJ1" s="469" t="s">
+      <c r="AJ1" s="451" t="s">
         <v>56</v>
       </c>
-      <c r="AK1" s="469" t="s">
+      <c r="AK1" s="451" t="s">
         <v>57</v>
       </c>
-      <c r="AL1" s="469" t="s">
+      <c r="AL1" s="451" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="2:53" ht="15.75" thickBot="1">
+    <row r="2" spans="2:53" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -21449,25 +21567,25 @@
       <c r="Y2" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="AB2" s="481" t="s">
+      <c r="AB2" s="448" t="s">
         <v>25</v>
       </c>
-      <c r="AC2" s="482"/>
-      <c r="AD2" s="476" t="s">
+      <c r="AC2" s="449"/>
+      <c r="AD2" s="452" t="s">
         <v>58</v>
       </c>
-      <c r="AE2" s="476"/>
+      <c r="AE2" s="452"/>
       <c r="AF2" s="429" t="s">
         <v>104</v>
       </c>
-      <c r="AG2" s="469"/>
-      <c r="AH2" s="469"/>
-      <c r="AI2" s="469"/>
-      <c r="AJ2" s="469"/>
-      <c r="AK2" s="469"/>
-      <c r="AL2" s="469"/>
-    </row>
-    <row r="3" spans="2:53" ht="15">
+      <c r="AG2" s="451"/>
+      <c r="AH2" s="451"/>
+      <c r="AI2" s="451"/>
+      <c r="AJ2" s="451"/>
+      <c r="AK2" s="451"/>
+      <c r="AL2" s="451"/>
+    </row>
+    <row r="3" spans="2:53" x14ac:dyDescent="0.25">
       <c r="B3" s="14">
         <v>0.37</v>
       </c>
@@ -21573,7 +21691,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="4" spans="2:53" ht="15">
+    <row r="4" spans="2:53" x14ac:dyDescent="0.25">
       <c r="B4" s="28">
         <v>0.44</v>
       </c>
@@ -21693,7 +21811,7 @@
       <c r="AZ4" s="85"/>
       <c r="BA4" s="85"/>
     </row>
-    <row r="5" spans="2:53" ht="15">
+    <row r="5" spans="2:53" x14ac:dyDescent="0.25">
       <c r="B5" s="28">
         <v>0.52</v>
       </c>
@@ -21808,7 +21926,7 @@
         <v>4.1335352770415241</v>
       </c>
     </row>
-    <row r="6" spans="2:53" ht="15">
+    <row r="6" spans="2:53" x14ac:dyDescent="0.25">
       <c r="B6" s="28">
         <v>0.61</v>
       </c>
@@ -21923,7 +22041,7 @@
         <v>3.8846282094031355</v>
       </c>
     </row>
-    <row r="7" spans="2:53" ht="15">
+    <row r="7" spans="2:53" x14ac:dyDescent="0.25">
       <c r="B7" s="28">
         <v>0.72</v>
       </c>
@@ -22038,7 +22156,7 @@
         <v>4.3380109823062849</v>
       </c>
     </row>
-    <row r="8" spans="2:53" ht="15">
+    <row r="8" spans="2:53" x14ac:dyDescent="0.25">
       <c r="B8" s="28">
         <v>0.85</v>
       </c>
@@ -22153,7 +22271,7 @@
         <v>5.1220488195278104</v>
       </c>
     </row>
-    <row r="9" spans="2:53" ht="15">
+    <row r="9" spans="2:53" x14ac:dyDescent="0.25">
       <c r="B9" s="28">
         <v>1.01</v>
       </c>
@@ -22268,7 +22386,7 @@
         <v>9.2011761823082541</v>
       </c>
     </row>
-    <row r="10" spans="2:53" ht="15">
+    <row r="10" spans="2:53" x14ac:dyDescent="0.25">
       <c r="B10" s="28">
         <v>1.19</v>
       </c>
@@ -22383,7 +22501,7 @@
         <v>4.9071065566941607</v>
       </c>
     </row>
-    <row r="11" spans="2:53" ht="15">
+    <row r="11" spans="2:53" x14ac:dyDescent="0.25">
       <c r="B11" s="28">
         <v>1.4</v>
       </c>
@@ -22498,7 +22616,7 @@
         <v>4.8620551779288306</v>
       </c>
     </row>
-    <row r="12" spans="2:53" ht="15">
+    <row r="12" spans="2:53" x14ac:dyDescent="0.25">
       <c r="B12" s="28">
         <v>1.65</v>
       </c>
@@ -22613,7 +22731,7 @@
         <v>5.0080984774862323</v>
       </c>
     </row>
-    <row r="13" spans="2:53" ht="15.75" thickBot="1">
+    <row r="13" spans="2:53" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="42">
         <v>1.95</v>
       </c>
@@ -22728,7 +22846,7 @@
         <v>11.004862236628849</v>
       </c>
     </row>
-    <row r="14" spans="2:53" ht="15">
+    <row r="14" spans="2:53" x14ac:dyDescent="0.25">
       <c r="B14" s="28">
         <v>2.2999999999999998</v>
       </c>
@@ -22843,7 +22961,7 @@
         <v>4.2835481425322222</v>
       </c>
     </row>
-    <row r="15" spans="2:53" ht="15">
+    <row r="15" spans="2:53" x14ac:dyDescent="0.25">
       <c r="B15" s="28">
         <v>2.72</v>
       </c>
@@ -22914,26 +23032,26 @@
       <c r="Y15" s="380">
         <v>1.0235026535253984</v>
       </c>
-      <c r="AG15" s="469" t="s">
+      <c r="AG15" s="451" t="s">
         <v>56</v>
       </c>
-      <c r="AH15" s="469" t="s">
+      <c r="AH15" s="451" t="s">
         <v>57</v>
       </c>
-      <c r="AI15" s="469" t="s">
+      <c r="AI15" s="451" t="s">
         <v>52</v>
       </c>
-      <c r="AJ15" s="469" t="s">
+      <c r="AJ15" s="451" t="s">
         <v>56</v>
       </c>
-      <c r="AK15" s="469" t="s">
+      <c r="AK15" s="451" t="s">
         <v>57</v>
       </c>
-      <c r="AL15" s="469" t="s">
+      <c r="AL15" s="451" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="16" spans="2:53" ht="15">
+    <row r="16" spans="2:53" x14ac:dyDescent="0.25">
       <c r="B16" s="28">
         <v>3.2</v>
       </c>
@@ -23004,25 +23122,25 @@
       <c r="Y16" s="380">
         <v>1.0708870356330553</v>
       </c>
-      <c r="AB16" s="481" t="s">
+      <c r="AB16" s="448" t="s">
         <v>40</v>
       </c>
-      <c r="AC16" s="483"/>
-      <c r="AD16" s="476" t="s">
+      <c r="AC16" s="450"/>
+      <c r="AD16" s="452" t="s">
         <v>58</v>
       </c>
-      <c r="AE16" s="476"/>
+      <c r="AE16" s="452"/>
       <c r="AF16" s="429" t="s">
         <v>104</v>
       </c>
-      <c r="AG16" s="469"/>
-      <c r="AH16" s="469"/>
-      <c r="AI16" s="469"/>
-      <c r="AJ16" s="469"/>
-      <c r="AK16" s="469"/>
-      <c r="AL16" s="469"/>
-    </row>
-    <row r="17" spans="2:40" ht="14.45" customHeight="1">
+      <c r="AG16" s="451"/>
+      <c r="AH16" s="451"/>
+      <c r="AI16" s="451"/>
+      <c r="AJ16" s="451"/>
+      <c r="AK16" s="451"/>
+      <c r="AL16" s="451"/>
+    </row>
+    <row r="17" spans="2:40" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="28">
         <v>3.78</v>
       </c>
@@ -23128,7 +23246,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="18" spans="2:40" ht="15">
+    <row r="18" spans="2:40" x14ac:dyDescent="0.25">
       <c r="B18" s="28">
         <v>4.46</v>
       </c>
@@ -23243,7 +23361,7 @@
         <v>3.3052276559865081</v>
       </c>
     </row>
-    <row r="19" spans="2:40" ht="15">
+    <row r="19" spans="2:40" x14ac:dyDescent="0.25">
       <c r="B19" s="28">
         <v>5.27</v>
       </c>
@@ -23358,7 +23476,7 @@
         <v>4.0281908702961342</v>
       </c>
     </row>
-    <row r="20" spans="2:40" ht="15">
+    <row r="20" spans="2:40" x14ac:dyDescent="0.25">
       <c r="B20" s="28">
         <v>6.21</v>
       </c>
@@ -23473,7 +23591,7 @@
         <v>4.1997803191833034</v>
       </c>
     </row>
-    <row r="21" spans="2:40" ht="15">
+    <row r="21" spans="2:40" x14ac:dyDescent="0.25">
       <c r="B21" s="28">
         <v>7.33</v>
       </c>
@@ -23588,7 +23706,7 @@
         <v>6.6448579022694725</v>
       </c>
     </row>
-    <row r="22" spans="2:40" ht="15">
+    <row r="22" spans="2:40" x14ac:dyDescent="0.25">
       <c r="B22" s="28">
         <v>8.65</v>
       </c>
@@ -23703,7 +23821,7 @@
         <v>4.8599320882852286</v>
       </c>
     </row>
-    <row r="23" spans="2:40" ht="15">
+    <row r="23" spans="2:40" x14ac:dyDescent="0.25">
       <c r="B23" s="28">
         <v>10.210000000000001</v>
       </c>
@@ -23818,7 +23936,7 @@
         <v>6.9994317105512422</v>
       </c>
     </row>
-    <row r="24" spans="2:40" ht="15">
+    <row r="24" spans="2:40" x14ac:dyDescent="0.25">
       <c r="B24" s="28">
         <v>12.05</v>
       </c>
@@ -23933,7 +24051,7 @@
         <v>5.3831231813773046</v>
       </c>
     </row>
-    <row r="25" spans="2:40" ht="15">
+    <row r="25" spans="2:40" x14ac:dyDescent="0.25">
       <c r="B25" s="28">
         <v>14.22</v>
       </c>
@@ -24048,7 +24166,7 @@
         <v>4.8810572687224667</v>
       </c>
     </row>
-    <row r="26" spans="2:40" ht="15">
+    <row r="26" spans="2:40" x14ac:dyDescent="0.25">
       <c r="B26" s="28">
         <v>16.78</v>
       </c>
@@ -24163,7 +24281,7 @@
         <v>3.6150765122727742</v>
       </c>
     </row>
-    <row r="27" spans="2:40" ht="15">
+    <row r="27" spans="2:40" x14ac:dyDescent="0.25">
       <c r="B27" s="28">
         <v>19.809999999999999</v>
       </c>
@@ -24278,7 +24396,7 @@
         <v>6.7727574121436023</v>
       </c>
     </row>
-    <row r="28" spans="2:40" ht="15">
+    <row r="28" spans="2:40" x14ac:dyDescent="0.25">
       <c r="B28" s="28">
         <v>23.37</v>
       </c>
@@ -24393,7 +24511,7 @@
         <v>5.6459777275913119</v>
       </c>
     </row>
-    <row r="29" spans="2:40" ht="15">
+    <row r="29" spans="2:40" x14ac:dyDescent="0.25">
       <c r="B29" s="28">
         <v>27.58</v>
       </c>
@@ -24465,7 +24583,7 @@
         <v>5.8188021228203191</v>
       </c>
     </row>
-    <row r="30" spans="2:40" ht="15">
+    <row r="30" spans="2:40" x14ac:dyDescent="0.25">
       <c r="B30" s="28">
         <v>32.549999999999997</v>
       </c>
@@ -24538,7 +24656,7 @@
       </c>
       <c r="AH30" s="83"/>
     </row>
-    <row r="31" spans="2:40" ht="15">
+    <row r="31" spans="2:40" x14ac:dyDescent="0.25">
       <c r="B31" s="28">
         <v>38.409999999999997</v>
       </c>
@@ -24609,14 +24727,14 @@
       <c r="Y31" s="380">
         <v>6.6148597422289619</v>
       </c>
-      <c r="AA31" s="479" t="s">
+      <c r="AA31" s="446" t="s">
         <v>25</v>
       </c>
-      <c r="AB31" s="479"/>
-      <c r="AC31" s="480" t="s">
+      <c r="AB31" s="446"/>
+      <c r="AC31" s="447" t="s">
         <v>40</v>
       </c>
-      <c r="AD31" s="480"/>
+      <c r="AD31" s="447"/>
       <c r="AJ31" s="230" t="s">
         <v>76</v>
       </c>
@@ -24633,7 +24751,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="32" spans="2:40" ht="15">
+    <row r="32" spans="2:40" x14ac:dyDescent="0.25">
       <c r="B32" s="28">
         <v>45.32</v>
       </c>
@@ -24736,7 +24854,7 @@
         <v>3.6685446490482859E-2</v>
       </c>
     </row>
-    <row r="33" spans="2:40" ht="15.75" thickBot="1">
+    <row r="33" spans="2:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B33" s="28">
         <v>53.48</v>
       </c>
@@ -24843,7 +24961,7 @@
         <v>0.11306722777991254</v>
       </c>
     </row>
-    <row r="34" spans="2:40" ht="15">
+    <row r="34" spans="2:40" x14ac:dyDescent="0.25">
       <c r="B34" s="14">
         <v>63.11</v>
       </c>
@@ -24950,7 +25068,7 @@
         <v>4.7747439937281255E-2</v>
       </c>
     </row>
-    <row r="35" spans="2:40" ht="15">
+    <row r="35" spans="2:40" x14ac:dyDescent="0.25">
       <c r="B35" s="28">
         <v>74.48</v>
       </c>
@@ -25057,7 +25175,7 @@
         <v>-0.18932400123422785</v>
       </c>
     </row>
-    <row r="36" spans="2:40" ht="15">
+    <row r="36" spans="2:40" x14ac:dyDescent="0.25">
       <c r="B36" s="28">
         <v>87.89</v>
       </c>
@@ -25164,7 +25282,7 @@
         <v>-9.8289875653147785E-2</v>
       </c>
     </row>
-    <row r="37" spans="2:40" ht="15">
+    <row r="37" spans="2:40" x14ac:dyDescent="0.25">
       <c r="B37" s="28">
         <v>103.72</v>
       </c>
@@ -25271,7 +25389,7 @@
         <v>-6.4526904685237918E-2</v>
       </c>
     </row>
-    <row r="38" spans="2:40" ht="15">
+    <row r="38" spans="2:40" x14ac:dyDescent="0.25">
       <c r="B38" s="28">
         <v>122.39</v>
       </c>
@@ -25378,7 +25496,7 @@
         <v>4.5248200775063058E-2</v>
       </c>
     </row>
-    <row r="39" spans="2:40" ht="15">
+    <row r="39" spans="2:40" x14ac:dyDescent="0.25">
       <c r="B39" s="28">
         <v>144.43</v>
       </c>
@@ -25485,7 +25603,7 @@
         <v>1.9282470866228862E-2</v>
       </c>
     </row>
-    <row r="40" spans="2:40" ht="15">
+    <row r="40" spans="2:40" x14ac:dyDescent="0.25">
       <c r="B40" s="28">
         <v>170.44</v>
       </c>
@@ -25592,7 +25710,7 @@
         <v>0.10979374564456568</v>
       </c>
     </row>
-    <row r="41" spans="2:40" ht="15">
+    <row r="41" spans="2:40" x14ac:dyDescent="0.25">
       <c r="B41" s="28">
         <v>201.13</v>
       </c>
@@ -25699,7 +25817,7 @@
         <v>0.20807480090515129</v>
       </c>
     </row>
-    <row r="42" spans="2:40" ht="15">
+    <row r="42" spans="2:40" x14ac:dyDescent="0.25">
       <c r="B42" s="28">
         <v>237.35</v>
       </c>
@@ -25787,7 +25905,7 @@
         <v>0.42567774936061398</v>
       </c>
     </row>
-    <row r="43" spans="2:40" ht="15">
+    <row r="43" spans="2:40" x14ac:dyDescent="0.25">
       <c r="B43" s="28">
         <v>280.08999999999997</v>
       </c>
@@ -25875,7 +25993,7 @@
         <v>1.3266062144692778</v>
       </c>
     </row>
-    <row r="44" spans="2:40" ht="15">
+    <row r="44" spans="2:40" x14ac:dyDescent="0.25">
       <c r="B44" s="28">
         <v>330.52</v>
       </c>
@@ -25947,7 +26065,7 @@
         <v>2.5208491281273697</v>
       </c>
     </row>
-    <row r="45" spans="2:40" ht="15">
+    <row r="45" spans="2:40" x14ac:dyDescent="0.25">
       <c r="B45" s="28">
         <v>390.04</v>
       </c>
@@ -26019,7 +26137,7 @@
         <v>2.388172858225929</v>
       </c>
     </row>
-    <row r="46" spans="2:40" ht="15.75" thickBot="1">
+    <row r="46" spans="2:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B46" s="42">
         <v>460.27</v>
       </c>
@@ -26091,7 +26209,7 @@
         <v>2.1322971948445799</v>
       </c>
     </row>
-    <row r="47" spans="2:40" ht="15">
+    <row r="47" spans="2:40" x14ac:dyDescent="0.25">
       <c r="B47" s="1" t="s">
         <v>24</v>
       </c>
@@ -26166,13 +26284,13 @@
         <v>100</v>
       </c>
     </row>
-    <row r="53" spans="2:21">
+    <row r="53" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="54" spans="2:21" ht="15" thickBot="1"/>
-    <row r="55" spans="2:21">
+    <row r="54" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="55" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B55" s="485" t="s">
         <v>1</v>
       </c>
@@ -26202,7 +26320,7 @@
       <c r="T55" s="486"/>
       <c r="U55" s="487"/>
     </row>
-    <row r="56" spans="2:21" ht="15" thickBot="1">
+    <row r="56" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B56" s="92" t="s">
         <v>65</v>
       </c>
@@ -26264,7 +26382,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="57" spans="2:21">
+    <row r="57" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B57" s="165">
         <v>5</v>
       </c>
@@ -26326,7 +26444,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="58" spans="2:21">
+    <row r="58" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B58" s="168">
         <v>1</v>
       </c>
@@ -26388,7 +26506,7 @@
         <v>93.215838326871108</v>
       </c>
     </row>
-    <row r="59" spans="2:21" ht="15" thickBot="1">
+    <row r="59" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B59" s="170">
         <v>0.85</v>
       </c>
@@ -26450,7 +26568,7 @@
         <v>91.816472799906009</v>
       </c>
     </row>
-    <row r="60" spans="2:21">
+    <row r="60" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B60" s="165">
         <v>0.3</v>
       </c>
@@ -26512,7 +26630,7 @@
         <v>70.403007872165432</v>
       </c>
     </row>
-    <row r="61" spans="2:21">
+    <row r="61" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B61" s="168">
         <v>0.25</v>
       </c>
@@ -26574,7 +26692,7 @@
         <v>63.588297497356365</v>
       </c>
     </row>
-    <row r="62" spans="2:21">
+    <row r="62" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B62" s="168">
         <v>0.125</v>
       </c>
@@ -26636,7 +26754,7 @@
         <v>41.543884384913639</v>
       </c>
     </row>
-    <row r="63" spans="2:21" ht="15" thickBot="1">
+    <row r="63" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B63" s="170">
         <v>6.3E-2</v>
       </c>
@@ -26698,7 +26816,7 @@
         <v>23.931382916226056</v>
       </c>
     </row>
-    <row r="64" spans="2:21">
+    <row r="64" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B64" s="165">
         <v>5.2999999999999999E-2</v>
       </c>
@@ -26760,7 +26878,7 @@
         <v>20.16214310891786</v>
       </c>
     </row>
-    <row r="65" spans="2:21">
+    <row r="65" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B65" s="168">
         <v>3.7999999999999999E-2</v>
       </c>
@@ -26822,7 +26940,7 @@
         <v>10.078721654329684</v>
       </c>
     </row>
-    <row r="66" spans="2:21" ht="15" thickBot="1">
+    <row r="66" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B66" s="170">
         <v>2.5000000000000001E-2</v>
       </c>
@@ -26884,7 +27002,7 @@
         <v>0.23616496298906497</v>
       </c>
     </row>
-    <row r="67" spans="2:21">
+    <row r="67" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B67" s="148" t="s">
         <v>70</v>
       </c>
@@ -26946,7 +27064,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="2:21" ht="15.75" thickBot="1">
+    <row r="68" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B68" s="143" t="s">
         <v>24</v>
       </c>
@@ -26986,24 +27104,24 @@
       <c r="T68" s="146"/>
       <c r="U68" s="147"/>
     </row>
-    <row r="69" spans="2:21" ht="15" thickBot="1"/>
-    <row r="70" spans="2:21">
-      <c r="B70" s="448" t="s">
+    <row r="69" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="70" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B70" s="476" t="s">
         <v>95</v>
       </c>
-      <c r="C70" s="449"/>
-      <c r="D70" s="449"/>
-      <c r="E70" s="449"/>
-      <c r="F70" s="450"/>
-      <c r="G70" s="448" t="s">
+      <c r="C70" s="477"/>
+      <c r="D70" s="477"/>
+      <c r="E70" s="477"/>
+      <c r="F70" s="478"/>
+      <c r="G70" s="476" t="s">
         <v>6</v>
       </c>
-      <c r="H70" s="449"/>
-      <c r="I70" s="449"/>
-      <c r="J70" s="449"/>
-      <c r="K70" s="450"/>
-    </row>
-    <row r="71" spans="2:21" ht="15" thickBot="1">
+      <c r="H70" s="477"/>
+      <c r="I70" s="477"/>
+      <c r="J70" s="477"/>
+      <c r="K70" s="478"/>
+    </row>
+    <row r="71" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B71" s="150" t="s">
         <v>65</v>
       </c>
@@ -27035,7 +27153,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="72" spans="2:21">
+    <row r="72" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B72" s="156">
         <v>5</v>
       </c>
@@ -27067,7 +27185,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="73" spans="2:21">
+    <row r="73" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B73" s="98">
         <v>1</v>
       </c>
@@ -27099,7 +27217,7 @@
         <v>62.622398414271558</v>
       </c>
     </row>
-    <row r="74" spans="2:21" ht="15" thickBot="1">
+    <row r="74" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B74" s="159">
         <v>0.85</v>
       </c>
@@ -27131,7 +27249,7 @@
         <v>58.313842087875784</v>
       </c>
     </row>
-    <row r="75" spans="2:21">
+    <row r="75" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B75" s="156">
         <v>0.3</v>
       </c>
@@ -27163,7 +27281,7 @@
         <v>36.936901222332338</v>
       </c>
     </row>
-    <row r="76" spans="2:21">
+    <row r="76" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B76" s="98">
         <v>0.25</v>
       </c>
@@ -27195,7 +27313,7 @@
         <v>33.714568880079284</v>
       </c>
     </row>
-    <row r="77" spans="2:21">
+    <row r="77" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B77" s="98">
         <v>0.125</v>
       </c>
@@ -27227,7 +27345,7 @@
         <v>23.1219028741328</v>
       </c>
     </row>
-    <row r="78" spans="2:21" ht="15" thickBot="1">
+    <row r="78" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B78" s="159">
         <v>6.3E-2</v>
       </c>
@@ -27259,7 +27377,7 @@
         <v>14.62371985464155</v>
       </c>
     </row>
-    <row r="79" spans="2:21">
+    <row r="79" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B79" s="156">
         <v>5.2999999999999999E-2</v>
       </c>
@@ -27291,7 +27409,7 @@
         <v>12.635612817971577</v>
       </c>
     </row>
-    <row r="80" spans="2:21">
+    <row r="80" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B80" s="98">
         <v>3.7999999999999999E-2</v>
       </c>
@@ -27323,7 +27441,7 @@
         <v>7.4364056821935804</v>
       </c>
     </row>
-    <row r="81" spans="2:11">
+    <row r="81" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B81" s="98">
         <v>2.5000000000000001E-2</v>
       </c>
@@ -27355,7 +27473,7 @@
         <v>1.0009910802774868</v>
       </c>
     </row>
-    <row r="82" spans="2:11" ht="15" thickBot="1">
+    <row r="82" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B82" s="159" t="s">
         <v>70</v>
       </c>
@@ -27387,7 +27505,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="2:11" ht="15.75" thickBot="1">
+    <row r="83" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B83" s="160" t="s">
         <v>24</v>
       </c>
@@ -27407,8 +27525,8 @@
       <c r="J83" s="163"/>
       <c r="K83" s="164"/>
     </row>
-    <row r="84" spans="2:11" ht="15" thickBot="1"/>
-    <row r="85" spans="2:11">
+    <row r="84" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="85" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B85" s="488" t="s">
         <v>7</v>
       </c>
@@ -27424,7 +27542,7 @@
       <c r="J85" s="489"/>
       <c r="K85" s="490"/>
     </row>
-    <row r="86" spans="2:11" ht="15" thickBot="1">
+    <row r="86" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B86" s="173" t="s">
         <v>65</v>
       </c>
@@ -27456,7 +27574,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="87" spans="2:11">
+    <row r="87" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B87" s="179">
         <v>5</v>
       </c>
@@ -27488,7 +27606,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="88" spans="2:11">
+    <row r="88" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B88" s="107">
         <v>1</v>
       </c>
@@ -27520,7 +27638,7 @@
         <v>81.952920210947298</v>
       </c>
     </row>
-    <row r="89" spans="2:11" ht="15" thickBot="1">
+    <row r="89" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B89" s="182">
         <v>0.85</v>
       </c>
@@ -27552,7 +27670,7 @@
         <v>77.327828258234291</v>
       </c>
     </row>
-    <row r="90" spans="2:11">
+    <row r="90" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B90" s="179">
         <v>0.3</v>
       </c>
@@ -27584,7 +27702,7 @@
         <v>43.410487271672345</v>
       </c>
     </row>
-    <row r="91" spans="2:11">
+    <row r="91" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B91" s="107">
         <v>0.25</v>
       </c>
@@ -27616,7 +27734,7 @@
         <v>39.51790876218697</v>
       </c>
     </row>
-    <row r="92" spans="2:11">
+    <row r="92" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B92" s="107">
         <v>0.125</v>
       </c>
@@ -27648,7 +27766,7 @@
         <v>26.769895458831087</v>
       </c>
     </row>
-    <row r="93" spans="2:11" ht="15" thickBot="1">
+    <row r="93" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B93" s="182">
         <v>6.3E-2</v>
       </c>
@@ -27680,7 +27798,7 @@
         <v>16.913600712827787</v>
       </c>
     </row>
-    <row r="94" spans="2:11">
+    <row r="94" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B94" s="176">
         <v>5.2999999999999999E-2</v>
       </c>
@@ -27712,7 +27830,7 @@
         <v>14.673062776505688</v>
       </c>
     </row>
-    <row r="95" spans="2:11">
+    <row r="95" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B95" s="107">
         <v>3.7999999999999999E-2</v>
       </c>
@@ -27744,7 +27862,7 @@
         <v>8.7114187138017058</v>
       </c>
     </row>
-    <row r="96" spans="2:11">
+    <row r="96" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B96" s="107">
         <v>2.5000000000000001E-2</v>
       </c>
@@ -27776,7 +27894,7 @@
         <v>0.67967301097215227</v>
       </c>
     </row>
-    <row r="97" spans="2:21" ht="15" thickBot="1">
+    <row r="97" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B97" s="109" t="s">
         <v>70</v>
       </c>
@@ -27808,7 +27926,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="2:21" ht="15.75" thickBot="1">
+    <row r="98" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B98" s="111" t="s">
         <v>24</v>
       </c>
@@ -27830,38 +27948,38 @@
       <c r="J98" s="114"/>
       <c r="K98" s="115"/>
     </row>
-    <row r="99" spans="2:21" ht="15" thickBot="1"/>
-    <row r="100" spans="2:21">
-      <c r="B100" s="460" t="s">
+    <row r="99" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="100" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B100" s="467" t="s">
         <v>9</v>
       </c>
-      <c r="C100" s="461"/>
-      <c r="D100" s="461"/>
-      <c r="E100" s="461"/>
-      <c r="F100" s="462"/>
-      <c r="G100" s="460" t="s">
+      <c r="C100" s="468"/>
+      <c r="D100" s="468"/>
+      <c r="E100" s="468"/>
+      <c r="F100" s="469"/>
+      <c r="G100" s="467" t="s">
         <v>10</v>
       </c>
-      <c r="H100" s="461"/>
-      <c r="I100" s="461"/>
-      <c r="J100" s="461"/>
-      <c r="K100" s="462"/>
-      <c r="L100" s="460" t="s">
+      <c r="H100" s="468"/>
+      <c r="I100" s="468"/>
+      <c r="J100" s="468"/>
+      <c r="K100" s="469"/>
+      <c r="L100" s="467" t="s">
         <v>11</v>
       </c>
-      <c r="M100" s="461"/>
-      <c r="N100" s="461"/>
-      <c r="O100" s="461"/>
-      <c r="P100" s="462"/>
-      <c r="Q100" s="460" t="s">
+      <c r="M100" s="468"/>
+      <c r="N100" s="468"/>
+      <c r="O100" s="468"/>
+      <c r="P100" s="469"/>
+      <c r="Q100" s="467" t="s">
         <v>12</v>
       </c>
-      <c r="R100" s="461"/>
-      <c r="S100" s="461"/>
-      <c r="T100" s="461"/>
-      <c r="U100" s="462"/>
-    </row>
-    <row r="101" spans="2:21" ht="15" thickBot="1">
+      <c r="R100" s="468"/>
+      <c r="S100" s="468"/>
+      <c r="T100" s="468"/>
+      <c r="U100" s="469"/>
+    </row>
+    <row r="101" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B101" s="183" t="s">
         <v>65</v>
       </c>
@@ -27923,7 +28041,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="102" spans="2:21">
+    <row r="102" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B102" s="189">
         <v>5</v>
       </c>
@@ -27985,7 +28103,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="103" spans="2:21">
+    <row r="103" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B103" s="116">
         <v>1</v>
       </c>
@@ -28047,7 +28165,7 @@
         <v>69.68717242029139</v>
       </c>
     </row>
-    <row r="104" spans="2:21" ht="15" thickBot="1">
+    <row r="104" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B104" s="192">
         <v>0.85</v>
       </c>
@@ -28109,7 +28227,7 @@
         <v>62.622051046488345</v>
       </c>
     </row>
-    <row r="105" spans="2:21">
+    <row r="105" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B105" s="189">
         <v>0.3</v>
       </c>
@@ -28171,7 +28289,7 @@
         <v>34.155447981814547</v>
       </c>
     </row>
-    <row r="106" spans="2:21">
+    <row r="106" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B106" s="116">
         <v>0.25</v>
       </c>
@@ -28233,7 +28351,7 @@
         <v>31.425273547460051</v>
       </c>
     </row>
-    <row r="107" spans="2:21">
+    <row r="107" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B107" s="116">
         <v>0.125</v>
       </c>
@@ -28295,7 +28413,7 @@
         <v>22.252452799076593</v>
       </c>
     </row>
-    <row r="108" spans="2:21" ht="15" thickBot="1">
+    <row r="108" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B108" s="192">
         <v>6.3E-2</v>
       </c>
@@ -28357,7 +28475,7 @@
         <v>14.133776191654007</v>
       </c>
     </row>
-    <row r="109" spans="2:21">
+    <row r="109" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B109" s="186">
         <v>5.2999999999999999E-2</v>
       </c>
@@ -28419,7 +28537,7 @@
         <v>12.034321519852071</v>
       </c>
     </row>
-    <row r="110" spans="2:21">
+    <row r="110" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B110" s="116">
         <v>3.7999999999999999E-2</v>
       </c>
@@ -28481,7 +28599,7 @@
         <v>6.4662026076817085</v>
       </c>
     </row>
-    <row r="111" spans="2:21">
+    <row r="111" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B111" s="116">
         <v>2.5000000000000001E-2</v>
       </c>
@@ -28543,7 +28661,7 @@
         <v>1.5017137203632416</v>
       </c>
     </row>
-    <row r="112" spans="2:21" ht="15" thickBot="1">
+    <row r="112" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B112" s="118" t="s">
         <v>70</v>
       </c>
@@ -28605,7 +28723,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="2:21" ht="15.75" thickBot="1">
+    <row r="113" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B113" s="120" t="s">
         <v>24</v>
       </c>
@@ -28645,38 +28763,38 @@
       <c r="T113" s="123"/>
       <c r="U113" s="124"/>
     </row>
-    <row r="114" spans="2:21" ht="15" thickBot="1"/>
-    <row r="115" spans="2:21">
-      <c r="B115" s="463" t="s">
+    <row r="114" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="115" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B115" s="470" t="s">
         <v>13</v>
       </c>
-      <c r="C115" s="464"/>
-      <c r="D115" s="464"/>
-      <c r="E115" s="464"/>
-      <c r="F115" s="465"/>
-      <c r="G115" s="466" t="s">
+      <c r="C115" s="471"/>
+      <c r="D115" s="471"/>
+      <c r="E115" s="471"/>
+      <c r="F115" s="472"/>
+      <c r="G115" s="473" t="s">
         <v>14</v>
       </c>
-      <c r="H115" s="467"/>
-      <c r="I115" s="467"/>
-      <c r="J115" s="467"/>
-      <c r="K115" s="468"/>
-      <c r="L115" s="466" t="s">
+      <c r="H115" s="474"/>
+      <c r="I115" s="474"/>
+      <c r="J115" s="474"/>
+      <c r="K115" s="475"/>
+      <c r="L115" s="473" t="s">
         <v>15</v>
       </c>
-      <c r="M115" s="467"/>
-      <c r="N115" s="467"/>
-      <c r="O115" s="467"/>
-      <c r="P115" s="468"/>
-      <c r="Q115" s="466" t="s">
+      <c r="M115" s="474"/>
+      <c r="N115" s="474"/>
+      <c r="O115" s="474"/>
+      <c r="P115" s="475"/>
+      <c r="Q115" s="473" t="s">
         <v>16</v>
       </c>
-      <c r="R115" s="467"/>
-      <c r="S115" s="467"/>
-      <c r="T115" s="467"/>
-      <c r="U115" s="468"/>
-    </row>
-    <row r="116" spans="2:21" ht="15" thickBot="1">
+      <c r="R115" s="474"/>
+      <c r="S115" s="474"/>
+      <c r="T115" s="474"/>
+      <c r="U115" s="475"/>
+    </row>
+    <row r="116" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B116" s="193" t="s">
         <v>65</v>
       </c>
@@ -28738,7 +28856,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="117" spans="2:21">
+    <row r="117" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B117" s="199"/>
       <c r="C117" s="200"/>
       <c r="D117" s="200"/>
@@ -28790,7 +28908,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="118" spans="2:21">
+    <row r="118" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B118" s="125"/>
       <c r="C118" s="68"/>
       <c r="D118" s="68"/>
@@ -28842,7 +28960,7 @@
         <v>62.763915547024951</v>
       </c>
     </row>
-    <row r="119" spans="2:21" ht="15" thickBot="1">
+    <row r="119" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B119" s="202"/>
       <c r="C119" s="132"/>
       <c r="D119" s="132"/>
@@ -28894,7 +29012,7 @@
         <v>58.108906879902236</v>
       </c>
     </row>
-    <row r="120" spans="2:21">
+    <row r="120" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B120" s="199"/>
       <c r="C120" s="200"/>
       <c r="D120" s="200"/>
@@ -28946,7 +29064,7 @@
         <v>31.83789491860874</v>
       </c>
     </row>
-    <row r="121" spans="2:21">
+    <row r="121" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B121" s="125"/>
       <c r="C121" s="68"/>
       <c r="D121" s="68"/>
@@ -28998,7 +29116,7 @@
         <v>28.337174318750868</v>
       </c>
     </row>
-    <row r="122" spans="2:21">
+    <row r="122" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B122" s="125"/>
       <c r="C122" s="68"/>
       <c r="D122" s="68"/>
@@ -29050,7 +29168,7 @@
         <v>19.184559902768825</v>
       </c>
     </row>
-    <row r="123" spans="2:21" ht="15" thickBot="1">
+    <row r="123" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B123" s="202"/>
       <c r="C123" s="132"/>
       <c r="D123" s="132"/>
@@ -29102,7 +29220,7 @@
         <v>12.784836188059955</v>
       </c>
     </row>
-    <row r="124" spans="2:21">
+    <row r="124" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B124" s="196"/>
       <c r="C124" s="197"/>
       <c r="D124" s="197"/>
@@ -29154,7 +29272,7 @@
         <v>10.82626569878262</v>
       </c>
     </row>
-    <row r="125" spans="2:21">
+    <row r="125" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B125" s="125"/>
       <c r="C125" s="68"/>
       <c r="D125" s="68"/>
@@ -29206,7 +29324,7 @@
         <v>6.5624398116478204</v>
       </c>
     </row>
-    <row r="126" spans="2:21">
+    <row r="126" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B126" s="125"/>
       <c r="C126" s="68"/>
       <c r="D126" s="68"/>
@@ -29258,7 +29376,7 @@
         <v>2.2806819464830141</v>
       </c>
     </row>
-    <row r="127" spans="2:21" ht="15" thickBot="1">
+    <row r="127" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B127" s="127"/>
       <c r="C127" s="128"/>
       <c r="D127" s="68"/>
@@ -29310,7 +29428,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="128" spans="2:21" ht="15.75" thickBot="1">
+    <row r="128" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B128" s="129"/>
       <c r="C128" s="130"/>
       <c r="D128" s="131"/>
@@ -29344,38 +29462,38 @@
       <c r="T128" s="132"/>
       <c r="U128" s="133"/>
     </row>
-    <row r="129" spans="2:21" ht="15" thickBot="1"/>
-    <row r="130" spans="2:21">
-      <c r="B130" s="448" t="s">
+    <row r="129" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="130" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B130" s="476" t="s">
         <v>17</v>
       </c>
-      <c r="C130" s="449"/>
-      <c r="D130" s="449"/>
-      <c r="E130" s="449"/>
-      <c r="F130" s="450"/>
-      <c r="G130" s="448" t="s">
+      <c r="C130" s="477"/>
+      <c r="D130" s="477"/>
+      <c r="E130" s="477"/>
+      <c r="F130" s="478"/>
+      <c r="G130" s="476" t="s">
         <v>18</v>
       </c>
-      <c r="H130" s="449"/>
-      <c r="I130" s="449"/>
-      <c r="J130" s="449"/>
-      <c r="K130" s="450"/>
-      <c r="L130" s="448" t="s">
+      <c r="H130" s="477"/>
+      <c r="I130" s="477"/>
+      <c r="J130" s="477"/>
+      <c r="K130" s="478"/>
+      <c r="L130" s="476" t="s">
         <v>19</v>
       </c>
-      <c r="M130" s="449"/>
-      <c r="N130" s="449"/>
-      <c r="O130" s="449"/>
-      <c r="P130" s="450"/>
-      <c r="Q130" s="448" t="s">
+      <c r="M130" s="477"/>
+      <c r="N130" s="477"/>
+      <c r="O130" s="477"/>
+      <c r="P130" s="478"/>
+      <c r="Q130" s="476" t="s">
         <v>20</v>
       </c>
-      <c r="R130" s="449"/>
-      <c r="S130" s="449"/>
-      <c r="T130" s="449"/>
-      <c r="U130" s="450"/>
-    </row>
-    <row r="131" spans="2:21" ht="15" thickBot="1">
+      <c r="R130" s="477"/>
+      <c r="S130" s="477"/>
+      <c r="T130" s="477"/>
+      <c r="U130" s="478"/>
+    </row>
+    <row r="131" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B131" s="150" t="s">
         <v>65</v>
       </c>
@@ -29437,7 +29555,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="132" spans="2:21">
+    <row r="132" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B132" s="156">
         <v>5</v>
       </c>
@@ -29499,7 +29617,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="133" spans="2:21">
+    <row r="133" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B133" s="98">
         <v>1</v>
       </c>
@@ -29561,7 +29679,7 @@
         <v>93.219644306574622</v>
       </c>
     </row>
-    <row r="134" spans="2:21" ht="15" thickBot="1">
+    <row r="134" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B134" s="159">
         <v>0.85</v>
       </c>
@@ -29623,7 +29741,7 @@
         <v>89.639404338077526</v>
       </c>
     </row>
-    <row r="135" spans="2:21">
+    <row r="135" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B135" s="156">
         <v>0.3</v>
       </c>
@@ -29685,7 +29803,7 @@
         <v>57.752364726398945</v>
       </c>
     </row>
-    <row r="136" spans="2:21">
+    <row r="136" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B136" s="98">
         <v>0.25</v>
       </c>
@@ -29747,7 +29865,7 @@
         <v>53.000409859120971</v>
       </c>
     </row>
-    <row r="137" spans="2:21">
+    <row r="137" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B137" s="98">
         <v>0.125</v>
       </c>
@@ -29809,7 +29927,7 @@
         <v>36.648638222979429</v>
       </c>
     </row>
-    <row r="138" spans="2:21" ht="15" thickBot="1">
+    <row r="138" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B138" s="159">
         <v>6.3E-2</v>
       </c>
@@ -29871,7 +29989,7 @@
         <v>23.336253244718037</v>
       </c>
     </row>
-    <row r="139" spans="2:21">
+    <row r="139" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B139" s="153">
         <v>5.2999999999999999E-2</v>
       </c>
@@ -29933,7 +30051,7 @@
         <v>20.530727379392928</v>
       </c>
     </row>
-    <row r="140" spans="2:21">
+    <row r="140" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B140" s="98">
         <v>3.7999999999999999E-2</v>
       </c>
@@ -29995,7 +30113,7 @@
         <v>12.039410767240199</v>
       </c>
     </row>
-    <row r="141" spans="2:21">
+    <row r="141" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B141" s="98">
         <v>2.5000000000000001E-2</v>
       </c>
@@ -30057,7 +30175,7 @@
         <v>1.6322036758737681</v>
       </c>
     </row>
-    <row r="142" spans="2:21" ht="15" thickBot="1">
+    <row r="142" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B142" s="100" t="s">
         <v>70</v>
       </c>
@@ -30119,7 +30237,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="143" spans="2:21" ht="15.75" thickBot="1">
+    <row r="143" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B143" s="102" t="s">
         <v>24</v>
       </c>
@@ -30159,31 +30277,31 @@
       <c r="T143" s="105"/>
       <c r="U143" s="106"/>
     </row>
-    <row r="144" spans="2:21" ht="15" thickBot="1"/>
-    <row r="145" spans="2:16">
-      <c r="B145" s="454" t="s">
+    <row r="144" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="145" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B145" s="482" t="s">
         <v>21</v>
       </c>
-      <c r="C145" s="455"/>
-      <c r="D145" s="455"/>
-      <c r="E145" s="455"/>
-      <c r="F145" s="456"/>
-      <c r="G145" s="454" t="s">
+      <c r="C145" s="483"/>
+      <c r="D145" s="483"/>
+      <c r="E145" s="483"/>
+      <c r="F145" s="484"/>
+      <c r="G145" s="482" t="s">
         <v>22</v>
       </c>
-      <c r="H145" s="455"/>
-      <c r="I145" s="455"/>
-      <c r="J145" s="455"/>
-      <c r="K145" s="456"/>
-      <c r="L145" s="454" t="s">
+      <c r="H145" s="483"/>
+      <c r="I145" s="483"/>
+      <c r="J145" s="483"/>
+      <c r="K145" s="484"/>
+      <c r="L145" s="482" t="s">
         <v>23</v>
       </c>
-      <c r="M145" s="455"/>
-      <c r="N145" s="455"/>
-      <c r="O145" s="455"/>
-      <c r="P145" s="456"/>
-    </row>
-    <row r="146" spans="2:16" ht="15" thickBot="1">
+      <c r="M145" s="483"/>
+      <c r="N145" s="483"/>
+      <c r="O145" s="483"/>
+      <c r="P145" s="484"/>
+    </row>
+    <row r="146" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B146" s="203" t="s">
         <v>65</v>
       </c>
@@ -30230,7 +30348,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="147" spans="2:16">
+    <row r="147" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B147" s="209">
         <v>5</v>
       </c>
@@ -30277,7 +30395,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="148" spans="2:16">
+    <row r="148" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B148" s="134">
         <v>1</v>
       </c>
@@ -30324,7 +30442,7 @@
         <v>89.367246568303599</v>
       </c>
     </row>
-    <row r="149" spans="2:16" ht="15" thickBot="1">
+    <row r="149" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B149" s="212">
         <v>0.85</v>
       </c>
@@ -30371,7 +30489,7 @@
         <v>84.236952213168905</v>
       </c>
     </row>
-    <row r="150" spans="2:16">
+    <row r="150" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B150" s="209">
         <v>0.3</v>
       </c>
@@ -30418,7 +30536,7 @@
         <v>48.262497247302349</v>
       </c>
     </row>
-    <row r="151" spans="2:16">
+    <row r="151" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B151" s="134">
         <v>0.25</v>
       </c>
@@ -30465,7 +30583,7 @@
         <v>42.709388534096739</v>
       </c>
     </row>
-    <row r="152" spans="2:16">
+    <row r="152" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B152" s="134">
         <v>0.125</v>
       </c>
@@ -30512,7 +30630,7 @@
         <v>26.479483226895681</v>
       </c>
     </row>
-    <row r="153" spans="2:16" ht="15" thickBot="1">
+    <row r="153" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B153" s="212">
         <v>6.3E-2</v>
       </c>
@@ -30559,7 +30677,7 @@
         <v>16.325332158848994</v>
       </c>
     </row>
-    <row r="154" spans="2:16">
+    <row r="154" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B154" s="206">
         <v>5.2999999999999999E-2</v>
       </c>
@@ -30606,7 +30724,7 @@
         <v>13.751743375174328</v>
       </c>
     </row>
-    <row r="155" spans="2:16">
+    <row r="155" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B155" s="134">
         <v>3.7999999999999999E-2</v>
       </c>
@@ -30653,7 +30771,7 @@
         <v>7.9196946340747161</v>
       </c>
     </row>
-    <row r="156" spans="2:16">
+    <row r="156" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B156" s="134">
         <v>2.5000000000000001E-2</v>
       </c>
@@ -30700,7 +30818,7 @@
         <v>1.7477794905674102</v>
       </c>
     </row>
-    <row r="157" spans="2:16" ht="15" thickBot="1">
+    <row r="157" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B157" s="136" t="s">
         <v>70</v>
       </c>
@@ -30747,7 +30865,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="158" spans="2:16" ht="15.75" thickBot="1">
+    <row r="158" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B158" s="138" t="s">
         <v>24</v>
       </c>
@@ -30780,24 +30898,17 @@
     </row>
   </sheetData>
   <mergeCells count="41">
-    <mergeCell ref="AL1:AL2"/>
-    <mergeCell ref="AB2:AC2"/>
-    <mergeCell ref="AD2:AE2"/>
-    <mergeCell ref="AG1:AG2"/>
-    <mergeCell ref="AH1:AH2"/>
-    <mergeCell ref="AI1:AI2"/>
-    <mergeCell ref="AJ1:AJ2"/>
-    <mergeCell ref="AK1:AK2"/>
-    <mergeCell ref="AK15:AK16"/>
-    <mergeCell ref="AL15:AL16"/>
-    <mergeCell ref="AB16:AC16"/>
-    <mergeCell ref="AD16:AE16"/>
-    <mergeCell ref="AA31:AB31"/>
-    <mergeCell ref="AC31:AD31"/>
-    <mergeCell ref="AJ15:AJ16"/>
-    <mergeCell ref="AG15:AG16"/>
-    <mergeCell ref="AH15:AH16"/>
-    <mergeCell ref="AI15:AI16"/>
+    <mergeCell ref="B145:F145"/>
+    <mergeCell ref="G145:K145"/>
+    <mergeCell ref="L145:P145"/>
+    <mergeCell ref="B115:F115"/>
+    <mergeCell ref="G115:K115"/>
+    <mergeCell ref="L115:P115"/>
+    <mergeCell ref="Q115:U115"/>
+    <mergeCell ref="B130:F130"/>
+    <mergeCell ref="G130:K130"/>
+    <mergeCell ref="L130:P130"/>
+    <mergeCell ref="Q130:U130"/>
     <mergeCell ref="Q100:U100"/>
     <mergeCell ref="B55:F55"/>
     <mergeCell ref="G55:K55"/>
@@ -30810,17 +30921,24 @@
     <mergeCell ref="B100:F100"/>
     <mergeCell ref="G100:K100"/>
     <mergeCell ref="L100:P100"/>
-    <mergeCell ref="Q115:U115"/>
-    <mergeCell ref="B130:F130"/>
-    <mergeCell ref="G130:K130"/>
-    <mergeCell ref="L130:P130"/>
-    <mergeCell ref="Q130:U130"/>
-    <mergeCell ref="B145:F145"/>
-    <mergeCell ref="G145:K145"/>
-    <mergeCell ref="L145:P145"/>
-    <mergeCell ref="B115:F115"/>
-    <mergeCell ref="G115:K115"/>
-    <mergeCell ref="L115:P115"/>
+    <mergeCell ref="AK15:AK16"/>
+    <mergeCell ref="AL15:AL16"/>
+    <mergeCell ref="AB16:AC16"/>
+    <mergeCell ref="AD16:AE16"/>
+    <mergeCell ref="AA31:AB31"/>
+    <mergeCell ref="AC31:AD31"/>
+    <mergeCell ref="AJ15:AJ16"/>
+    <mergeCell ref="AG15:AG16"/>
+    <mergeCell ref="AH15:AH16"/>
+    <mergeCell ref="AI15:AI16"/>
+    <mergeCell ref="AL1:AL2"/>
+    <mergeCell ref="AB2:AC2"/>
+    <mergeCell ref="AD2:AE2"/>
+    <mergeCell ref="AG1:AG2"/>
+    <mergeCell ref="AH1:AH2"/>
+    <mergeCell ref="AI1:AI2"/>
+    <mergeCell ref="AJ1:AJ2"/>
+    <mergeCell ref="AK1:AK2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -30831,68 +30949,68 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1F56B83-6FD0-4F97-A83F-B325F07CC791}">
   <dimension ref="A1:N40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E23" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="X5" sqref="X5"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.625" customWidth="1"/>
-    <col min="2" max="2" width="15.5" customWidth="1"/>
+    <col min="1" max="1" width="11.5703125" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" customWidth="1"/>
     <col min="3" max="3" width="18" customWidth="1"/>
-    <col min="4" max="4" width="9.25" customWidth="1"/>
-    <col min="5" max="5" width="14.875" customWidth="1"/>
-    <col min="6" max="6" width="19.5" customWidth="1"/>
-    <col min="8" max="8" width="14.5" customWidth="1"/>
-    <col min="9" max="9" width="18.25" customWidth="1"/>
-    <col min="11" max="11" width="17.625" customWidth="1"/>
-    <col min="12" max="12" width="16.375" customWidth="1"/>
-    <col min="14" max="14" width="12.5" customWidth="1"/>
+    <col min="4" max="4" width="9.28515625" customWidth="1"/>
+    <col min="5" max="5" width="14.85546875" customWidth="1"/>
+    <col min="6" max="6" width="19.42578125" customWidth="1"/>
+    <col min="8" max="8" width="14.42578125" customWidth="1"/>
+    <col min="9" max="9" width="18.28515625" customWidth="1"/>
+    <col min="11" max="11" width="17.5703125" customWidth="1"/>
+    <col min="12" max="12" width="16.42578125" customWidth="1"/>
+    <col min="14" max="14" width="12.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15" thickBot="1">
-      <c r="A1" s="476" t="s">
+    <row r="1" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="452" t="s">
         <v>96</v>
       </c>
-      <c r="B1" s="491"/>
-      <c r="C1" s="491"/>
-      <c r="D1" s="491"/>
-      <c r="E1" s="491"/>
-      <c r="F1" s="491"/>
-      <c r="G1" s="491"/>
-      <c r="H1" s="491"/>
-      <c r="I1" s="491"/>
-      <c r="J1" s="491"/>
-      <c r="K1" s="491"/>
-      <c r="L1" s="491"/>
-      <c r="M1" s="491"/>
-      <c r="N1" s="476"/>
-    </row>
-    <row r="2" spans="1:14">
+      <c r="B1" s="494"/>
+      <c r="C1" s="494"/>
+      <c r="D1" s="494"/>
+      <c r="E1" s="494"/>
+      <c r="F1" s="494"/>
+      <c r="G1" s="494"/>
+      <c r="H1" s="494"/>
+      <c r="I1" s="494"/>
+      <c r="J1" s="494"/>
+      <c r="K1" s="494"/>
+      <c r="L1" s="494"/>
+      <c r="M1" s="494"/>
+      <c r="N1" s="452"/>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="229"/>
-      <c r="B2" s="492" t="s">
+      <c r="B2" s="491" t="s">
         <v>111</v>
       </c>
-      <c r="C2" s="493"/>
-      <c r="D2" s="494"/>
-      <c r="E2" s="492" t="s">
+      <c r="C2" s="492"/>
+      <c r="D2" s="493"/>
+      <c r="E2" s="491" t="s">
         <v>108</v>
       </c>
-      <c r="F2" s="493"/>
-      <c r="G2" s="494"/>
-      <c r="H2" s="492" t="s">
+      <c r="F2" s="492"/>
+      <c r="G2" s="493"/>
+      <c r="H2" s="491" t="s">
         <v>110</v>
       </c>
-      <c r="I2" s="493"/>
-      <c r="J2" s="494"/>
-      <c r="K2" s="492" t="s">
+      <c r="I2" s="492"/>
+      <c r="J2" s="493"/>
+      <c r="K2" s="491" t="s">
         <v>75</v>
       </c>
-      <c r="L2" s="493"/>
-      <c r="M2" s="494"/>
+      <c r="L2" s="492"/>
+      <c r="M2" s="493"/>
       <c r="N2" s="246"/>
     </row>
-    <row r="3" spans="1:14" ht="15">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="230" t="s">
         <v>76</v>
       </c>
@@ -30936,7 +31054,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="15">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="231" t="s">
         <v>79</v>
       </c>
@@ -30988,7 +31106,7 @@
         <v>0.22851828638601948</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="15">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="231" t="s">
         <v>80</v>
       </c>
@@ -31040,7 +31158,7 @@
         <v>0.22851828638601948</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="15">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="232" t="s">
         <v>81</v>
       </c>
@@ -31092,7 +31210,7 @@
         <v>-0.3027637470411495</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="15">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="233" t="s">
         <v>82</v>
       </c>
@@ -31144,7 +31262,7 @@
         <v>-9.3318329100743891E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="15">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="234" t="s">
         <v>83</v>
       </c>
@@ -31196,7 +31314,7 @@
         <v>5.0766638815107075E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="15">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="234" t="s">
         <v>84</v>
       </c>
@@ -31248,7 +31366,7 @@
         <v>5.0766638815107075E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="15">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="235" t="s">
         <v>85</v>
       </c>
@@ -31300,7 +31418,7 @@
         <v>-3.8520880931257544E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="15">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="235" t="s">
         <v>86</v>
       </c>
@@ -31352,7 +31470,7 @@
         <v>-3.8520880931257544E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:14" ht="15">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="236" t="s">
         <v>87</v>
       </c>
@@ -31404,7 +31522,7 @@
         <v>-6.340384840026668E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="15">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="236" t="s">
         <v>88</v>
       </c>
@@ -31456,7 +31574,7 @@
         <v>-6.340384840026668E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:14" ht="15.75" thickBot="1">
+    <row r="14" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="237" t="s">
         <v>89</v>
       </c>
@@ -31508,49 +31626,49 @@
         <v>-3.2730377491297959E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="15" thickBot="1">
-      <c r="A16" s="476" t="s">
+    <row r="16" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="452" t="s">
         <v>106</v>
       </c>
-      <c r="B16" s="491"/>
-      <c r="C16" s="491"/>
-      <c r="D16" s="491"/>
-      <c r="E16" s="491"/>
-      <c r="F16" s="491"/>
-      <c r="G16" s="491"/>
-      <c r="H16" s="491"/>
-      <c r="I16" s="491"/>
-      <c r="J16" s="491"/>
-      <c r="K16" s="491"/>
-      <c r="L16" s="491"/>
-      <c r="M16" s="491"/>
-      <c r="N16" s="476"/>
-    </row>
-    <row r="17" spans="1:14">
+      <c r="B16" s="494"/>
+      <c r="C16" s="494"/>
+      <c r="D16" s="494"/>
+      <c r="E16" s="494"/>
+      <c r="F16" s="494"/>
+      <c r="G16" s="494"/>
+      <c r="H16" s="494"/>
+      <c r="I16" s="494"/>
+      <c r="J16" s="494"/>
+      <c r="K16" s="494"/>
+      <c r="L16" s="494"/>
+      <c r="M16" s="494"/>
+      <c r="N16" s="452"/>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="229"/>
-      <c r="B17" s="492" t="s">
+      <c r="B17" s="491" t="s">
         <v>111</v>
       </c>
-      <c r="C17" s="493"/>
-      <c r="D17" s="494"/>
-      <c r="E17" s="492" t="s">
+      <c r="C17" s="492"/>
+      <c r="D17" s="493"/>
+      <c r="E17" s="491" t="s">
         <v>109</v>
       </c>
-      <c r="F17" s="493"/>
-      <c r="G17" s="494"/>
-      <c r="H17" s="492" t="s">
+      <c r="F17" s="492"/>
+      <c r="G17" s="493"/>
+      <c r="H17" s="491" t="s">
         <v>110</v>
       </c>
-      <c r="I17" s="493"/>
-      <c r="J17" s="494"/>
-      <c r="K17" s="492" t="s">
+      <c r="I17" s="492"/>
+      <c r="J17" s="493"/>
+      <c r="K17" s="491" t="s">
         <v>75</v>
       </c>
-      <c r="L17" s="493"/>
-      <c r="M17" s="494"/>
+      <c r="L17" s="492"/>
+      <c r="M17" s="493"/>
       <c r="N17" s="246"/>
     </row>
-    <row r="18" spans="1:14" ht="15">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="230" t="s">
         <v>76</v>
       </c>
@@ -31594,7 +31712,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="19" spans="1:14" ht="15">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="231" t="s">
         <v>79</v>
       </c>
@@ -31646,7 +31764,7 @@
         <v>-0.10058679002726996</v>
       </c>
     </row>
-    <row r="20" spans="1:14" ht="15">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="231" t="s">
         <v>80</v>
       </c>
@@ -31698,7 +31816,7 @@
         <v>-0.10058679002726996</v>
       </c>
     </row>
-    <row r="21" spans="1:14" ht="15">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="232" t="s">
         <v>81</v>
       </c>
@@ -31750,7 +31868,7 @@
         <v>-0.32001589401318498</v>
       </c>
     </row>
-    <row r="22" spans="1:14" ht="15">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="234" t="s">
         <v>83</v>
       </c>
@@ -31802,7 +31920,7 @@
         <v>0.11743877238132332</v>
       </c>
     </row>
-    <row r="23" spans="1:14" ht="15">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="234" t="s">
         <v>84</v>
       </c>
@@ -31854,7 +31972,7 @@
         <v>0.11743877238132332</v>
       </c>
     </row>
-    <row r="24" spans="1:14" ht="15">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" s="235" t="s">
         <v>86</v>
       </c>
@@ -31906,7 +32024,7 @@
         <v>-4.5718099286610456E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:14" ht="15">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" s="236" t="s">
         <v>87</v>
       </c>
@@ -31958,7 +32076,7 @@
         <v>-0.11251612892623995</v>
       </c>
     </row>
-    <row r="26" spans="1:14" ht="15">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" s="236" t="s">
         <v>88</v>
       </c>
@@ -32010,7 +32128,7 @@
         <v>-0.11251612892623995</v>
       </c>
     </row>
-    <row r="27" spans="1:14" ht="15.75" thickBot="1">
+    <row r="27" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="237" t="s">
         <v>89</v>
       </c>
@@ -32062,49 +32180,49 @@
         <v>-4.9570413884485784E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:14" ht="15" thickBot="1">
-      <c r="A30" s="476" t="s">
+    <row r="30" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="452" t="s">
         <v>107</v>
       </c>
-      <c r="B30" s="491"/>
-      <c r="C30" s="491"/>
-      <c r="D30" s="491"/>
-      <c r="E30" s="491"/>
-      <c r="F30" s="491"/>
-      <c r="G30" s="491"/>
-      <c r="H30" s="491"/>
-      <c r="I30" s="491"/>
-      <c r="J30" s="491"/>
-      <c r="K30" s="491"/>
-      <c r="L30" s="491"/>
-      <c r="M30" s="491"/>
-      <c r="N30" s="476"/>
-    </row>
-    <row r="31" spans="1:14">
+      <c r="B30" s="494"/>
+      <c r="C30" s="494"/>
+      <c r="D30" s="494"/>
+      <c r="E30" s="494"/>
+      <c r="F30" s="494"/>
+      <c r="G30" s="494"/>
+      <c r="H30" s="494"/>
+      <c r="I30" s="494"/>
+      <c r="J30" s="494"/>
+      <c r="K30" s="494"/>
+      <c r="L30" s="494"/>
+      <c r="M30" s="494"/>
+      <c r="N30" s="452"/>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" s="229"/>
-      <c r="B31" s="492" t="s">
+      <c r="B31" s="491" t="s">
         <v>111</v>
       </c>
-      <c r="C31" s="493"/>
-      <c r="D31" s="494"/>
-      <c r="E31" s="492" t="s">
+      <c r="C31" s="492"/>
+      <c r="D31" s="493"/>
+      <c r="E31" s="491" t="s">
         <v>109</v>
       </c>
-      <c r="F31" s="493"/>
-      <c r="G31" s="494"/>
-      <c r="H31" s="492" t="s">
+      <c r="F31" s="492"/>
+      <c r="G31" s="493"/>
+      <c r="H31" s="491" t="s">
         <v>110</v>
       </c>
-      <c r="I31" s="493"/>
-      <c r="J31" s="494"/>
-      <c r="K31" s="492" t="s">
+      <c r="I31" s="492"/>
+      <c r="J31" s="493"/>
+      <c r="K31" s="491" t="s">
         <v>75</v>
       </c>
-      <c r="L31" s="493"/>
-      <c r="M31" s="494"/>
+      <c r="L31" s="492"/>
+      <c r="M31" s="493"/>
       <c r="N31" s="246"/>
     </row>
-    <row r="32" spans="1:14" ht="15">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" s="230" t="s">
         <v>76</v>
       </c>
@@ -32148,7 +32266,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="33" spans="1:14" ht="15">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" s="231" t="s">
         <v>79</v>
       </c>
@@ -32192,7 +32310,7 @@
         <v>-0.10058679002726996</v>
       </c>
     </row>
-    <row r="34" spans="1:14" ht="15">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" s="232" t="s">
         <v>81</v>
       </c>
@@ -32236,7 +32354,7 @@
         <v>-0.32001589401318498</v>
       </c>
     </row>
-    <row r="35" spans="1:14" ht="15">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35" s="234" t="s">
         <v>83</v>
       </c>
@@ -32280,7 +32398,7 @@
         <v>0.11743877238132332</v>
       </c>
     </row>
-    <row r="36" spans="1:14" ht="15">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36" s="234" t="s">
         <v>84</v>
       </c>
@@ -32324,7 +32442,7 @@
         <v>0.11743877238132332</v>
       </c>
     </row>
-    <row r="37" spans="1:14" ht="15">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37" s="235" t="s">
         <v>86</v>
       </c>
@@ -32368,7 +32486,7 @@
         <v>-4.5718099286610456E-2</v>
       </c>
     </row>
-    <row r="38" spans="1:14" ht="15">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38" s="236" t="s">
         <v>87</v>
       </c>
@@ -32412,7 +32530,7 @@
         <v>-0.11251612892623995</v>
       </c>
     </row>
-    <row r="39" spans="1:14" ht="15">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39" s="236" t="s">
         <v>88</v>
       </c>
@@ -32456,7 +32574,7 @@
         <v>-0.11251612892623995</v>
       </c>
     </row>
-    <row r="40" spans="1:14" ht="15.75" thickBot="1">
+    <row r="40" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="237" t="s">
         <v>89</v>
       </c>
@@ -32502,6 +32620,11 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A30:N30"/>
+    <mergeCell ref="B31:D31"/>
+    <mergeCell ref="E31:G31"/>
+    <mergeCell ref="H31:J31"/>
+    <mergeCell ref="K31:M31"/>
     <mergeCell ref="B17:D17"/>
     <mergeCell ref="E17:G17"/>
     <mergeCell ref="H17:J17"/>
@@ -32512,11 +32635,6 @@
     <mergeCell ref="H2:J2"/>
     <mergeCell ref="K2:M2"/>
     <mergeCell ref="A16:N16"/>
-    <mergeCell ref="A30:N30"/>
-    <mergeCell ref="B31:D31"/>
-    <mergeCell ref="E31:G31"/>
-    <mergeCell ref="H31:J31"/>
-    <mergeCell ref="K31:M31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
corrigiendo las sumas de los new sizes equisdelol
</commit_message>
<xml_diff>
--- a/GSD/baskets_new_sizes/basketGSD_hypflux_NEW_SIZES.xlsx
+++ b/GSD/baskets_new_sizes/basketGSD_hypflux_NEW_SIZES.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\huck4481\Documents\GitHub\La_Jara\GSD\baskets_new_sizes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD825A68-1722-43DB-ACBE-C4C8A9F34046}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{396DC27F-0574-40FF-BE74-22283B9EBD3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-25320" yWindow="195" windowWidth="25440" windowHeight="15390" activeTab="1" xr2:uid="{FF2C68C4-0230-4397-BD30-01ABAA0FCBBF}"/>
   </bookViews>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="703" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="703" uniqueCount="112">
   <si>
     <t>Size</t>
   </si>
@@ -345,9 +345,6 @@
   </si>
   <si>
     <t>SPRING 2023 WEIGHTS</t>
-  </si>
-  <si>
-    <t>c</t>
   </si>
   <si>
     <t>SPRING 2023 - NORMALIZE USING CLOSED BASKET WEIGHTS</t>
@@ -1278,7 +1275,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="499">
+  <cellXfs count="500">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2614,6 +2611,105 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="31" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="31" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="31" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="31" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="31" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="31" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="29" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="29" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="29" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="29" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="29" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="29" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="30" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="30" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="30" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2632,108 +2728,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="31" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="31" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="31" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="30" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="30" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="30" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="29" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="29" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="29" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="29" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="29" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="29" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="36" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="36" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="36" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="36" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="36" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="36" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="31" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="31" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="31" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="38" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="38" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="38" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="38" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="38" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="38" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="30" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2752,6 +2749,9 @@
     <xf numFmtId="0" fontId="0" fillId="33" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2761,7 +2761,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="41" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -3790,7 +3790,7 @@
                   <c:v>7.529399999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8.8132999999999999</c:v>
+                  <c:v>5.7776999999999994</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>7.0016999999999996</c:v>
@@ -5747,7 +5747,7 @@
                   <c:v>-0.37669547662608038</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.86255060728744948</c:v>
+                  <c:v>1.1575910931174089</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>3.0456556588650203</c:v>
@@ -5917,7 +5917,7 @@
                   <c:v>0.17051823518474263</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.28782408405478088</c:v>
+                  <c:v>0.6322580645161292</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>-5.5586500421326221E-2</c:v>
@@ -11055,7 +11055,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{695C6E5A-89DB-4EF6-9D1B-F4A1EC0E0EDD}">
   <dimension ref="B1:AN158"/>
   <sheetViews>
-    <sheetView topLeftCell="U1" zoomScale="76" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A33" zoomScale="76" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="AA18" sqref="AA18:AI29"/>
     </sheetView>
   </sheetViews>
@@ -11078,22 +11078,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:40" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="AG1" s="455" t="s">
+      <c r="AG1" s="473" t="s">
         <v>56</v>
       </c>
-      <c r="AH1" s="455" t="s">
+      <c r="AH1" s="473" t="s">
         <v>57</v>
       </c>
-      <c r="AI1" s="455" t="s">
+      <c r="AI1" s="473" t="s">
         <v>52</v>
       </c>
-      <c r="AJ1" s="455" t="s">
+      <c r="AJ1" s="473" t="s">
         <v>56</v>
       </c>
-      <c r="AK1" s="449" t="s">
+      <c r="AK1" s="482" t="s">
         <v>57</v>
       </c>
-      <c r="AL1" s="449" t="s">
+      <c r="AL1" s="482" t="s">
         <v>52</v>
       </c>
     </row>
@@ -11170,23 +11170,23 @@
       <c r="Y2" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="AB2" s="452" t="s">
+      <c r="AB2" s="485" t="s">
         <v>25</v>
       </c>
-      <c r="AC2" s="453"/>
-      <c r="AD2" s="456" t="s">
+      <c r="AC2" s="486"/>
+      <c r="AD2" s="480" t="s">
         <v>58</v>
       </c>
-      <c r="AE2" s="456"/>
+      <c r="AE2" s="480"/>
       <c r="AF2" s="97" t="s">
-        <v>104</v>
-      </c>
-      <c r="AG2" s="457"/>
-      <c r="AH2" s="455"/>
-      <c r="AI2" s="455"/>
-      <c r="AJ2" s="455"/>
-      <c r="AK2" s="449"/>
-      <c r="AL2" s="449"/>
+        <v>103</v>
+      </c>
+      <c r="AG2" s="488"/>
+      <c r="AH2" s="473"/>
+      <c r="AI2" s="473"/>
+      <c r="AJ2" s="473"/>
+      <c r="AK2" s="482"/>
+      <c r="AL2" s="482"/>
     </row>
     <row r="3" spans="2:40" x14ac:dyDescent="0.25">
       <c r="B3" s="14">
@@ -11275,7 +11275,7 @@
         <v>60</v>
       </c>
       <c r="AF3" s="57" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="AG3" s="427" t="s">
         <v>60</v>
@@ -12821,22 +12821,22 @@
       <c r="Y16" s="41">
         <v>1.1583636475738333</v>
       </c>
-      <c r="AG16" s="455" t="s">
+      <c r="AG16" s="473" t="s">
         <v>56</v>
       </c>
-      <c r="AH16" s="455" t="s">
+      <c r="AH16" s="473" t="s">
         <v>57</v>
       </c>
-      <c r="AI16" s="455" t="s">
+      <c r="AI16" s="473" t="s">
         <v>52</v>
       </c>
-      <c r="AJ16" s="455" t="s">
+      <c r="AJ16" s="473" t="s">
         <v>56</v>
       </c>
-      <c r="AK16" s="449" t="s">
+      <c r="AK16" s="482" t="s">
         <v>57</v>
       </c>
-      <c r="AL16" s="449" t="s">
+      <c r="AL16" s="482" t="s">
         <v>52</v>
       </c>
       <c r="AN16" s="445"/>
@@ -12914,23 +12914,23 @@
       <c r="Y17" s="41">
         <v>1.2284974412725813</v>
       </c>
-      <c r="AB17" s="452" t="s">
+      <c r="AB17" s="485" t="s">
         <v>40</v>
       </c>
-      <c r="AC17" s="454"/>
-      <c r="AD17" s="456" t="s">
+      <c r="AC17" s="487"/>
+      <c r="AD17" s="480" t="s">
         <v>58</v>
       </c>
-      <c r="AE17" s="456"/>
+      <c r="AE17" s="480"/>
       <c r="AF17" s="261" t="s">
-        <v>104</v>
-      </c>
-      <c r="AG17" s="455"/>
-      <c r="AH17" s="455"/>
-      <c r="AI17" s="455"/>
-      <c r="AJ17" s="455"/>
-      <c r="AK17" s="449"/>
-      <c r="AL17" s="449"/>
+        <v>103</v>
+      </c>
+      <c r="AG17" s="473"/>
+      <c r="AH17" s="473"/>
+      <c r="AI17" s="473"/>
+      <c r="AJ17" s="473"/>
+      <c r="AK17" s="482"/>
+      <c r="AL17" s="482"/>
       <c r="AN17" s="445"/>
     </row>
     <row r="18" spans="2:40" x14ac:dyDescent="0.25">
@@ -13020,7 +13020,7 @@
         <v>60</v>
       </c>
       <c r="AF18" s="419" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="AG18" s="57" t="s">
         <v>60</v>
@@ -14595,14 +14595,14 @@
       <c r="Y32" s="41">
         <v>6.9971946482520506</v>
       </c>
-      <c r="AA32" s="450" t="s">
+      <c r="AA32" s="483" t="s">
         <v>25</v>
       </c>
-      <c r="AB32" s="450"/>
-      <c r="AC32" s="451" t="s">
+      <c r="AB32" s="483"/>
+      <c r="AC32" s="484" t="s">
         <v>40</v>
       </c>
-      <c r="AD32" s="451"/>
+      <c r="AD32" s="484"/>
       <c r="AI32" s="230" t="s">
         <v>76</v>
       </c>
@@ -16135,45 +16135,45 @@
       </c>
     </row>
     <row r="51" spans="2:40" x14ac:dyDescent="0.25">
-      <c r="AA51" s="456" t="s">
-        <v>103</v>
-      </c>
-      <c r="AB51" s="456"/>
-      <c r="AC51" s="456"/>
-      <c r="AD51" s="456"/>
-      <c r="AE51" s="456"/>
-      <c r="AF51" s="456"/>
-      <c r="AG51" s="456"/>
-      <c r="AH51" s="456"/>
-      <c r="AI51" s="456"/>
-      <c r="AJ51" s="456"/>
-      <c r="AK51" s="456"/>
-      <c r="AL51" s="456"/>
-      <c r="AM51" s="456"/>
-      <c r="AN51" s="456"/>
+      <c r="AA51" s="480" t="s">
+        <v>102</v>
+      </c>
+      <c r="AB51" s="480"/>
+      <c r="AC51" s="480"/>
+      <c r="AD51" s="480"/>
+      <c r="AE51" s="480"/>
+      <c r="AF51" s="480"/>
+      <c r="AG51" s="480"/>
+      <c r="AH51" s="480"/>
+      <c r="AI51" s="480"/>
+      <c r="AJ51" s="480"/>
+      <c r="AK51" s="480"/>
+      <c r="AL51" s="480"/>
+      <c r="AM51" s="480"/>
+      <c r="AN51" s="480"/>
     </row>
     <row r="52" spans="2:40" x14ac:dyDescent="0.25">
       <c r="AA52" s="56"/>
-      <c r="AB52" s="467" t="s">
+      <c r="AB52" s="481" t="s">
         <v>72</v>
       </c>
-      <c r="AC52" s="467"/>
-      <c r="AD52" s="467"/>
-      <c r="AE52" s="467" t="s">
+      <c r="AC52" s="481"/>
+      <c r="AD52" s="481"/>
+      <c r="AE52" s="481" t="s">
         <v>73</v>
       </c>
-      <c r="AF52" s="467"/>
-      <c r="AG52" s="467"/>
-      <c r="AH52" s="467" t="s">
+      <c r="AF52" s="481"/>
+      <c r="AG52" s="481"/>
+      <c r="AH52" s="481" t="s">
         <v>74</v>
       </c>
-      <c r="AI52" s="467"/>
-      <c r="AJ52" s="467"/>
-      <c r="AK52" s="467" t="s">
+      <c r="AI52" s="481"/>
+      <c r="AJ52" s="481"/>
+      <c r="AK52" s="481" t="s">
         <v>75</v>
       </c>
-      <c r="AL52" s="467"/>
-      <c r="AM52" s="467"/>
+      <c r="AL52" s="481"/>
+      <c r="AM52" s="481"/>
       <c r="AN52" s="56"/>
     </row>
     <row r="53" spans="2:40" x14ac:dyDescent="0.25">
@@ -16184,37 +16184,37 @@
         <v>76</v>
       </c>
       <c r="AB53" s="392" t="s">
+        <v>100</v>
+      </c>
+      <c r="AC53" s="57" t="s">
         <v>101</v>
-      </c>
-      <c r="AC53" s="57" t="s">
-        <v>102</v>
       </c>
       <c r="AD53" s="57" t="s">
         <v>78</v>
       </c>
       <c r="AE53" s="392" t="s">
+        <v>100</v>
+      </c>
+      <c r="AF53" s="57" t="s">
         <v>101</v>
-      </c>
-      <c r="AF53" s="57" t="s">
-        <v>102</v>
       </c>
       <c r="AG53" s="57" t="s">
         <v>78</v>
       </c>
       <c r="AH53" s="392" t="s">
+        <v>100</v>
+      </c>
+      <c r="AI53" s="57" t="s">
         <v>101</v>
-      </c>
-      <c r="AI53" s="57" t="s">
-        <v>102</v>
       </c>
       <c r="AJ53" s="57" t="s">
         <v>78</v>
       </c>
       <c r="AK53" s="392" t="s">
+        <v>100</v>
+      </c>
+      <c r="AL53" s="57" t="s">
         <v>101</v>
-      </c>
-      <c r="AL53" s="57" t="s">
-        <v>102</v>
       </c>
       <c r="AM53" s="57" t="s">
         <v>78</v>
@@ -16268,34 +16268,34 @@
       </c>
     </row>
     <row r="55" spans="2:40" x14ac:dyDescent="0.25">
-      <c r="B55" s="464" t="s">
+      <c r="B55" s="477" t="s">
         <v>1</v>
       </c>
-      <c r="C55" s="465"/>
-      <c r="D55" s="465"/>
-      <c r="E55" s="465"/>
-      <c r="F55" s="466"/>
-      <c r="G55" s="464" t="s">
+      <c r="C55" s="478"/>
+      <c r="D55" s="478"/>
+      <c r="E55" s="478"/>
+      <c r="F55" s="479"/>
+      <c r="G55" s="477" t="s">
         <v>2</v>
       </c>
-      <c r="H55" s="465"/>
-      <c r="I55" s="465"/>
-      <c r="J55" s="465"/>
-      <c r="K55" s="466"/>
-      <c r="L55" s="464" t="s">
+      <c r="H55" s="478"/>
+      <c r="I55" s="478"/>
+      <c r="J55" s="478"/>
+      <c r="K55" s="479"/>
+      <c r="L55" s="477" t="s">
         <v>3</v>
       </c>
-      <c r="M55" s="465"/>
-      <c r="N55" s="465"/>
-      <c r="O55" s="465"/>
-      <c r="P55" s="466"/>
-      <c r="Q55" s="464" t="s">
+      <c r="M55" s="478"/>
+      <c r="N55" s="478"/>
+      <c r="O55" s="478"/>
+      <c r="P55" s="479"/>
+      <c r="Q55" s="477" t="s">
         <v>4</v>
       </c>
-      <c r="R55" s="465"/>
-      <c r="S55" s="465"/>
-      <c r="T55" s="465"/>
-      <c r="U55" s="466"/>
+      <c r="R55" s="478"/>
+      <c r="S55" s="478"/>
+      <c r="T55" s="478"/>
+      <c r="U55" s="479"/>
       <c r="AA55" s="218" t="s">
         <v>80</v>
       </c>
@@ -17506,20 +17506,20 @@
     </row>
     <row r="69" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="70" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B70" s="458" t="s">
+      <c r="B70" s="449" t="s">
         <v>5</v>
       </c>
-      <c r="C70" s="459"/>
-      <c r="D70" s="459"/>
-      <c r="E70" s="459"/>
-      <c r="F70" s="460"/>
-      <c r="G70" s="458" t="s">
+      <c r="C70" s="450"/>
+      <c r="D70" s="450"/>
+      <c r="E70" s="450"/>
+      <c r="F70" s="451"/>
+      <c r="G70" s="449" t="s">
         <v>6</v>
       </c>
-      <c r="H70" s="459"/>
-      <c r="I70" s="459"/>
-      <c r="J70" s="459"/>
-      <c r="K70" s="460"/>
+      <c r="H70" s="450"/>
+      <c r="I70" s="450"/>
+      <c r="J70" s="450"/>
+      <c r="K70" s="451"/>
     </row>
     <row r="71" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B71" s="150" t="s">
@@ -17927,20 +17927,20 @@
     </row>
     <row r="84" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="85" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B85" s="461" t="s">
+      <c r="B85" s="474" t="s">
         <v>7</v>
       </c>
-      <c r="C85" s="462"/>
-      <c r="D85" s="462"/>
-      <c r="E85" s="462"/>
-      <c r="F85" s="463"/>
-      <c r="G85" s="461" t="s">
+      <c r="C85" s="475"/>
+      <c r="D85" s="475"/>
+      <c r="E85" s="475"/>
+      <c r="F85" s="476"/>
+      <c r="G85" s="474" t="s">
         <v>8</v>
       </c>
-      <c r="H85" s="462"/>
-      <c r="I85" s="462"/>
-      <c r="J85" s="462"/>
-      <c r="K85" s="463"/>
+      <c r="H85" s="475"/>
+      <c r="I85" s="475"/>
+      <c r="J85" s="475"/>
+      <c r="K85" s="476"/>
     </row>
     <row r="86" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B86" s="173" t="s">
@@ -18350,34 +18350,34 @@
     </row>
     <row r="99" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="100" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B100" s="468" t="s">
+      <c r="B100" s="461" t="s">
         <v>9</v>
       </c>
-      <c r="C100" s="469"/>
-      <c r="D100" s="469"/>
-      <c r="E100" s="469"/>
-      <c r="F100" s="470"/>
-      <c r="G100" s="468" t="s">
+      <c r="C100" s="462"/>
+      <c r="D100" s="462"/>
+      <c r="E100" s="462"/>
+      <c r="F100" s="463"/>
+      <c r="G100" s="461" t="s">
         <v>10</v>
       </c>
-      <c r="H100" s="469"/>
-      <c r="I100" s="469"/>
-      <c r="J100" s="469"/>
-      <c r="K100" s="470"/>
-      <c r="L100" s="471" t="s">
+      <c r="H100" s="462"/>
+      <c r="I100" s="462"/>
+      <c r="J100" s="462"/>
+      <c r="K100" s="463"/>
+      <c r="L100" s="464" t="s">
         <v>11</v>
       </c>
-      <c r="M100" s="472"/>
-      <c r="N100" s="472"/>
-      <c r="O100" s="472"/>
-      <c r="P100" s="473"/>
-      <c r="Q100" s="468" t="s">
+      <c r="M100" s="465"/>
+      <c r="N100" s="465"/>
+      <c r="O100" s="465"/>
+      <c r="P100" s="466"/>
+      <c r="Q100" s="461" t="s">
         <v>12</v>
       </c>
-      <c r="R100" s="469"/>
-      <c r="S100" s="469"/>
-      <c r="T100" s="469"/>
-      <c r="U100" s="470"/>
+      <c r="R100" s="462"/>
+      <c r="S100" s="462"/>
+      <c r="T100" s="462"/>
+      <c r="U100" s="463"/>
     </row>
     <row r="101" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B101" s="183" t="s">
@@ -19165,34 +19165,34 @@
     </row>
     <row r="114" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="115" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B115" s="474" t="s">
+      <c r="B115" s="467" t="s">
         <v>13</v>
       </c>
-      <c r="C115" s="475"/>
-      <c r="D115" s="475"/>
-      <c r="E115" s="475"/>
-      <c r="F115" s="476"/>
-      <c r="G115" s="474" t="s">
+      <c r="C115" s="468"/>
+      <c r="D115" s="468"/>
+      <c r="E115" s="468"/>
+      <c r="F115" s="469"/>
+      <c r="G115" s="467" t="s">
         <v>14</v>
       </c>
-      <c r="H115" s="475"/>
-      <c r="I115" s="475"/>
-      <c r="J115" s="475"/>
-      <c r="K115" s="476"/>
-      <c r="L115" s="477" t="s">
+      <c r="H115" s="468"/>
+      <c r="I115" s="468"/>
+      <c r="J115" s="468"/>
+      <c r="K115" s="469"/>
+      <c r="L115" s="470" t="s">
         <v>15</v>
       </c>
-      <c r="M115" s="478"/>
-      <c r="N115" s="478"/>
-      <c r="O115" s="478"/>
-      <c r="P115" s="479"/>
-      <c r="Q115" s="474" t="s">
+      <c r="M115" s="471"/>
+      <c r="N115" s="471"/>
+      <c r="O115" s="471"/>
+      <c r="P115" s="472"/>
+      <c r="Q115" s="467" t="s">
         <v>16</v>
       </c>
-      <c r="R115" s="475"/>
-      <c r="S115" s="475"/>
-      <c r="T115" s="475"/>
-      <c r="U115" s="476"/>
+      <c r="R115" s="468"/>
+      <c r="S115" s="468"/>
+      <c r="T115" s="468"/>
+      <c r="U115" s="469"/>
     </row>
     <row r="116" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B116" s="193" t="s">
@@ -19980,34 +19980,34 @@
     </row>
     <row r="129" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="130" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B130" s="458" t="s">
+      <c r="B130" s="449" t="s">
         <v>17</v>
       </c>
-      <c r="C130" s="459"/>
-      <c r="D130" s="459"/>
-      <c r="E130" s="459"/>
-      <c r="F130" s="460"/>
-      <c r="G130" s="458" t="s">
+      <c r="C130" s="450"/>
+      <c r="D130" s="450"/>
+      <c r="E130" s="450"/>
+      <c r="F130" s="451"/>
+      <c r="G130" s="449" t="s">
         <v>18</v>
       </c>
-      <c r="H130" s="459"/>
-      <c r="I130" s="459"/>
-      <c r="J130" s="459"/>
-      <c r="K130" s="460"/>
-      <c r="L130" s="480" t="s">
+      <c r="H130" s="450"/>
+      <c r="I130" s="450"/>
+      <c r="J130" s="450"/>
+      <c r="K130" s="451"/>
+      <c r="L130" s="452" t="s">
         <v>19</v>
       </c>
-      <c r="M130" s="481"/>
-      <c r="N130" s="481"/>
-      <c r="O130" s="481"/>
-      <c r="P130" s="482"/>
-      <c r="Q130" s="458" t="s">
+      <c r="M130" s="453"/>
+      <c r="N130" s="453"/>
+      <c r="O130" s="453"/>
+      <c r="P130" s="454"/>
+      <c r="Q130" s="449" t="s">
         <v>20</v>
       </c>
-      <c r="R130" s="459"/>
-      <c r="S130" s="459"/>
-      <c r="T130" s="459"/>
-      <c r="U130" s="460"/>
+      <c r="R130" s="450"/>
+      <c r="S130" s="450"/>
+      <c r="T130" s="450"/>
+      <c r="U130" s="451"/>
     </row>
     <row r="131" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B131" s="150" t="s">
@@ -20795,27 +20795,27 @@
     </row>
     <row r="144" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="145" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B145" s="483" t="s">
+      <c r="B145" s="455" t="s">
         <v>21</v>
       </c>
-      <c r="C145" s="484"/>
-      <c r="D145" s="484"/>
-      <c r="E145" s="484"/>
-      <c r="F145" s="485"/>
-      <c r="G145" s="483" t="s">
+      <c r="C145" s="456"/>
+      <c r="D145" s="456"/>
+      <c r="E145" s="456"/>
+      <c r="F145" s="457"/>
+      <c r="G145" s="455" t="s">
         <v>22</v>
       </c>
-      <c r="H145" s="484"/>
-      <c r="I145" s="484"/>
-      <c r="J145" s="484"/>
-      <c r="K145" s="485"/>
-      <c r="L145" s="486" t="s">
+      <c r="H145" s="456"/>
+      <c r="I145" s="456"/>
+      <c r="J145" s="456"/>
+      <c r="K145" s="457"/>
+      <c r="L145" s="458" t="s">
         <v>23</v>
       </c>
-      <c r="M145" s="487"/>
-      <c r="N145" s="487"/>
-      <c r="O145" s="487"/>
-      <c r="P145" s="488"/>
+      <c r="M145" s="459"/>
+      <c r="N145" s="459"/>
+      <c r="O145" s="459"/>
+      <c r="P145" s="460"/>
     </row>
     <row r="146" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B146" s="203" t="s">
@@ -21414,36 +21414,6 @@
     </row>
   </sheetData>
   <mergeCells count="46">
-    <mergeCell ref="B130:F130"/>
-    <mergeCell ref="G130:K130"/>
-    <mergeCell ref="L130:P130"/>
-    <mergeCell ref="Q130:U130"/>
-    <mergeCell ref="B145:F145"/>
-    <mergeCell ref="G145:K145"/>
-    <mergeCell ref="L145:P145"/>
-    <mergeCell ref="B100:F100"/>
-    <mergeCell ref="G100:K100"/>
-    <mergeCell ref="L100:P100"/>
-    <mergeCell ref="Q100:U100"/>
-    <mergeCell ref="B115:F115"/>
-    <mergeCell ref="G115:K115"/>
-    <mergeCell ref="L115:P115"/>
-    <mergeCell ref="Q115:U115"/>
-    <mergeCell ref="AH16:AH17"/>
-    <mergeCell ref="AI16:AI17"/>
-    <mergeCell ref="B70:F70"/>
-    <mergeCell ref="G70:K70"/>
-    <mergeCell ref="B85:F85"/>
-    <mergeCell ref="G85:K85"/>
-    <mergeCell ref="B55:F55"/>
-    <mergeCell ref="G55:K55"/>
-    <mergeCell ref="L55:P55"/>
-    <mergeCell ref="Q55:U55"/>
-    <mergeCell ref="AA51:AN51"/>
-    <mergeCell ref="AB52:AD52"/>
-    <mergeCell ref="AE52:AG52"/>
-    <mergeCell ref="AH52:AJ52"/>
-    <mergeCell ref="AK52:AM52"/>
     <mergeCell ref="AL1:AL2"/>
     <mergeCell ref="AL16:AL17"/>
     <mergeCell ref="AK16:AK17"/>
@@ -21460,6 +21430,36 @@
     <mergeCell ref="AH1:AH2"/>
     <mergeCell ref="AI1:AI2"/>
     <mergeCell ref="AG16:AG17"/>
+    <mergeCell ref="AH16:AH17"/>
+    <mergeCell ref="AI16:AI17"/>
+    <mergeCell ref="B70:F70"/>
+    <mergeCell ref="G70:K70"/>
+    <mergeCell ref="B85:F85"/>
+    <mergeCell ref="G85:K85"/>
+    <mergeCell ref="B55:F55"/>
+    <mergeCell ref="G55:K55"/>
+    <mergeCell ref="L55:P55"/>
+    <mergeCell ref="Q55:U55"/>
+    <mergeCell ref="AA51:AN51"/>
+    <mergeCell ref="AB52:AD52"/>
+    <mergeCell ref="AE52:AG52"/>
+    <mergeCell ref="AH52:AJ52"/>
+    <mergeCell ref="AK52:AM52"/>
+    <mergeCell ref="B100:F100"/>
+    <mergeCell ref="G100:K100"/>
+    <mergeCell ref="L100:P100"/>
+    <mergeCell ref="Q100:U100"/>
+    <mergeCell ref="B115:F115"/>
+    <mergeCell ref="G115:K115"/>
+    <mergeCell ref="L115:P115"/>
+    <mergeCell ref="Q115:U115"/>
+    <mergeCell ref="B130:F130"/>
+    <mergeCell ref="G130:K130"/>
+    <mergeCell ref="L130:P130"/>
+    <mergeCell ref="Q130:U130"/>
+    <mergeCell ref="B145:F145"/>
+    <mergeCell ref="G145:K145"/>
+    <mergeCell ref="L145:P145"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -21470,8 +21470,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F64C6BB9-54B5-42EC-B225-E298A2E667FE}">
   <dimension ref="B1:BA158"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="W1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AD17" sqref="AD17:AI17"/>
+    <sheetView tabSelected="1" topLeftCell="P1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="AN49" sqref="AN49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21494,22 +21494,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:53" x14ac:dyDescent="0.25">
-      <c r="AG1" s="455" t="s">
+      <c r="AG1" s="473" t="s">
         <v>56</v>
       </c>
-      <c r="AH1" s="455" t="s">
+      <c r="AH1" s="473" t="s">
         <v>57</v>
       </c>
-      <c r="AI1" s="455" t="s">
+      <c r="AI1" s="473" t="s">
         <v>52</v>
       </c>
-      <c r="AJ1" s="455" t="s">
+      <c r="AJ1" s="473" t="s">
         <v>56</v>
       </c>
-      <c r="AK1" s="455" t="s">
+      <c r="AK1" s="473" t="s">
         <v>57</v>
       </c>
-      <c r="AL1" s="455" t="s">
+      <c r="AL1" s="473" t="s">
         <v>52</v>
       </c>
     </row>
@@ -21586,23 +21586,23 @@
       <c r="Y2" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="AB2" s="452" t="s">
+      <c r="AB2" s="485" t="s">
         <v>25</v>
       </c>
-      <c r="AC2" s="453"/>
-      <c r="AD2" s="456" t="s">
+      <c r="AC2" s="486"/>
+      <c r="AD2" s="480" t="s">
         <v>58</v>
       </c>
-      <c r="AE2" s="456"/>
+      <c r="AE2" s="480"/>
       <c r="AF2" s="429" t="s">
-        <v>104</v>
-      </c>
-      <c r="AG2" s="455"/>
-      <c r="AH2" s="455"/>
-      <c r="AI2" s="455"/>
-      <c r="AJ2" s="455"/>
-      <c r="AK2" s="455"/>
-      <c r="AL2" s="455"/>
+        <v>103</v>
+      </c>
+      <c r="AG2" s="473"/>
+      <c r="AH2" s="473"/>
+      <c r="AI2" s="473"/>
+      <c r="AJ2" s="473"/>
+      <c r="AK2" s="473"/>
+      <c r="AL2" s="473"/>
     </row>
     <row r="3" spans="2:53" x14ac:dyDescent="0.25">
       <c r="B3" s="14">
@@ -21689,7 +21689,7 @@
         <v>60</v>
       </c>
       <c r="AF3" s="57" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="AG3" s="57" t="s">
         <v>60</v>
@@ -21710,7 +21710,7 @@
         <v>55</v>
       </c>
       <c r="AN3" s="448" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="4" spans="2:53" x14ac:dyDescent="0.25">
@@ -21793,7 +21793,7 @@
       <c r="AC4" s="388">
         <v>-0.10058679002726996</v>
       </c>
-      <c r="AD4" s="216">
+      <c r="AD4" s="262">
         <f>SUM(C57:C59)</f>
         <v>1.5851</v>
       </c>
@@ -21921,13 +21921,13 @@
       <c r="AC5" s="388">
         <v>-0.10058679002726996</v>
       </c>
-      <c r="AD5" s="216">
-        <f>SUM(H57:H59)</f>
-        <v>0.98799999999999999</v>
-      </c>
-      <c r="AE5" s="216">
-        <f>SUM(H60:H63)</f>
-        <v>8.8132999999999999</v>
+      <c r="AD5" s="262">
+        <f>SUM(R57:R59)</f>
+        <v>0.69650000000000001</v>
+      </c>
+      <c r="AE5" s="262">
+        <f>SUM(R60:R63)</f>
+        <v>5.7776999999999994</v>
       </c>
       <c r="AF5" s="218">
         <v>5.9919999999999991</v>
@@ -21957,11 +21957,11 @@
       </c>
       <c r="AM5" s="447">
         <f t="shared" ref="AM5:AM28" si="3">AN5-AG5</f>
-        <v>12.790115347721821</v>
+        <v>9.4630153477218215</v>
       </c>
       <c r="AN5" s="447">
         <f t="shared" ref="AN5:AN28" si="4">SUM(AD5:AE5,AH5:AI5)</f>
-        <v>14.291707673860909</v>
+        <v>10.964607673860909</v>
       </c>
     </row>
     <row r="6" spans="2:53" x14ac:dyDescent="0.25">
@@ -22048,7 +22048,7 @@
         <f>SUM(C72:C74)</f>
         <v>1.5595000000000001</v>
       </c>
-      <c r="AE6" s="216">
+      <c r="AE6" s="262">
         <f>SUM(C75:C78)</f>
         <v>7.0016999999999996</v>
       </c>
@@ -22290,7 +22290,7 @@
       <c r="AC8" s="390">
         <v>0.11743877238132332</v>
       </c>
-      <c r="AD8" s="217">
+      <c r="AD8" s="499">
         <f>SUM(C102:C104)</f>
         <v>6.3570000000000002</v>
       </c>
@@ -22659,7 +22659,7 @@
       <c r="AC11" s="389">
         <v>-0.11251612892623995</v>
       </c>
-      <c r="AD11" s="217">
+      <c r="AD11" s="499">
         <f>SUM(C132:C134)</f>
         <v>3.1258999999999997</v>
       </c>
@@ -22905,7 +22905,7 @@
       <c r="AC13" s="391">
         <v>-4.9570413884485784E-2</v>
       </c>
-      <c r="AD13" s="217">
+      <c r="AD13" s="499">
         <f>SUM(C147:C149)</f>
         <v>0.41239999999999999</v>
       </c>
@@ -23142,22 +23142,22 @@
       <c r="Y15" s="380">
         <v>1.0235026535253984</v>
       </c>
-      <c r="AG15" s="455" t="s">
+      <c r="AG15" s="473" t="s">
         <v>56</v>
       </c>
-      <c r="AH15" s="455" t="s">
+      <c r="AH15" s="473" t="s">
         <v>57</v>
       </c>
-      <c r="AI15" s="455" t="s">
+      <c r="AI15" s="473" t="s">
         <v>52</v>
       </c>
-      <c r="AJ15" s="455" t="s">
+      <c r="AJ15" s="473" t="s">
         <v>56</v>
       </c>
-      <c r="AK15" s="455" t="s">
+      <c r="AK15" s="473" t="s">
         <v>57</v>
       </c>
-      <c r="AL15" s="455" t="s">
+      <c r="AL15" s="473" t="s">
         <v>52</v>
       </c>
       <c r="AM15" s="447"/>
@@ -23234,23 +23234,23 @@
       <c r="Y16" s="380">
         <v>1.0708870356330553</v>
       </c>
-      <c r="AB16" s="452" t="s">
+      <c r="AB16" s="485" t="s">
         <v>40</v>
       </c>
-      <c r="AC16" s="454"/>
-      <c r="AD16" s="456" t="s">
+      <c r="AC16" s="487"/>
+      <c r="AD16" s="480" t="s">
         <v>58</v>
       </c>
-      <c r="AE16" s="456"/>
+      <c r="AE16" s="480"/>
       <c r="AF16" s="429" t="s">
-        <v>104</v>
-      </c>
-      <c r="AG16" s="455"/>
-      <c r="AH16" s="455"/>
-      <c r="AI16" s="455"/>
-      <c r="AJ16" s="455"/>
-      <c r="AK16" s="455"/>
-      <c r="AL16" s="455"/>
+        <v>103</v>
+      </c>
+      <c r="AG16" s="473"/>
+      <c r="AH16" s="473"/>
+      <c r="AI16" s="473"/>
+      <c r="AJ16" s="473"/>
+      <c r="AK16" s="473"/>
+      <c r="AL16" s="473"/>
       <c r="AM16" s="447"/>
       <c r="AN16" s="447"/>
     </row>
@@ -23339,7 +23339,7 @@
         <v>60</v>
       </c>
       <c r="AF17" s="57" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="AG17" s="57" t="s">
         <v>60</v>
@@ -23442,11 +23442,11 @@
       <c r="AC18" s="388">
         <v>-0.10058679002726996</v>
       </c>
-      <c r="AD18" s="216">
+      <c r="AD18" s="262">
         <f>SUM(H57:H59)</f>
         <v>0.98799999999999999</v>
       </c>
-      <c r="AE18" s="216">
+      <c r="AE18" s="262">
         <f>SUM(H60:H63)</f>
         <v>8.8132999999999999</v>
       </c>
@@ -23569,7 +23569,7 @@
         <f>SUM(M57:M59)</f>
         <v>1.8402000000000001</v>
       </c>
-      <c r="AE19" s="216">
+      <c r="AE19" s="262">
         <f>SUM(M60:M63)</f>
         <v>11.34998</v>
       </c>
@@ -23688,11 +23688,11 @@
       <c r="AC20" s="432">
         <v>-0.3029856615539851</v>
       </c>
-      <c r="AD20" s="216">
+      <c r="AD20" s="262">
         <f>SUM(H72:H74)</f>
         <v>6.3091999999999997</v>
       </c>
-      <c r="AE20" s="216">
+      <c r="AE20" s="262">
         <f>SUM(H75:H78)</f>
         <v>6.6124999999999998</v>
       </c>
@@ -23938,7 +23938,7 @@
         <f>SUM(H102:H104)</f>
         <v>3.6301000000000001</v>
       </c>
-      <c r="AE22" s="217">
+      <c r="AE22" s="499">
         <f>SUM(H105:H108)</f>
         <v>8.4920000000000009</v>
       </c>
@@ -24057,7 +24057,7 @@
       <c r="AC23" s="390">
         <v>0.11743877238132332</v>
       </c>
-      <c r="AD23" s="217">
+      <c r="AD23" s="499">
         <f>SUM(M102:M104)</f>
         <v>2.6212</v>
       </c>
@@ -24180,7 +24180,7 @@
       <c r="AC24" s="226">
         <v>-4.5718099286610456E-2</v>
       </c>
-      <c r="AD24" s="217">
+      <c r="AD24" s="499">
         <f>SUM(H117:H119)</f>
         <v>3.512</v>
       </c>
@@ -24426,7 +24426,7 @@
       <c r="AC26" s="389">
         <v>-0.11251612892623995</v>
       </c>
-      <c r="AD26" s="217">
+      <c r="AD26" s="499">
         <f>SUM(H132:H134)</f>
         <v>1.081</v>
       </c>
@@ -24931,14 +24931,14 @@
       <c r="Y31" s="380">
         <v>6.6148597422289619</v>
       </c>
-      <c r="AA31" s="450" t="s">
+      <c r="AA31" s="483" t="s">
         <v>25</v>
       </c>
-      <c r="AB31" s="450"/>
-      <c r="AC31" s="451" t="s">
+      <c r="AB31" s="483"/>
+      <c r="AC31" s="484" t="s">
         <v>40</v>
       </c>
-      <c r="AD31" s="451"/>
+      <c r="AD31" s="484"/>
       <c r="AJ31" s="230" t="s">
         <v>76</v>
       </c>
@@ -25150,11 +25150,11 @@
       </c>
       <c r="AK33" s="240">
         <f t="shared" si="8"/>
-        <v>0.85220000000000007</v>
+        <v>1.1436999999999999</v>
       </c>
       <c r="AL33" s="240">
         <f t="shared" si="9"/>
-        <v>2.5366800000000005</v>
+        <v>5.572280000000001</v>
       </c>
       <c r="AM33" s="240">
         <f t="shared" si="10"/>
@@ -25238,7 +25238,7 @@
       </c>
       <c r="AA34" s="60">
         <f t="shared" si="11"/>
-        <v>8.8132999999999999</v>
+        <v>5.7776999999999994</v>
       </c>
       <c r="AB34" s="86">
         <f t="shared" ref="AB34:AB42" si="13">AG5</f>
@@ -27310,20 +27310,20 @@
     </row>
     <row r="69" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="70" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B70" s="480" t="s">
-        <v>95</v>
-      </c>
-      <c r="C70" s="481"/>
-      <c r="D70" s="481"/>
-      <c r="E70" s="481"/>
-      <c r="F70" s="482"/>
-      <c r="G70" s="480" t="s">
+      <c r="B70" s="452" t="s">
+        <v>5</v>
+      </c>
+      <c r="C70" s="453"/>
+      <c r="D70" s="453"/>
+      <c r="E70" s="453"/>
+      <c r="F70" s="454"/>
+      <c r="G70" s="452" t="s">
         <v>6</v>
       </c>
-      <c r="H70" s="481"/>
-      <c r="I70" s="481"/>
-      <c r="J70" s="481"/>
-      <c r="K70" s="482"/>
+      <c r="H70" s="453"/>
+      <c r="I70" s="453"/>
+      <c r="J70" s="453"/>
+      <c r="K70" s="454"/>
     </row>
     <row r="71" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B71" s="150" t="s">
@@ -28154,34 +28154,34 @@
     </row>
     <row r="99" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="100" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B100" s="471" t="s">
+      <c r="B100" s="464" t="s">
         <v>9</v>
       </c>
-      <c r="C100" s="472"/>
-      <c r="D100" s="472"/>
-      <c r="E100" s="472"/>
-      <c r="F100" s="473"/>
-      <c r="G100" s="471" t="s">
+      <c r="C100" s="465"/>
+      <c r="D100" s="465"/>
+      <c r="E100" s="465"/>
+      <c r="F100" s="466"/>
+      <c r="G100" s="464" t="s">
         <v>10</v>
       </c>
-      <c r="H100" s="472"/>
-      <c r="I100" s="472"/>
-      <c r="J100" s="472"/>
-      <c r="K100" s="473"/>
-      <c r="L100" s="471" t="s">
+      <c r="H100" s="465"/>
+      <c r="I100" s="465"/>
+      <c r="J100" s="465"/>
+      <c r="K100" s="466"/>
+      <c r="L100" s="464" t="s">
         <v>11</v>
       </c>
-      <c r="M100" s="472"/>
-      <c r="N100" s="472"/>
-      <c r="O100" s="472"/>
-      <c r="P100" s="473"/>
-      <c r="Q100" s="471" t="s">
+      <c r="M100" s="465"/>
+      <c r="N100" s="465"/>
+      <c r="O100" s="465"/>
+      <c r="P100" s="466"/>
+      <c r="Q100" s="464" t="s">
         <v>12</v>
       </c>
-      <c r="R100" s="472"/>
-      <c r="S100" s="472"/>
-      <c r="T100" s="472"/>
-      <c r="U100" s="473"/>
+      <c r="R100" s="465"/>
+      <c r="S100" s="465"/>
+      <c r="T100" s="465"/>
+      <c r="U100" s="466"/>
     </row>
     <row r="101" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B101" s="183" t="s">
@@ -28969,34 +28969,34 @@
     </row>
     <row r="114" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="115" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B115" s="474" t="s">
+      <c r="B115" s="467" t="s">
         <v>13</v>
       </c>
-      <c r="C115" s="475"/>
-      <c r="D115" s="475"/>
-      <c r="E115" s="475"/>
-      <c r="F115" s="476"/>
-      <c r="G115" s="477" t="s">
+      <c r="C115" s="468"/>
+      <c r="D115" s="468"/>
+      <c r="E115" s="468"/>
+      <c r="F115" s="469"/>
+      <c r="G115" s="470" t="s">
         <v>14</v>
       </c>
-      <c r="H115" s="478"/>
-      <c r="I115" s="478"/>
-      <c r="J115" s="478"/>
-      <c r="K115" s="479"/>
-      <c r="L115" s="477" t="s">
+      <c r="H115" s="471"/>
+      <c r="I115" s="471"/>
+      <c r="J115" s="471"/>
+      <c r="K115" s="472"/>
+      <c r="L115" s="470" t="s">
         <v>15</v>
       </c>
-      <c r="M115" s="478"/>
-      <c r="N115" s="478"/>
-      <c r="O115" s="478"/>
-      <c r="P115" s="479"/>
-      <c r="Q115" s="477" t="s">
+      <c r="M115" s="471"/>
+      <c r="N115" s="471"/>
+      <c r="O115" s="471"/>
+      <c r="P115" s="472"/>
+      <c r="Q115" s="470" t="s">
         <v>16</v>
       </c>
-      <c r="R115" s="478"/>
-      <c r="S115" s="478"/>
-      <c r="T115" s="478"/>
-      <c r="U115" s="479"/>
+      <c r="R115" s="471"/>
+      <c r="S115" s="471"/>
+      <c r="T115" s="471"/>
+      <c r="U115" s="472"/>
     </row>
     <row r="116" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B116" s="193" t="s">
@@ -29668,34 +29668,34 @@
     </row>
     <row r="129" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="130" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B130" s="480" t="s">
+      <c r="B130" s="452" t="s">
         <v>17</v>
       </c>
-      <c r="C130" s="481"/>
-      <c r="D130" s="481"/>
-      <c r="E130" s="481"/>
-      <c r="F130" s="482"/>
-      <c r="G130" s="480" t="s">
+      <c r="C130" s="453"/>
+      <c r="D130" s="453"/>
+      <c r="E130" s="453"/>
+      <c r="F130" s="454"/>
+      <c r="G130" s="452" t="s">
         <v>18</v>
       </c>
-      <c r="H130" s="481"/>
-      <c r="I130" s="481"/>
-      <c r="J130" s="481"/>
-      <c r="K130" s="482"/>
-      <c r="L130" s="480" t="s">
+      <c r="H130" s="453"/>
+      <c r="I130" s="453"/>
+      <c r="J130" s="453"/>
+      <c r="K130" s="454"/>
+      <c r="L130" s="452" t="s">
         <v>19</v>
       </c>
-      <c r="M130" s="481"/>
-      <c r="N130" s="481"/>
-      <c r="O130" s="481"/>
-      <c r="P130" s="482"/>
-      <c r="Q130" s="480" t="s">
+      <c r="M130" s="453"/>
+      <c r="N130" s="453"/>
+      <c r="O130" s="453"/>
+      <c r="P130" s="454"/>
+      <c r="Q130" s="452" t="s">
         <v>20</v>
       </c>
-      <c r="R130" s="481"/>
-      <c r="S130" s="481"/>
-      <c r="T130" s="481"/>
-      <c r="U130" s="482"/>
+      <c r="R130" s="453"/>
+      <c r="S130" s="453"/>
+      <c r="T130" s="453"/>
+      <c r="U130" s="454"/>
     </row>
     <row r="131" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B131" s="150" t="s">
@@ -30483,27 +30483,27 @@
     </row>
     <row r="144" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="145" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B145" s="486" t="s">
+      <c r="B145" s="458" t="s">
         <v>21</v>
       </c>
-      <c r="C145" s="487"/>
-      <c r="D145" s="487"/>
-      <c r="E145" s="487"/>
-      <c r="F145" s="488"/>
-      <c r="G145" s="486" t="s">
+      <c r="C145" s="459"/>
+      <c r="D145" s="459"/>
+      <c r="E145" s="459"/>
+      <c r="F145" s="460"/>
+      <c r="G145" s="458" t="s">
         <v>22</v>
       </c>
-      <c r="H145" s="487"/>
-      <c r="I145" s="487"/>
-      <c r="J145" s="487"/>
-      <c r="K145" s="488"/>
-      <c r="L145" s="486" t="s">
+      <c r="H145" s="459"/>
+      <c r="I145" s="459"/>
+      <c r="J145" s="459"/>
+      <c r="K145" s="460"/>
+      <c r="L145" s="458" t="s">
         <v>23</v>
       </c>
-      <c r="M145" s="487"/>
-      <c r="N145" s="487"/>
-      <c r="O145" s="487"/>
-      <c r="P145" s="488"/>
+      <c r="M145" s="459"/>
+      <c r="N145" s="459"/>
+      <c r="O145" s="459"/>
+      <c r="P145" s="460"/>
     </row>
     <row r="146" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B146" s="203" t="s">
@@ -31102,17 +31102,24 @@
     </row>
   </sheetData>
   <mergeCells count="41">
-    <mergeCell ref="B145:F145"/>
-    <mergeCell ref="G145:K145"/>
-    <mergeCell ref="L145:P145"/>
-    <mergeCell ref="B115:F115"/>
-    <mergeCell ref="G115:K115"/>
-    <mergeCell ref="L115:P115"/>
-    <mergeCell ref="Q115:U115"/>
-    <mergeCell ref="B130:F130"/>
-    <mergeCell ref="G130:K130"/>
-    <mergeCell ref="L130:P130"/>
-    <mergeCell ref="Q130:U130"/>
+    <mergeCell ref="AL1:AL2"/>
+    <mergeCell ref="AB2:AC2"/>
+    <mergeCell ref="AD2:AE2"/>
+    <mergeCell ref="AG1:AG2"/>
+    <mergeCell ref="AH1:AH2"/>
+    <mergeCell ref="AI1:AI2"/>
+    <mergeCell ref="AJ1:AJ2"/>
+    <mergeCell ref="AK1:AK2"/>
+    <mergeCell ref="AK15:AK16"/>
+    <mergeCell ref="AL15:AL16"/>
+    <mergeCell ref="AB16:AC16"/>
+    <mergeCell ref="AD16:AE16"/>
+    <mergeCell ref="AA31:AB31"/>
+    <mergeCell ref="AC31:AD31"/>
+    <mergeCell ref="AJ15:AJ16"/>
+    <mergeCell ref="AG15:AG16"/>
+    <mergeCell ref="AH15:AH16"/>
+    <mergeCell ref="AI15:AI16"/>
     <mergeCell ref="Q100:U100"/>
     <mergeCell ref="B55:F55"/>
     <mergeCell ref="G55:K55"/>
@@ -31125,24 +31132,17 @@
     <mergeCell ref="B100:F100"/>
     <mergeCell ref="G100:K100"/>
     <mergeCell ref="L100:P100"/>
-    <mergeCell ref="AK15:AK16"/>
-    <mergeCell ref="AL15:AL16"/>
-    <mergeCell ref="AB16:AC16"/>
-    <mergeCell ref="AD16:AE16"/>
-    <mergeCell ref="AA31:AB31"/>
-    <mergeCell ref="AC31:AD31"/>
-    <mergeCell ref="AJ15:AJ16"/>
-    <mergeCell ref="AG15:AG16"/>
-    <mergeCell ref="AH15:AH16"/>
-    <mergeCell ref="AI15:AI16"/>
-    <mergeCell ref="AL1:AL2"/>
-    <mergeCell ref="AB2:AC2"/>
-    <mergeCell ref="AD2:AE2"/>
-    <mergeCell ref="AG1:AG2"/>
-    <mergeCell ref="AH1:AH2"/>
-    <mergeCell ref="AI1:AI2"/>
-    <mergeCell ref="AJ1:AJ2"/>
-    <mergeCell ref="AK1:AK2"/>
+    <mergeCell ref="Q115:U115"/>
+    <mergeCell ref="B130:F130"/>
+    <mergeCell ref="G130:K130"/>
+    <mergeCell ref="L130:P130"/>
+    <mergeCell ref="Q130:U130"/>
+    <mergeCell ref="B145:F145"/>
+    <mergeCell ref="G145:K145"/>
+    <mergeCell ref="L145:P145"/>
+    <mergeCell ref="B115:F115"/>
+    <mergeCell ref="G115:K115"/>
+    <mergeCell ref="L115:P115"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -31173,45 +31173,45 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="456" t="s">
-        <v>96</v>
-      </c>
-      <c r="B1" s="498"/>
-      <c r="C1" s="498"/>
-      <c r="D1" s="498"/>
-      <c r="E1" s="498"/>
-      <c r="F1" s="498"/>
-      <c r="G1" s="498"/>
-      <c r="H1" s="498"/>
-      <c r="I1" s="498"/>
-      <c r="J1" s="498"/>
-      <c r="K1" s="498"/>
-      <c r="L1" s="498"/>
-      <c r="M1" s="498"/>
-      <c r="N1" s="456"/>
+      <c r="A1" s="480" t="s">
+        <v>95</v>
+      </c>
+      <c r="B1" s="495"/>
+      <c r="C1" s="495"/>
+      <c r="D1" s="495"/>
+      <c r="E1" s="495"/>
+      <c r="F1" s="495"/>
+      <c r="G1" s="495"/>
+      <c r="H1" s="495"/>
+      <c r="I1" s="495"/>
+      <c r="J1" s="495"/>
+      <c r="K1" s="495"/>
+      <c r="L1" s="495"/>
+      <c r="M1" s="495"/>
+      <c r="N1" s="480"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="229"/>
-      <c r="B2" s="495" t="s">
-        <v>111</v>
-      </c>
-      <c r="C2" s="496"/>
-      <c r="D2" s="497"/>
-      <c r="E2" s="495" t="s">
-        <v>108</v>
-      </c>
-      <c r="F2" s="496"/>
-      <c r="G2" s="497"/>
-      <c r="H2" s="495" t="s">
+      <c r="B2" s="496" t="s">
         <v>110</v>
       </c>
-      <c r="I2" s="496"/>
-      <c r="J2" s="497"/>
-      <c r="K2" s="495" t="s">
+      <c r="C2" s="497"/>
+      <c r="D2" s="498"/>
+      <c r="E2" s="496" t="s">
+        <v>107</v>
+      </c>
+      <c r="F2" s="497"/>
+      <c r="G2" s="498"/>
+      <c r="H2" s="496" t="s">
+        <v>109</v>
+      </c>
+      <c r="I2" s="497"/>
+      <c r="J2" s="498"/>
+      <c r="K2" s="496" t="s">
         <v>75</v>
       </c>
-      <c r="L2" s="496"/>
-      <c r="M2" s="497"/>
+      <c r="L2" s="497"/>
+      <c r="M2" s="498"/>
       <c r="N2" s="246"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
@@ -31222,7 +31222,7 @@
         <v>77</v>
       </c>
       <c r="C3" s="215" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D3" s="239" t="s">
         <v>78</v>
@@ -31231,7 +31231,7 @@
         <v>77</v>
       </c>
       <c r="F3" s="215" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G3" s="239" t="s">
         <v>78</v>
@@ -31240,7 +31240,7 @@
         <v>77</v>
       </c>
       <c r="I3" s="215" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="J3" s="239" t="s">
         <v>78</v>
@@ -31249,7 +31249,7 @@
         <v>77</v>
       </c>
       <c r="L3" s="215" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="M3" s="239" t="s">
         <v>78</v>
@@ -31831,45 +31831,45 @@
       </c>
     </row>
     <row r="16" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="456" t="s">
-        <v>106</v>
-      </c>
-      <c r="B16" s="498"/>
-      <c r="C16" s="498"/>
-      <c r="D16" s="498"/>
-      <c r="E16" s="498"/>
-      <c r="F16" s="498"/>
-      <c r="G16" s="498"/>
-      <c r="H16" s="498"/>
-      <c r="I16" s="498"/>
-      <c r="J16" s="498"/>
-      <c r="K16" s="498"/>
-      <c r="L16" s="498"/>
-      <c r="M16" s="498"/>
-      <c r="N16" s="456"/>
+      <c r="A16" s="480" t="s">
+        <v>105</v>
+      </c>
+      <c r="B16" s="495"/>
+      <c r="C16" s="495"/>
+      <c r="D16" s="495"/>
+      <c r="E16" s="495"/>
+      <c r="F16" s="495"/>
+      <c r="G16" s="495"/>
+      <c r="H16" s="495"/>
+      <c r="I16" s="495"/>
+      <c r="J16" s="495"/>
+      <c r="K16" s="495"/>
+      <c r="L16" s="495"/>
+      <c r="M16" s="495"/>
+      <c r="N16" s="480"/>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="229"/>
-      <c r="B17" s="495" t="s">
-        <v>111</v>
-      </c>
-      <c r="C17" s="496"/>
-      <c r="D17" s="497"/>
-      <c r="E17" s="495" t="s">
+      <c r="B17" s="496" t="s">
+        <v>110</v>
+      </c>
+      <c r="C17" s="497"/>
+      <c r="D17" s="498"/>
+      <c r="E17" s="496" t="s">
+        <v>108</v>
+      </c>
+      <c r="F17" s="497"/>
+      <c r="G17" s="498"/>
+      <c r="H17" s="496" t="s">
         <v>109</v>
       </c>
-      <c r="F17" s="496"/>
-      <c r="G17" s="497"/>
-      <c r="H17" s="495" t="s">
-        <v>110</v>
-      </c>
-      <c r="I17" s="496"/>
-      <c r="J17" s="497"/>
-      <c r="K17" s="495" t="s">
+      <c r="I17" s="497"/>
+      <c r="J17" s="498"/>
+      <c r="K17" s="496" t="s">
         <v>75</v>
       </c>
-      <c r="L17" s="496"/>
-      <c r="M17" s="497"/>
+      <c r="L17" s="497"/>
+      <c r="M17" s="498"/>
       <c r="N17" s="246"/>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
@@ -31880,7 +31880,7 @@
         <v>77</v>
       </c>
       <c r="C18" s="215" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D18" s="239" t="s">
         <v>78</v>
@@ -31889,7 +31889,7 @@
         <v>77</v>
       </c>
       <c r="F18" s="215" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G18" s="239" t="s">
         <v>78</v>
@@ -31898,7 +31898,7 @@
         <v>77</v>
       </c>
       <c r="I18" s="215" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="J18" s="239" t="s">
         <v>78</v>
@@ -31907,7 +31907,7 @@
         <v>77</v>
       </c>
       <c r="L18" s="215" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="M18" s="239" t="s">
         <v>78</v>
@@ -31974,25 +31974,25 @@
       </c>
       <c r="B20" s="240">
         <f>'Summer Weights'!AK33</f>
-        <v>0.85220000000000007</v>
+        <v>1.1436999999999999</v>
       </c>
       <c r="C20" s="218">
         <v>0.98799999999999999</v>
       </c>
       <c r="D20" s="241">
         <f t="shared" ref="D20:D25" si="4">B20/C20</f>
-        <v>0.86255060728744948</v>
+        <v>1.1575910931174089</v>
       </c>
       <c r="E20" s="244">
         <f>'Summer Weights'!AL33</f>
-        <v>2.5366800000000005</v>
+        <v>5.572280000000001</v>
       </c>
       <c r="F20" s="254">
         <v>8.8132999999999999</v>
       </c>
       <c r="G20" s="241">
         <f t="shared" ref="G20:G27" si="5">E20/F20</f>
-        <v>0.28782408405478088</v>
+        <v>0.6322580645161292</v>
       </c>
       <c r="H20" s="244">
         <f>'Summer Weights'!AM33</f>
@@ -32385,45 +32385,45 @@
       </c>
     </row>
     <row r="30" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="456" t="s">
-        <v>107</v>
-      </c>
-      <c r="B30" s="498"/>
-      <c r="C30" s="498"/>
-      <c r="D30" s="498"/>
-      <c r="E30" s="498"/>
-      <c r="F30" s="498"/>
-      <c r="G30" s="498"/>
-      <c r="H30" s="498"/>
-      <c r="I30" s="498"/>
-      <c r="J30" s="498"/>
-      <c r="K30" s="498"/>
-      <c r="L30" s="498"/>
-      <c r="M30" s="498"/>
-      <c r="N30" s="456"/>
+      <c r="A30" s="480" t="s">
+        <v>106</v>
+      </c>
+      <c r="B30" s="495"/>
+      <c r="C30" s="495"/>
+      <c r="D30" s="495"/>
+      <c r="E30" s="495"/>
+      <c r="F30" s="495"/>
+      <c r="G30" s="495"/>
+      <c r="H30" s="495"/>
+      <c r="I30" s="495"/>
+      <c r="J30" s="495"/>
+      <c r="K30" s="495"/>
+      <c r="L30" s="495"/>
+      <c r="M30" s="495"/>
+      <c r="N30" s="480"/>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" s="229"/>
-      <c r="B31" s="495" t="s">
-        <v>111</v>
-      </c>
-      <c r="C31" s="496"/>
-      <c r="D31" s="497"/>
-      <c r="E31" s="495" t="s">
+      <c r="B31" s="496" t="s">
+        <v>110</v>
+      </c>
+      <c r="C31" s="497"/>
+      <c r="D31" s="498"/>
+      <c r="E31" s="496" t="s">
+        <v>108</v>
+      </c>
+      <c r="F31" s="497"/>
+      <c r="G31" s="498"/>
+      <c r="H31" s="496" t="s">
         <v>109</v>
       </c>
-      <c r="F31" s="496"/>
-      <c r="G31" s="497"/>
-      <c r="H31" s="495" t="s">
-        <v>110</v>
-      </c>
-      <c r="I31" s="496"/>
-      <c r="J31" s="497"/>
-      <c r="K31" s="495" t="s">
+      <c r="I31" s="497"/>
+      <c r="J31" s="498"/>
+      <c r="K31" s="496" t="s">
         <v>75</v>
       </c>
-      <c r="L31" s="496"/>
-      <c r="M31" s="497"/>
+      <c r="L31" s="497"/>
+      <c r="M31" s="498"/>
       <c r="N31" s="246"/>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
@@ -32434,7 +32434,7 @@
         <v>77</v>
       </c>
       <c r="C32" s="215" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D32" s="239" t="s">
         <v>78</v>
@@ -32443,7 +32443,7 @@
         <v>77</v>
       </c>
       <c r="F32" s="215" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G32" s="239" t="s">
         <v>78</v>
@@ -32452,7 +32452,7 @@
         <v>77</v>
       </c>
       <c r="I32" s="215" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="J32" s="239" t="s">
         <v>78</v>
@@ -32461,7 +32461,7 @@
         <v>77</v>
       </c>
       <c r="L32" s="215" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="M32" s="239" t="s">
         <v>78</v>
@@ -32824,11 +32824,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="A30:N30"/>
-    <mergeCell ref="B31:D31"/>
-    <mergeCell ref="E31:G31"/>
-    <mergeCell ref="H31:J31"/>
-    <mergeCell ref="K31:M31"/>
     <mergeCell ref="B17:D17"/>
     <mergeCell ref="E17:G17"/>
     <mergeCell ref="H17:J17"/>
@@ -32839,6 +32834,11 @@
     <mergeCell ref="H2:J2"/>
     <mergeCell ref="K2:M2"/>
     <mergeCell ref="A16:N16"/>
+    <mergeCell ref="A30:N30"/>
+    <mergeCell ref="B31:D31"/>
+    <mergeCell ref="E31:G31"/>
+    <mergeCell ref="H31:J31"/>
+    <mergeCell ref="K31:M31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
updating regressions to test CS 1 mm cutoff
</commit_message>
<xml_diff>
--- a/GSD/baskets_new_sizes/basketGSD_hypflux_NEW_SIZES.xlsx
+++ b/GSD/baskets_new_sizes/basketGSD_hypflux_NEW_SIZES.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nicol\Documents\GitHub\La_Jara\GSD\baskets_new_sizes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\huck4481\Documents\GitHub\La_Jara\GSD\baskets_new_sizes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E888199E-8A9A-4DB1-9938-49CE1A6F0DED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DEB89F6-6C18-41C3-82AB-2BCEE81B9D47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{FF2C68C4-0230-4397-BD30-01ABAA0FCBBF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{FF2C68C4-0230-4397-BD30-01ABAA0FCBBF}"/>
   </bookViews>
   <sheets>
     <sheet name="Spring Weights" sheetId="1" r:id="rId1"/>
@@ -2651,6 +2651,124 @@
     <xf numFmtId="165" fontId="3" fillId="51" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="32" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="40" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="42" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="31" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="31" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="31" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="31" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="31" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="31" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="29" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="29" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="29" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="29" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="29" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="29" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="30" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="30" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="30" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2669,108 +2787,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="31" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="31" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="31" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="30" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="30" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="30" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="29" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="29" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="29" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="29" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="29" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="29" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="36" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="36" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="36" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="36" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="36" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="36" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="31" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="31" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="31" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="38" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="38" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="38" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="38" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="38" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="38" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="30" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2789,6 +2808,9 @@
     <xf numFmtId="0" fontId="0" fillId="33" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2796,28 +2818,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="32" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="40" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="42" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -5683,7 +5683,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="es-AR"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -6809,7 +6809,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="es-AR"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -7088,8 +7088,8 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-0.21779710250835815"/>
-                  <c:y val="-0.44794181190775917"/>
+                  <c:x val="-0.29143362243477056"/>
+                  <c:y val="-4.3052724524628667E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -7252,8 +7252,8 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-0.2184004725627394"/>
-                  <c:y val="-0.20057324246482053"/>
+                  <c:x val="-0.28512532927072243"/>
+                  <c:y val="0.19685854172573691"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -7668,7 +7668,7 @@
                   <c:v>-0.2142122573951242</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-0.12091619396052283</c:v>
+                  <c:v>-0.12091619396052281</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0.19235164956740658</c:v>
@@ -7680,7 +7680,7 @@
                   <c:v>0.30506992688237528</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.73881089123312471</c:v>
+                  <c:v>0.23687120662044178</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7911,7 +7911,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="es-AR"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -11378,22 +11378,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:40" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="AG1" s="450" t="s">
+      <c r="AG1" s="475" t="s">
         <v>56</v>
       </c>
-      <c r="AH1" s="450" t="s">
+      <c r="AH1" s="475" t="s">
         <v>57</v>
       </c>
-      <c r="AI1" s="450" t="s">
+      <c r="AI1" s="475" t="s">
         <v>52</v>
       </c>
-      <c r="AJ1" s="450" t="s">
+      <c r="AJ1" s="475" t="s">
         <v>56</v>
       </c>
-      <c r="AK1" s="444" t="s">
+      <c r="AK1" s="484" t="s">
         <v>57</v>
       </c>
-      <c r="AL1" s="444" t="s">
+      <c r="AL1" s="484" t="s">
         <v>52</v>
       </c>
     </row>
@@ -11470,23 +11470,23 @@
       <c r="Y2" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="AB2" s="447" t="s">
+      <c r="AB2" s="487" t="s">
         <v>25</v>
       </c>
-      <c r="AC2" s="448"/>
-      <c r="AD2" s="451" t="s">
+      <c r="AC2" s="488"/>
+      <c r="AD2" s="482" t="s">
         <v>58</v>
       </c>
-      <c r="AE2" s="451"/>
+      <c r="AE2" s="482"/>
       <c r="AF2" s="97" t="s">
         <v>103</v>
       </c>
-      <c r="AG2" s="452"/>
-      <c r="AH2" s="450"/>
-      <c r="AI2" s="450"/>
-      <c r="AJ2" s="450"/>
-      <c r="AK2" s="444"/>
-      <c r="AL2" s="444"/>
+      <c r="AG2" s="490"/>
+      <c r="AH2" s="475"/>
+      <c r="AI2" s="475"/>
+      <c r="AJ2" s="475"/>
+      <c r="AK2" s="484"/>
+      <c r="AL2" s="484"/>
     </row>
     <row r="3" spans="2:40" x14ac:dyDescent="0.25">
       <c r="B3" s="14">
@@ -13217,22 +13217,22 @@
       <c r="Y16" s="41">
         <v>1.1583636475738333</v>
       </c>
-      <c r="AG16" s="450" t="s">
+      <c r="AG16" s="475" t="s">
         <v>56</v>
       </c>
-      <c r="AH16" s="450" t="s">
+      <c r="AH16" s="475" t="s">
         <v>57</v>
       </c>
-      <c r="AI16" s="450" t="s">
+      <c r="AI16" s="475" t="s">
         <v>52</v>
       </c>
-      <c r="AJ16" s="450" t="s">
+      <c r="AJ16" s="475" t="s">
         <v>56</v>
       </c>
-      <c r="AK16" s="444" t="s">
+      <c r="AK16" s="484" t="s">
         <v>57</v>
       </c>
-      <c r="AL16" s="444" t="s">
+      <c r="AL16" s="484" t="s">
         <v>52</v>
       </c>
       <c r="AN16" s="435"/>
@@ -13311,23 +13311,23 @@
         <v>1.2284974412725813</v>
       </c>
       <c r="Z17" s="435"/>
-      <c r="AB17" s="447" t="s">
+      <c r="AB17" s="487" t="s">
         <v>40</v>
       </c>
-      <c r="AC17" s="449"/>
-      <c r="AD17" s="451" t="s">
+      <c r="AC17" s="489"/>
+      <c r="AD17" s="482" t="s">
         <v>58</v>
       </c>
-      <c r="AE17" s="451"/>
+      <c r="AE17" s="482"/>
       <c r="AF17" s="252" t="s">
         <v>103</v>
       </c>
-      <c r="AG17" s="450"/>
-      <c r="AH17" s="450"/>
-      <c r="AI17" s="450"/>
-      <c r="AJ17" s="450"/>
-      <c r="AK17" s="444"/>
-      <c r="AL17" s="444"/>
+      <c r="AG17" s="475"/>
+      <c r="AH17" s="475"/>
+      <c r="AI17" s="475"/>
+      <c r="AJ17" s="475"/>
+      <c r="AK17" s="484"/>
+      <c r="AL17" s="484"/>
       <c r="AN17" s="435"/>
     </row>
     <row r="18" spans="2:40" x14ac:dyDescent="0.25">
@@ -15036,14 +15036,14 @@
       <c r="Y32" s="41">
         <v>6.9971946482520506</v>
       </c>
-      <c r="AA32" s="445" t="s">
+      <c r="AA32" s="485" t="s">
         <v>25</v>
       </c>
-      <c r="AB32" s="445"/>
-      <c r="AC32" s="446" t="s">
+      <c r="AB32" s="485"/>
+      <c r="AC32" s="486" t="s">
         <v>40</v>
       </c>
-      <c r="AD32" s="446"/>
+      <c r="AD32" s="486"/>
       <c r="AI32" s="229" t="s">
         <v>76</v>
       </c>
@@ -16576,45 +16576,45 @@
       </c>
     </row>
     <row r="51" spans="2:40" x14ac:dyDescent="0.25">
-      <c r="AA51" s="451" t="s">
+      <c r="AA51" s="482" t="s">
         <v>102</v>
       </c>
-      <c r="AB51" s="451"/>
-      <c r="AC51" s="451"/>
-      <c r="AD51" s="451"/>
-      <c r="AE51" s="451"/>
-      <c r="AF51" s="451"/>
-      <c r="AG51" s="451"/>
-      <c r="AH51" s="451"/>
-      <c r="AI51" s="451"/>
-      <c r="AJ51" s="451"/>
-      <c r="AK51" s="451"/>
-      <c r="AL51" s="451"/>
-      <c r="AM51" s="451"/>
-      <c r="AN51" s="451"/>
+      <c r="AB51" s="482"/>
+      <c r="AC51" s="482"/>
+      <c r="AD51" s="482"/>
+      <c r="AE51" s="482"/>
+      <c r="AF51" s="482"/>
+      <c r="AG51" s="482"/>
+      <c r="AH51" s="482"/>
+      <c r="AI51" s="482"/>
+      <c r="AJ51" s="482"/>
+      <c r="AK51" s="482"/>
+      <c r="AL51" s="482"/>
+      <c r="AM51" s="482"/>
+      <c r="AN51" s="482"/>
     </row>
     <row r="52" spans="2:40" x14ac:dyDescent="0.25">
       <c r="AA52" s="56"/>
-      <c r="AB52" s="462" t="s">
+      <c r="AB52" s="483" t="s">
         <v>72</v>
       </c>
-      <c r="AC52" s="462"/>
-      <c r="AD52" s="462"/>
-      <c r="AE52" s="462" t="s">
+      <c r="AC52" s="483"/>
+      <c r="AD52" s="483"/>
+      <c r="AE52" s="483" t="s">
         <v>73</v>
       </c>
-      <c r="AF52" s="462"/>
-      <c r="AG52" s="462"/>
-      <c r="AH52" s="462" t="s">
+      <c r="AF52" s="483"/>
+      <c r="AG52" s="483"/>
+      <c r="AH52" s="483" t="s">
         <v>74</v>
       </c>
-      <c r="AI52" s="462"/>
-      <c r="AJ52" s="462"/>
-      <c r="AK52" s="462" t="s">
+      <c r="AI52" s="483"/>
+      <c r="AJ52" s="483"/>
+      <c r="AK52" s="483" t="s">
         <v>75</v>
       </c>
-      <c r="AL52" s="462"/>
-      <c r="AM52" s="462"/>
+      <c r="AL52" s="483"/>
+      <c r="AM52" s="483"/>
       <c r="AN52" s="56"/>
     </row>
     <row r="53" spans="2:40" x14ac:dyDescent="0.25">
@@ -16709,34 +16709,34 @@
       </c>
     </row>
     <row r="55" spans="2:40" x14ac:dyDescent="0.25">
-      <c r="B55" s="459" t="s">
+      <c r="B55" s="479" t="s">
         <v>1</v>
       </c>
-      <c r="C55" s="460"/>
-      <c r="D55" s="460"/>
-      <c r="E55" s="460"/>
-      <c r="F55" s="461"/>
-      <c r="G55" s="459" t="s">
+      <c r="C55" s="480"/>
+      <c r="D55" s="480"/>
+      <c r="E55" s="480"/>
+      <c r="F55" s="481"/>
+      <c r="G55" s="479" t="s">
         <v>2</v>
       </c>
-      <c r="H55" s="460"/>
-      <c r="I55" s="460"/>
-      <c r="J55" s="460"/>
-      <c r="K55" s="461"/>
-      <c r="L55" s="459" t="s">
+      <c r="H55" s="480"/>
+      <c r="I55" s="480"/>
+      <c r="J55" s="480"/>
+      <c r="K55" s="481"/>
+      <c r="L55" s="479" t="s">
         <v>3</v>
       </c>
-      <c r="M55" s="460"/>
-      <c r="N55" s="460"/>
-      <c r="O55" s="460"/>
-      <c r="P55" s="461"/>
-      <c r="Q55" s="459" t="s">
+      <c r="M55" s="480"/>
+      <c r="N55" s="480"/>
+      <c r="O55" s="480"/>
+      <c r="P55" s="481"/>
+      <c r="Q55" s="479" t="s">
         <v>4</v>
       </c>
-      <c r="R55" s="460"/>
-      <c r="S55" s="460"/>
-      <c r="T55" s="460"/>
-      <c r="U55" s="461"/>
+      <c r="R55" s="480"/>
+      <c r="S55" s="480"/>
+      <c r="T55" s="480"/>
+      <c r="U55" s="481"/>
       <c r="AA55" s="218" t="s">
         <v>80</v>
       </c>
@@ -17947,20 +17947,20 @@
     </row>
     <row r="69" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="70" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B70" s="453" t="s">
+      <c r="B70" s="451" t="s">
         <v>5</v>
       </c>
-      <c r="C70" s="454"/>
-      <c r="D70" s="454"/>
-      <c r="E70" s="454"/>
-      <c r="F70" s="455"/>
-      <c r="G70" s="453" t="s">
+      <c r="C70" s="452"/>
+      <c r="D70" s="452"/>
+      <c r="E70" s="452"/>
+      <c r="F70" s="453"/>
+      <c r="G70" s="451" t="s">
         <v>6</v>
       </c>
-      <c r="H70" s="454"/>
-      <c r="I70" s="454"/>
-      <c r="J70" s="454"/>
-      <c r="K70" s="455"/>
+      <c r="H70" s="452"/>
+      <c r="I70" s="452"/>
+      <c r="J70" s="452"/>
+      <c r="K70" s="453"/>
     </row>
     <row r="71" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B71" s="150" t="s">
@@ -18368,20 +18368,20 @@
     </row>
     <row r="84" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="85" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B85" s="456" t="s">
+      <c r="B85" s="476" t="s">
         <v>7</v>
       </c>
-      <c r="C85" s="457"/>
-      <c r="D85" s="457"/>
-      <c r="E85" s="457"/>
-      <c r="F85" s="458"/>
-      <c r="G85" s="456" t="s">
+      <c r="C85" s="477"/>
+      <c r="D85" s="477"/>
+      <c r="E85" s="477"/>
+      <c r="F85" s="478"/>
+      <c r="G85" s="476" t="s">
         <v>8</v>
       </c>
-      <c r="H85" s="457"/>
-      <c r="I85" s="457"/>
-      <c r="J85" s="457"/>
-      <c r="K85" s="458"/>
+      <c r="H85" s="477"/>
+      <c r="I85" s="477"/>
+      <c r="J85" s="477"/>
+      <c r="K85" s="478"/>
     </row>
     <row r="86" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B86" s="173" t="s">
@@ -20421,34 +20421,34 @@
     </row>
     <row r="129" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="130" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B130" s="453" t="s">
+      <c r="B130" s="451" t="s">
         <v>17</v>
       </c>
-      <c r="C130" s="454"/>
-      <c r="D130" s="454"/>
-      <c r="E130" s="454"/>
-      <c r="F130" s="455"/>
-      <c r="G130" s="453" t="s">
+      <c r="C130" s="452"/>
+      <c r="D130" s="452"/>
+      <c r="E130" s="452"/>
+      <c r="F130" s="453"/>
+      <c r="G130" s="451" t="s">
         <v>18</v>
       </c>
-      <c r="H130" s="454"/>
-      <c r="I130" s="454"/>
-      <c r="J130" s="454"/>
-      <c r="K130" s="455"/>
-      <c r="L130" s="475" t="s">
+      <c r="H130" s="452"/>
+      <c r="I130" s="452"/>
+      <c r="J130" s="452"/>
+      <c r="K130" s="453"/>
+      <c r="L130" s="454" t="s">
         <v>19</v>
       </c>
-      <c r="M130" s="476"/>
-      <c r="N130" s="476"/>
-      <c r="O130" s="476"/>
-      <c r="P130" s="477"/>
-      <c r="Q130" s="453" t="s">
+      <c r="M130" s="455"/>
+      <c r="N130" s="455"/>
+      <c r="O130" s="455"/>
+      <c r="P130" s="456"/>
+      <c r="Q130" s="451" t="s">
         <v>20</v>
       </c>
-      <c r="R130" s="454"/>
-      <c r="S130" s="454"/>
-      <c r="T130" s="454"/>
-      <c r="U130" s="455"/>
+      <c r="R130" s="452"/>
+      <c r="S130" s="452"/>
+      <c r="T130" s="452"/>
+      <c r="U130" s="453"/>
     </row>
     <row r="131" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B131" s="150" t="s">
@@ -21236,27 +21236,27 @@
     </row>
     <row r="144" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="145" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B145" s="478" t="s">
+      <c r="B145" s="457" t="s">
         <v>21</v>
       </c>
-      <c r="C145" s="479"/>
-      <c r="D145" s="479"/>
-      <c r="E145" s="479"/>
-      <c r="F145" s="480"/>
-      <c r="G145" s="478" t="s">
+      <c r="C145" s="458"/>
+      <c r="D145" s="458"/>
+      <c r="E145" s="458"/>
+      <c r="F145" s="459"/>
+      <c r="G145" s="457" t="s">
         <v>22</v>
       </c>
-      <c r="H145" s="479"/>
-      <c r="I145" s="479"/>
-      <c r="J145" s="479"/>
-      <c r="K145" s="480"/>
-      <c r="L145" s="481" t="s">
+      <c r="H145" s="458"/>
+      <c r="I145" s="458"/>
+      <c r="J145" s="458"/>
+      <c r="K145" s="459"/>
+      <c r="L145" s="460" t="s">
         <v>23</v>
       </c>
-      <c r="M145" s="482"/>
-      <c r="N145" s="482"/>
-      <c r="O145" s="482"/>
-      <c r="P145" s="483"/>
+      <c r="M145" s="461"/>
+      <c r="N145" s="461"/>
+      <c r="O145" s="461"/>
+      <c r="P145" s="462"/>
     </row>
     <row r="146" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B146" s="203" t="s">
@@ -21855,36 +21855,6 @@
     </row>
   </sheetData>
   <mergeCells count="46">
-    <mergeCell ref="B130:F130"/>
-    <mergeCell ref="G130:K130"/>
-    <mergeCell ref="L130:P130"/>
-    <mergeCell ref="Q130:U130"/>
-    <mergeCell ref="B145:F145"/>
-    <mergeCell ref="G145:K145"/>
-    <mergeCell ref="L145:P145"/>
-    <mergeCell ref="B100:F100"/>
-    <mergeCell ref="G100:K100"/>
-    <mergeCell ref="L100:P100"/>
-    <mergeCell ref="Q100:U100"/>
-    <mergeCell ref="B115:F115"/>
-    <mergeCell ref="G115:K115"/>
-    <mergeCell ref="L115:P115"/>
-    <mergeCell ref="Q115:U115"/>
-    <mergeCell ref="AH16:AH17"/>
-    <mergeCell ref="AI16:AI17"/>
-    <mergeCell ref="B70:F70"/>
-    <mergeCell ref="G70:K70"/>
-    <mergeCell ref="B85:F85"/>
-    <mergeCell ref="G85:K85"/>
-    <mergeCell ref="B55:F55"/>
-    <mergeCell ref="G55:K55"/>
-    <mergeCell ref="L55:P55"/>
-    <mergeCell ref="Q55:U55"/>
-    <mergeCell ref="AA51:AN51"/>
-    <mergeCell ref="AB52:AD52"/>
-    <mergeCell ref="AE52:AG52"/>
-    <mergeCell ref="AH52:AJ52"/>
-    <mergeCell ref="AK52:AM52"/>
     <mergeCell ref="AL1:AL2"/>
     <mergeCell ref="AL16:AL17"/>
     <mergeCell ref="AK16:AK17"/>
@@ -21901,6 +21871,36 @@
     <mergeCell ref="AH1:AH2"/>
     <mergeCell ref="AI1:AI2"/>
     <mergeCell ref="AG16:AG17"/>
+    <mergeCell ref="AH16:AH17"/>
+    <mergeCell ref="AI16:AI17"/>
+    <mergeCell ref="B70:F70"/>
+    <mergeCell ref="G70:K70"/>
+    <mergeCell ref="B85:F85"/>
+    <mergeCell ref="G85:K85"/>
+    <mergeCell ref="B55:F55"/>
+    <mergeCell ref="G55:K55"/>
+    <mergeCell ref="L55:P55"/>
+    <mergeCell ref="Q55:U55"/>
+    <mergeCell ref="AA51:AN51"/>
+    <mergeCell ref="AB52:AD52"/>
+    <mergeCell ref="AE52:AG52"/>
+    <mergeCell ref="AH52:AJ52"/>
+    <mergeCell ref="AK52:AM52"/>
+    <mergeCell ref="B100:F100"/>
+    <mergeCell ref="G100:K100"/>
+    <mergeCell ref="L100:P100"/>
+    <mergeCell ref="Q100:U100"/>
+    <mergeCell ref="B115:F115"/>
+    <mergeCell ref="G115:K115"/>
+    <mergeCell ref="L115:P115"/>
+    <mergeCell ref="Q115:U115"/>
+    <mergeCell ref="B130:F130"/>
+    <mergeCell ref="G130:K130"/>
+    <mergeCell ref="L130:P130"/>
+    <mergeCell ref="Q130:U130"/>
+    <mergeCell ref="B145:F145"/>
+    <mergeCell ref="G145:K145"/>
+    <mergeCell ref="L145:P145"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -21911,7 +21911,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F64C6BB9-54B5-42EC-B225-E298A2E667FE}">
   <dimension ref="B1:BA158"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A51" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="N85" sqref="N85"/>
     </sheetView>
   </sheetViews>
@@ -21935,22 +21935,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:53" x14ac:dyDescent="0.25">
-      <c r="AG1" s="450" t="s">
+      <c r="AG1" s="475" t="s">
         <v>56</v>
       </c>
-      <c r="AH1" s="450" t="s">
+      <c r="AH1" s="475" t="s">
         <v>57</v>
       </c>
-      <c r="AI1" s="450" t="s">
+      <c r="AI1" s="475" t="s">
         <v>52</v>
       </c>
-      <c r="AJ1" s="450" t="s">
+      <c r="AJ1" s="475" t="s">
         <v>56</v>
       </c>
-      <c r="AK1" s="450" t="s">
+      <c r="AK1" s="475" t="s">
         <v>57</v>
       </c>
-      <c r="AL1" s="450" t="s">
+      <c r="AL1" s="475" t="s">
         <v>52</v>
       </c>
     </row>
@@ -22027,23 +22027,23 @@
       <c r="Y2" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="AB2" s="447" t="s">
+      <c r="AB2" s="487" t="s">
         <v>25</v>
       </c>
-      <c r="AC2" s="448"/>
-      <c r="AD2" s="451" t="s">
+      <c r="AC2" s="488"/>
+      <c r="AD2" s="482" t="s">
         <v>58</v>
       </c>
-      <c r="AE2" s="451"/>
+      <c r="AE2" s="482"/>
       <c r="AF2" s="97" t="s">
         <v>103</v>
       </c>
-      <c r="AG2" s="450"/>
-      <c r="AH2" s="450"/>
-      <c r="AI2" s="450"/>
-      <c r="AJ2" s="450"/>
-      <c r="AK2" s="450"/>
-      <c r="AL2" s="450"/>
+      <c r="AG2" s="475"/>
+      <c r="AH2" s="475"/>
+      <c r="AI2" s="475"/>
+      <c r="AJ2" s="475"/>
+      <c r="AK2" s="475"/>
+      <c r="AL2" s="475"/>
     </row>
     <row r="3" spans="2:53" x14ac:dyDescent="0.25">
       <c r="B3" s="14">
@@ -23584,22 +23584,22 @@
       <c r="Y15" s="371">
         <v>1.0235026535253984</v>
       </c>
-      <c r="AG15" s="450" t="s">
+      <c r="AG15" s="475" t="s">
         <v>56</v>
       </c>
-      <c r="AH15" s="450" t="s">
+      <c r="AH15" s="475" t="s">
         <v>57</v>
       </c>
-      <c r="AI15" s="450" t="s">
+      <c r="AI15" s="475" t="s">
         <v>52</v>
       </c>
-      <c r="AJ15" s="450" t="s">
+      <c r="AJ15" s="475" t="s">
         <v>56</v>
       </c>
-      <c r="AK15" s="450" t="s">
+      <c r="AK15" s="475" t="s">
         <v>57</v>
       </c>
-      <c r="AL15" s="450" t="s">
+      <c r="AL15" s="475" t="s">
         <v>52</v>
       </c>
       <c r="AM15" s="437"/>
@@ -23676,23 +23676,23 @@
       <c r="Y16" s="371">
         <v>1.0708870356330553</v>
       </c>
-      <c r="AB16" s="447" t="s">
+      <c r="AB16" s="487" t="s">
         <v>40</v>
       </c>
-      <c r="AC16" s="449"/>
-      <c r="AD16" s="451" t="s">
+      <c r="AC16" s="489"/>
+      <c r="AD16" s="482" t="s">
         <v>58</v>
       </c>
-      <c r="AE16" s="451"/>
+      <c r="AE16" s="482"/>
       <c r="AF16" s="97" t="s">
         <v>103</v>
       </c>
-      <c r="AG16" s="450"/>
-      <c r="AH16" s="450"/>
-      <c r="AI16" s="450"/>
-      <c r="AJ16" s="450"/>
-      <c r="AK16" s="450"/>
-      <c r="AL16" s="450"/>
+      <c r="AG16" s="475"/>
+      <c r="AH16" s="475"/>
+      <c r="AI16" s="475"/>
+      <c r="AJ16" s="475"/>
+      <c r="AK16" s="475"/>
+      <c r="AL16" s="475"/>
       <c r="AM16" s="437"/>
       <c r="AN16" s="437"/>
     </row>
@@ -25373,14 +25373,14 @@
       <c r="Y31" s="371">
         <v>6.6148597422289619</v>
       </c>
-      <c r="AA31" s="445" t="s">
+      <c r="AA31" s="485" t="s">
         <v>25</v>
       </c>
-      <c r="AB31" s="445"/>
-      <c r="AC31" s="446" t="s">
+      <c r="AB31" s="485"/>
+      <c r="AC31" s="486" t="s">
         <v>40</v>
       </c>
-      <c r="AD31" s="446"/>
+      <c r="AD31" s="486"/>
       <c r="AJ31" s="229" t="s">
         <v>76</v>
       </c>
@@ -25591,11 +25591,11 @@
         <v>80</v>
       </c>
       <c r="AK33" s="239">
-        <f t="shared" ref="AK32:AK37" si="12">AD19-AD5</f>
+        <f t="shared" ref="AK33:AK37" si="12">AD19-AD5</f>
         <v>1.1436999999999999</v>
       </c>
       <c r="AL33" s="239">
-        <f t="shared" ref="AL32:AL37" si="13">AE19-AE5</f>
+        <f t="shared" ref="AL33:AL37" si="13">AE19-AE5</f>
         <v>5.572280000000001</v>
       </c>
       <c r="AM33" s="239">
@@ -26938,34 +26938,34 @@
     </row>
     <row r="54" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="55" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B55" s="484" t="s">
+      <c r="B55" s="491" t="s">
         <v>1</v>
       </c>
-      <c r="C55" s="485"/>
-      <c r="D55" s="485"/>
-      <c r="E55" s="485"/>
-      <c r="F55" s="486"/>
-      <c r="G55" s="484" t="s">
+      <c r="C55" s="492"/>
+      <c r="D55" s="492"/>
+      <c r="E55" s="492"/>
+      <c r="F55" s="493"/>
+      <c r="G55" s="491" t="s">
         <v>2</v>
       </c>
-      <c r="H55" s="485"/>
-      <c r="I55" s="485"/>
-      <c r="J55" s="485"/>
-      <c r="K55" s="486"/>
-      <c r="L55" s="484" t="s">
+      <c r="H55" s="492"/>
+      <c r="I55" s="492"/>
+      <c r="J55" s="492"/>
+      <c r="K55" s="493"/>
+      <c r="L55" s="491" t="s">
         <v>3</v>
       </c>
-      <c r="M55" s="485"/>
-      <c r="N55" s="485"/>
-      <c r="O55" s="485"/>
-      <c r="P55" s="486"/>
-      <c r="Q55" s="484" t="s">
+      <c r="M55" s="492"/>
+      <c r="N55" s="492"/>
+      <c r="O55" s="492"/>
+      <c r="P55" s="493"/>
+      <c r="Q55" s="491" t="s">
         <v>4</v>
       </c>
-      <c r="R55" s="485"/>
-      <c r="S55" s="485"/>
-      <c r="T55" s="485"/>
-      <c r="U55" s="486"/>
+      <c r="R55" s="492"/>
+      <c r="S55" s="492"/>
+      <c r="T55" s="492"/>
+      <c r="U55" s="493"/>
     </row>
     <row r="56" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B56" s="92" t="s">
@@ -27752,32 +27752,32 @@
       <c r="U68" s="147"/>
     </row>
     <row r="69" spans="2:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="V69" s="494" t="s">
+      <c r="V69" s="444" t="s">
         <v>112</v>
       </c>
-      <c r="W69" s="494" t="s">
+      <c r="W69" s="444" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="70" spans="2:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B70" s="475" t="s">
+      <c r="B70" s="454" t="s">
         <v>5</v>
       </c>
-      <c r="C70" s="476"/>
-      <c r="D70" s="476"/>
-      <c r="E70" s="476"/>
-      <c r="F70" s="477"/>
-      <c r="G70" s="475" t="s">
+      <c r="C70" s="455"/>
+      <c r="D70" s="455"/>
+      <c r="E70" s="455"/>
+      <c r="F70" s="456"/>
+      <c r="G70" s="454" t="s">
         <v>6</v>
       </c>
-      <c r="H70" s="476"/>
-      <c r="I70" s="476"/>
-      <c r="J70" s="476"/>
-      <c r="K70" s="477"/>
-      <c r="R70" s="494" t="s">
+      <c r="H70" s="455"/>
+      <c r="I70" s="455"/>
+      <c r="J70" s="455"/>
+      <c r="K70" s="456"/>
+      <c r="R70" s="444" t="s">
         <v>112</v>
       </c>
-      <c r="S70" s="494" t="s">
+      <c r="S70" s="444" t="s">
         <v>113</v>
       </c>
       <c r="V70" s="151" t="s">
@@ -27786,10 +27786,10 @@
       <c r="W70" s="151" t="s">
         <v>68</v>
       </c>
-      <c r="Y70" s="494" t="s">
+      <c r="Y70" s="444" t="s">
         <v>112</v>
       </c>
-      <c r="Z70" s="494" t="s">
+      <c r="Z70" s="444" t="s">
         <v>113</v>
       </c>
     </row>
@@ -27824,10 +27824,10 @@
       <c r="K71" s="152" t="s">
         <v>69</v>
       </c>
-      <c r="M71" s="494" t="s">
+      <c r="M71" s="444" t="s">
         <v>112</v>
       </c>
-      <c r="N71" s="494" t="s">
+      <c r="N71" s="444" t="s">
         <v>113</v>
       </c>
       <c r="Q71" s="156">
@@ -27897,7 +27897,7 @@
         <v>6.3091999999999997</v>
       </c>
       <c r="P72">
-        <f t="shared" ref="P72:P73" si="18">(N72-M72)/M72</f>
+        <f t="shared" ref="P72" si="18">(N72-M72)/M72</f>
         <v>3.0456556588650203</v>
       </c>
       <c r="Q72" s="98">
@@ -27918,19 +27918,19 @@
       <c r="W72" s="220">
         <v>37.377601585728442</v>
       </c>
-      <c r="Y72" s="496">
+      <c r="Y72" s="446">
         <f>V72-V71</f>
         <v>11.129658385093167</v>
       </c>
-      <c r="Z72" s="496">
+      <c r="Z72" s="446">
         <f>W72-W71</f>
         <v>37.377601585728442</v>
       </c>
-      <c r="AB72" s="497">
+      <c r="AB72" s="447">
         <f>Y72/100*$C$83</f>
         <v>1.1468</v>
       </c>
-      <c r="AC72" s="497">
+      <c r="AC72" s="447">
         <f>Z72/100*$H$83</f>
         <v>5.6570999999999998</v>
       </c>
@@ -27984,19 +27984,19 @@
       <c r="W73" s="275">
         <v>41.686157912124216</v>
       </c>
-      <c r="Y73" s="496">
+      <c r="Y73" s="446">
         <f t="shared" ref="Y73:Z82" si="19">V73-V72</f>
         <v>4.0052406832298129</v>
       </c>
-      <c r="Z73" s="496">
+      <c r="Z73" s="446">
         <f t="shared" si="19"/>
         <v>4.3085563263957738</v>
       </c>
-      <c r="AB73" s="497">
+      <c r="AB73" s="447">
         <f t="shared" ref="AB73:AB82" si="20">Y73/100*$C$83</f>
         <v>0.41269999999999996</v>
       </c>
-      <c r="AC73" s="497">
+      <c r="AC73" s="447">
         <f t="shared" ref="AC73:AC82" si="21">Z73/100*$H$83</f>
         <v>0.65210000000000035</v>
       </c>
@@ -28044,10 +28044,10 @@
         <f>(N74-M74)/M74</f>
         <v>0.73879618159294591</v>
       </c>
-      <c r="Q74" s="495">
+      <c r="Q74" s="445">
         <v>0.5</v>
       </c>
-      <c r="U74" s="495">
+      <c r="U74" s="445">
         <v>0.5</v>
       </c>
       <c r="V74">
@@ -28058,19 +28058,19 @@
         <f>_xlfn.FORECAST.LINEAR(U74,J74:J75,B74:B75)</f>
         <v>55.289665735651859</v>
       </c>
-      <c r="Y74" s="496">
+      <c r="Y74" s="446">
         <f t="shared" si="19"/>
         <v>24.26939229249011</v>
       </c>
-      <c r="Z74" s="496">
+      <c r="Z74" s="446">
         <f t="shared" si="19"/>
         <v>13.603507823527643</v>
       </c>
-      <c r="AB74" s="497">
+      <c r="AB74" s="447">
         <f t="shared" si="20"/>
         <v>2.500718181818181</v>
       </c>
-      <c r="AC74" s="497">
+      <c r="AC74" s="447">
         <f t="shared" si="21"/>
         <v>2.0588909090909091</v>
       </c>
@@ -28124,19 +28124,19 @@
       <c r="W75" s="277">
         <v>63.063098777667662</v>
       </c>
-      <c r="Y75" s="496">
+      <c r="Y75" s="446">
         <f t="shared" si="19"/>
         <v>13.868224167137214</v>
       </c>
-      <c r="Z75" s="496">
+      <c r="Z75" s="446">
         <f t="shared" si="19"/>
         <v>7.7734330420158031</v>
       </c>
-      <c r="AB75" s="498">
+      <c r="AB75" s="448">
         <f t="shared" si="20"/>
         <v>1.4289818181818186</v>
       </c>
-      <c r="AC75" s="498">
+      <c r="AC75" s="448">
         <f t="shared" si="21"/>
         <v>1.1765090909090918</v>
       </c>
@@ -28181,7 +28181,7 @@
         <v>8.3680909090909097</v>
       </c>
       <c r="P76">
-        <f t="shared" ref="P75:P76" si="22">(N76-M76)/M76</f>
+        <f t="shared" ref="P76" si="22">(N76-M76)/M76</f>
         <v>1.0609953786630371</v>
       </c>
       <c r="Q76" s="98">
@@ -28202,19 +28202,19 @@
       <c r="W76" s="220">
         <v>66.285431119920716</v>
       </c>
-      <c r="Y76" s="496">
+      <c r="Y76" s="446">
         <f t="shared" si="19"/>
         <v>5.0883152173913047</v>
       </c>
-      <c r="Z76" s="496">
+      <c r="Z76" s="446">
         <f t="shared" si="19"/>
         <v>3.2223323422530541</v>
       </c>
-      <c r="AB76" s="499">
+      <c r="AB76" s="449">
         <f t="shared" si="20"/>
         <v>0.52429999999999999</v>
       </c>
-      <c r="AC76" s="499">
+      <c r="AC76" s="449">
         <f t="shared" si="21"/>
         <v>0.48769999999999974</v>
       </c>
@@ -28268,19 +28268,19 @@
       <c r="W77" s="220">
         <v>76.8780971258672</v>
       </c>
-      <c r="Y77" s="496">
+      <c r="Y77" s="446">
         <f t="shared" si="19"/>
         <v>14.436141304347821</v>
       </c>
-      <c r="Z77" s="496">
+      <c r="Z77" s="446">
         <f t="shared" si="19"/>
         <v>10.592666005946484</v>
       </c>
-      <c r="AB77" s="499">
+      <c r="AB77" s="449">
         <f t="shared" si="20"/>
         <v>1.4874999999999996</v>
       </c>
-      <c r="AC77" s="499">
+      <c r="AC77" s="449">
         <f t="shared" si="21"/>
         <v>1.6032000000000004</v>
       </c>
@@ -28334,19 +28334,19 @@
       <c r="W78" s="275">
         <v>85.37628014535845</v>
       </c>
-      <c r="Y78" s="496">
+      <c r="Y78" s="446">
         <f t="shared" si="19"/>
         <v>10.289208074534159</v>
       </c>
-      <c r="Z78" s="496">
+      <c r="Z78" s="446">
         <f t="shared" si="19"/>
         <v>8.4981830194912504</v>
       </c>
-      <c r="AB78" s="500">
+      <c r="AB78" s="450">
         <f t="shared" si="20"/>
         <v>1.0601999999999998</v>
       </c>
-      <c r="AC78" s="500">
+      <c r="AC78" s="450">
         <f t="shared" si="21"/>
         <v>1.2862000000000009</v>
       </c>
@@ -28400,19 +28400,19 @@
       <c r="W79" s="277">
         <v>87.364387182028423</v>
       </c>
-      <c r="Y79" s="496">
+      <c r="Y79" s="446">
         <f t="shared" si="19"/>
         <v>2.5174689440993774</v>
       </c>
-      <c r="Z79" s="496">
+      <c r="Z79" s="446">
         <f t="shared" si="19"/>
         <v>1.9881070366699731</v>
       </c>
-      <c r="AB79" s="497">
+      <c r="AB79" s="447">
         <f t="shared" si="20"/>
         <v>0.25939999999999985</v>
       </c>
-      <c r="AC79" s="497">
+      <c r="AC79" s="447">
         <f t="shared" si="21"/>
         <v>0.30090000000000039</v>
       </c>
@@ -28466,19 +28466,19 @@
       <c r="W80" s="220">
         <v>92.56359431780642</v>
       </c>
-      <c r="Y80" s="496">
+      <c r="Y80" s="446">
         <f t="shared" si="19"/>
         <v>6.1781832298136692</v>
       </c>
-      <c r="Z80" s="496">
+      <c r="Z80" s="446">
         <f t="shared" si="19"/>
         <v>5.1992071357779963</v>
       </c>
-      <c r="AB80" s="497">
+      <c r="AB80" s="447">
         <f t="shared" si="20"/>
         <v>0.6366000000000005</v>
       </c>
-      <c r="AC80" s="497">
+      <c r="AC80" s="447">
         <f t="shared" si="21"/>
         <v>0.78689999999999982</v>
       </c>
@@ -28532,19 +28532,19 @@
       <c r="W81" s="220">
         <v>98.999008919722513</v>
       </c>
-      <c r="Y81" s="496">
+      <c r="Y81" s="446">
         <f t="shared" si="19"/>
         <v>6.5382375776397481</v>
       </c>
-      <c r="Z81" s="496">
+      <c r="Z81" s="446">
         <f t="shared" si="19"/>
         <v>6.4354146019160936</v>
       </c>
-      <c r="AB81" s="497">
+      <c r="AB81" s="447">
         <f t="shared" si="20"/>
         <v>0.67369999999999963</v>
       </c>
-      <c r="AC81" s="497">
+      <c r="AC81" s="447">
         <f t="shared" si="21"/>
         <v>0.97400000000000075</v>
       </c>
@@ -28598,19 +28598,19 @@
       <c r="W82" s="275">
         <v>100.00000000000003</v>
       </c>
-      <c r="Y82" s="496">
+      <c r="Y82" s="446">
         <f t="shared" si="19"/>
         <v>1.6799301242236169</v>
       </c>
-      <c r="Z82" s="496">
+      <c r="Z82" s="446">
         <f t="shared" si="19"/>
         <v>1.0009910802775153</v>
       </c>
-      <c r="AB82" s="497">
+      <c r="AB82" s="447">
         <f t="shared" si="20"/>
         <v>0.17310000000000147</v>
       </c>
-      <c r="AC82" s="497">
+      <c r="AC82" s="447">
         <f t="shared" si="21"/>
         <v>0.15150000000000194</v>
       </c>
@@ -28637,20 +28637,20 @@
     </row>
     <row r="84" spans="2:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="85" spans="2:29" x14ac:dyDescent="0.25">
-      <c r="B85" s="487" t="s">
+      <c r="B85" s="494" t="s">
         <v>7</v>
       </c>
-      <c r="C85" s="488"/>
-      <c r="D85" s="488"/>
-      <c r="E85" s="488"/>
-      <c r="F85" s="489"/>
-      <c r="G85" s="487" t="s">
+      <c r="C85" s="495"/>
+      <c r="D85" s="495"/>
+      <c r="E85" s="495"/>
+      <c r="F85" s="496"/>
+      <c r="G85" s="494" t="s">
         <v>8</v>
       </c>
-      <c r="H85" s="488"/>
-      <c r="I85" s="488"/>
-      <c r="J85" s="488"/>
-      <c r="K85" s="489"/>
+      <c r="H85" s="495"/>
+      <c r="I85" s="495"/>
+      <c r="J85" s="495"/>
+      <c r="K85" s="496"/>
     </row>
     <row r="86" spans="2:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B86" s="173" t="s">
@@ -30582,34 +30582,34 @@
     </row>
     <row r="129" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="130" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B130" s="475" t="s">
+      <c r="B130" s="454" t="s">
         <v>17</v>
       </c>
-      <c r="C130" s="476"/>
-      <c r="D130" s="476"/>
-      <c r="E130" s="476"/>
-      <c r="F130" s="477"/>
-      <c r="G130" s="475" t="s">
+      <c r="C130" s="455"/>
+      <c r="D130" s="455"/>
+      <c r="E130" s="455"/>
+      <c r="F130" s="456"/>
+      <c r="G130" s="454" t="s">
         <v>18</v>
       </c>
-      <c r="H130" s="476"/>
-      <c r="I130" s="476"/>
-      <c r="J130" s="476"/>
-      <c r="K130" s="477"/>
-      <c r="L130" s="475" t="s">
+      <c r="H130" s="455"/>
+      <c r="I130" s="455"/>
+      <c r="J130" s="455"/>
+      <c r="K130" s="456"/>
+      <c r="L130" s="454" t="s">
         <v>19</v>
       </c>
-      <c r="M130" s="476"/>
-      <c r="N130" s="476"/>
-      <c r="O130" s="476"/>
-      <c r="P130" s="477"/>
-      <c r="Q130" s="475" t="s">
+      <c r="M130" s="455"/>
+      <c r="N130" s="455"/>
+      <c r="O130" s="455"/>
+      <c r="P130" s="456"/>
+      <c r="Q130" s="454" t="s">
         <v>20</v>
       </c>
-      <c r="R130" s="476"/>
-      <c r="S130" s="476"/>
-      <c r="T130" s="476"/>
-      <c r="U130" s="477"/>
+      <c r="R130" s="455"/>
+      <c r="S130" s="455"/>
+      <c r="T130" s="455"/>
+      <c r="U130" s="456"/>
     </row>
     <row r="131" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B131" s="150" t="s">
@@ -31397,27 +31397,27 @@
     </row>
     <row r="144" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="145" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B145" s="481" t="s">
+      <c r="B145" s="460" t="s">
         <v>21</v>
       </c>
-      <c r="C145" s="482"/>
-      <c r="D145" s="482"/>
-      <c r="E145" s="482"/>
-      <c r="F145" s="483"/>
-      <c r="G145" s="481" t="s">
+      <c r="C145" s="461"/>
+      <c r="D145" s="461"/>
+      <c r="E145" s="461"/>
+      <c r="F145" s="462"/>
+      <c r="G145" s="460" t="s">
         <v>22</v>
       </c>
-      <c r="H145" s="482"/>
-      <c r="I145" s="482"/>
-      <c r="J145" s="482"/>
-      <c r="K145" s="483"/>
-      <c r="L145" s="481" t="s">
+      <c r="H145" s="461"/>
+      <c r="I145" s="461"/>
+      <c r="J145" s="461"/>
+      <c r="K145" s="462"/>
+      <c r="L145" s="460" t="s">
         <v>23</v>
       </c>
-      <c r="M145" s="482"/>
-      <c r="N145" s="482"/>
-      <c r="O145" s="482"/>
-      <c r="P145" s="483"/>
+      <c r="M145" s="461"/>
+      <c r="N145" s="461"/>
+      <c r="O145" s="461"/>
+      <c r="P145" s="462"/>
     </row>
     <row r="146" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B146" s="203" t="s">
@@ -32016,17 +32016,24 @@
     </row>
   </sheetData>
   <mergeCells count="41">
-    <mergeCell ref="B145:F145"/>
-    <mergeCell ref="G145:K145"/>
-    <mergeCell ref="L145:P145"/>
-    <mergeCell ref="B115:F115"/>
-    <mergeCell ref="G115:K115"/>
-    <mergeCell ref="L115:P115"/>
-    <mergeCell ref="Q115:U115"/>
-    <mergeCell ref="B130:F130"/>
-    <mergeCell ref="G130:K130"/>
-    <mergeCell ref="L130:P130"/>
-    <mergeCell ref="Q130:U130"/>
+    <mergeCell ref="AL1:AL2"/>
+    <mergeCell ref="AB2:AC2"/>
+    <mergeCell ref="AD2:AE2"/>
+    <mergeCell ref="AG1:AG2"/>
+    <mergeCell ref="AH1:AH2"/>
+    <mergeCell ref="AI1:AI2"/>
+    <mergeCell ref="AJ1:AJ2"/>
+    <mergeCell ref="AK1:AK2"/>
+    <mergeCell ref="AK15:AK16"/>
+    <mergeCell ref="AL15:AL16"/>
+    <mergeCell ref="AB16:AC16"/>
+    <mergeCell ref="AD16:AE16"/>
+    <mergeCell ref="AA31:AB31"/>
+    <mergeCell ref="AC31:AD31"/>
+    <mergeCell ref="AJ15:AJ16"/>
+    <mergeCell ref="AG15:AG16"/>
+    <mergeCell ref="AH15:AH16"/>
+    <mergeCell ref="AI15:AI16"/>
     <mergeCell ref="Q100:U100"/>
     <mergeCell ref="B55:F55"/>
     <mergeCell ref="G55:K55"/>
@@ -32039,24 +32046,17 @@
     <mergeCell ref="B100:F100"/>
     <mergeCell ref="G100:K100"/>
     <mergeCell ref="L100:P100"/>
-    <mergeCell ref="AK15:AK16"/>
-    <mergeCell ref="AL15:AL16"/>
-    <mergeCell ref="AB16:AC16"/>
-    <mergeCell ref="AD16:AE16"/>
-    <mergeCell ref="AA31:AB31"/>
-    <mergeCell ref="AC31:AD31"/>
-    <mergeCell ref="AJ15:AJ16"/>
-    <mergeCell ref="AG15:AG16"/>
-    <mergeCell ref="AH15:AH16"/>
-    <mergeCell ref="AI15:AI16"/>
-    <mergeCell ref="AL1:AL2"/>
-    <mergeCell ref="AB2:AC2"/>
-    <mergeCell ref="AD2:AE2"/>
-    <mergeCell ref="AG1:AG2"/>
-    <mergeCell ref="AH1:AH2"/>
-    <mergeCell ref="AI1:AI2"/>
-    <mergeCell ref="AJ1:AJ2"/>
-    <mergeCell ref="AK1:AK2"/>
+    <mergeCell ref="Q115:U115"/>
+    <mergeCell ref="B130:F130"/>
+    <mergeCell ref="G130:K130"/>
+    <mergeCell ref="L130:P130"/>
+    <mergeCell ref="Q130:U130"/>
+    <mergeCell ref="B145:F145"/>
+    <mergeCell ref="G145:K145"/>
+    <mergeCell ref="L145:P145"/>
+    <mergeCell ref="B115:F115"/>
+    <mergeCell ref="G115:K115"/>
+    <mergeCell ref="L115:P115"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -32067,8 +32067,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1F56B83-6FD0-4F97-A83F-B325F07CC791}">
   <dimension ref="A1:N40"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G46" sqref="G46"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -32087,45 +32087,45 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="451" t="s">
+      <c r="A1" s="482" t="s">
         <v>95</v>
       </c>
-      <c r="B1" s="493"/>
-      <c r="C1" s="493"/>
-      <c r="D1" s="493"/>
-      <c r="E1" s="493"/>
-      <c r="F1" s="493"/>
-      <c r="G1" s="493"/>
-      <c r="H1" s="493"/>
-      <c r="I1" s="493"/>
-      <c r="J1" s="493"/>
-      <c r="K1" s="493"/>
-      <c r="L1" s="493"/>
-      <c r="M1" s="493"/>
-      <c r="N1" s="451"/>
+      <c r="B1" s="497"/>
+      <c r="C1" s="497"/>
+      <c r="D1" s="497"/>
+      <c r="E1" s="497"/>
+      <c r="F1" s="497"/>
+      <c r="G1" s="497"/>
+      <c r="H1" s="497"/>
+      <c r="I1" s="497"/>
+      <c r="J1" s="497"/>
+      <c r="K1" s="497"/>
+      <c r="L1" s="497"/>
+      <c r="M1" s="497"/>
+      <c r="N1" s="482"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="228"/>
-      <c r="B2" s="490" t="s">
+      <c r="B2" s="498" t="s">
         <v>110</v>
       </c>
-      <c r="C2" s="491"/>
-      <c r="D2" s="492"/>
-      <c r="E2" s="490" t="s">
+      <c r="C2" s="499"/>
+      <c r="D2" s="500"/>
+      <c r="E2" s="498" t="s">
         <v>107</v>
       </c>
-      <c r="F2" s="491"/>
-      <c r="G2" s="492"/>
-      <c r="H2" s="490" t="s">
+      <c r="F2" s="499"/>
+      <c r="G2" s="500"/>
+      <c r="H2" s="498" t="s">
         <v>109</v>
       </c>
-      <c r="I2" s="491"/>
-      <c r="J2" s="492"/>
-      <c r="K2" s="490" t="s">
+      <c r="I2" s="499"/>
+      <c r="J2" s="500"/>
+      <c r="K2" s="498" t="s">
         <v>75</v>
       </c>
-      <c r="L2" s="491"/>
-      <c r="M2" s="492"/>
+      <c r="L2" s="499"/>
+      <c r="M2" s="500"/>
       <c r="N2" s="244"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
@@ -32794,45 +32794,45 @@
       </c>
     </row>
     <row r="16" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="451" t="s">
+      <c r="A16" s="482" t="s">
         <v>105</v>
       </c>
-      <c r="B16" s="493"/>
-      <c r="C16" s="493"/>
-      <c r="D16" s="493"/>
-      <c r="E16" s="493"/>
-      <c r="F16" s="493"/>
-      <c r="G16" s="493"/>
-      <c r="H16" s="493"/>
-      <c r="I16" s="493"/>
-      <c r="J16" s="493"/>
-      <c r="K16" s="493"/>
-      <c r="L16" s="493"/>
-      <c r="M16" s="493"/>
-      <c r="N16" s="451"/>
+      <c r="B16" s="497"/>
+      <c r="C16" s="497"/>
+      <c r="D16" s="497"/>
+      <c r="E16" s="497"/>
+      <c r="F16" s="497"/>
+      <c r="G16" s="497"/>
+      <c r="H16" s="497"/>
+      <c r="I16" s="497"/>
+      <c r="J16" s="497"/>
+      <c r="K16" s="497"/>
+      <c r="L16" s="497"/>
+      <c r="M16" s="497"/>
+      <c r="N16" s="482"/>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="228"/>
-      <c r="B17" s="490" t="s">
+      <c r="B17" s="498" t="s">
         <v>110</v>
       </c>
-      <c r="C17" s="491"/>
-      <c r="D17" s="492"/>
-      <c r="E17" s="490" t="s">
+      <c r="C17" s="499"/>
+      <c r="D17" s="500"/>
+      <c r="E17" s="498" t="s">
         <v>108</v>
       </c>
-      <c r="F17" s="491"/>
-      <c r="G17" s="492"/>
-      <c r="H17" s="490" t="s">
+      <c r="F17" s="499"/>
+      <c r="G17" s="500"/>
+      <c r="H17" s="498" t="s">
         <v>109</v>
       </c>
-      <c r="I17" s="491"/>
-      <c r="J17" s="492"/>
-      <c r="K17" s="490" t="s">
+      <c r="I17" s="499"/>
+      <c r="J17" s="500"/>
+      <c r="K17" s="498" t="s">
         <v>75</v>
       </c>
-      <c r="L17" s="491"/>
-      <c r="M17" s="492"/>
+      <c r="L17" s="499"/>
+      <c r="M17" s="500"/>
       <c r="N17" s="244"/>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
@@ -33384,45 +33384,45 @@
       </c>
     </row>
     <row r="30" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="451" t="s">
+      <c r="A30" s="482" t="s">
         <v>106</v>
       </c>
-      <c r="B30" s="493"/>
-      <c r="C30" s="493"/>
-      <c r="D30" s="493"/>
-      <c r="E30" s="493"/>
-      <c r="F30" s="493"/>
-      <c r="G30" s="493"/>
-      <c r="H30" s="493"/>
-      <c r="I30" s="493"/>
-      <c r="J30" s="493"/>
-      <c r="K30" s="493"/>
-      <c r="L30" s="493"/>
-      <c r="M30" s="493"/>
-      <c r="N30" s="451"/>
+      <c r="B30" s="497"/>
+      <c r="C30" s="497"/>
+      <c r="D30" s="497"/>
+      <c r="E30" s="497"/>
+      <c r="F30" s="497"/>
+      <c r="G30" s="497"/>
+      <c r="H30" s="497"/>
+      <c r="I30" s="497"/>
+      <c r="J30" s="497"/>
+      <c r="K30" s="497"/>
+      <c r="L30" s="497"/>
+      <c r="M30" s="497"/>
+      <c r="N30" s="482"/>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" s="228"/>
-      <c r="B31" s="490" t="s">
+      <c r="B31" s="498" t="s">
         <v>110</v>
       </c>
-      <c r="C31" s="491"/>
-      <c r="D31" s="492"/>
-      <c r="E31" s="490" t="s">
+      <c r="C31" s="499"/>
+      <c r="D31" s="500"/>
+      <c r="E31" s="498" t="s">
         <v>108</v>
       </c>
-      <c r="F31" s="491"/>
-      <c r="G31" s="492"/>
-      <c r="H31" s="490" t="s">
+      <c r="F31" s="499"/>
+      <c r="G31" s="500"/>
+      <c r="H31" s="498" t="s">
         <v>109</v>
       </c>
-      <c r="I31" s="491"/>
-      <c r="J31" s="492"/>
-      <c r="K31" s="490" t="s">
+      <c r="I31" s="499"/>
+      <c r="J31" s="500"/>
+      <c r="K31" s="498" t="s">
         <v>75</v>
       </c>
-      <c r="L31" s="491"/>
-      <c r="M31" s="492"/>
+      <c r="L31" s="499"/>
+      <c r="M31" s="500"/>
       <c r="N31" s="244"/>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
@@ -33481,6 +33481,7 @@
         <v>1.5851</v>
       </c>
       <c r="D33" s="240">
+        <f>B33/C33</f>
         <v>-0.37669547662608038</v>
       </c>
       <c r="E33" s="242">
@@ -33491,6 +33492,7 @@
         <v>7.529399999999999</v>
       </c>
       <c r="G33" s="240">
+        <f>E33/F33</f>
         <v>5.3917215161656415E-2</v>
       </c>
       <c r="H33" s="242">
@@ -33501,6 +33503,7 @@
         <v>3.7933434306569351</v>
       </c>
       <c r="J33" s="240">
+        <f>H33/I33</f>
         <v>0.14194609149272011</v>
       </c>
       <c r="K33" s="239">
@@ -33511,6 +33514,7 @@
         <v>0.20310881995133825</v>
       </c>
       <c r="M33" s="420">
+        <f>K33/L33</f>
         <v>0.18061966240201743</v>
       </c>
       <c r="N33" s="379">
@@ -33529,6 +33533,7 @@
         <v>1.5595000000000001</v>
       </c>
       <c r="D34" s="240">
+        <f t="shared" ref="D34:D40" si="8">B34/C34</f>
         <v>3.0456556588650203</v>
       </c>
       <c r="E34" s="242">
@@ -33539,6 +33544,7 @@
         <v>7.0016999999999996</v>
       </c>
       <c r="G34" s="240">
+        <f t="shared" ref="G34:G40" si="9">E34/F34</f>
         <v>-6.1235821461973795E-3</v>
       </c>
       <c r="H34" s="242">
@@ -33549,6 +33555,7 @@
         <v>3.2029096365455167</v>
       </c>
       <c r="J34" s="240">
+        <f t="shared" ref="J34:J40" si="10">H34/I34</f>
         <v>0.2406337151637577</v>
       </c>
       <c r="K34" s="239">
@@ -33559,6 +33566,7 @@
         <v>0.18703707902634226</v>
       </c>
       <c r="M34" s="420">
+        <f t="shared" ref="M34:M40" si="11">K34/L34</f>
         <v>0.25528328492852753</v>
       </c>
       <c r="N34" s="422">
@@ -33573,40 +33581,44 @@
         <v>-2.7269000000000001</v>
       </c>
       <c r="C35" s="443">
-        <f t="shared" ref="C35:C40" si="8">C22</f>
+        <f t="shared" ref="C35:C40" si="12">C22</f>
         <v>6.3570000000000002</v>
       </c>
       <c r="D35" s="240">
+        <f t="shared" si="8"/>
         <v>-0.42896020135283941</v>
       </c>
       <c r="E35" s="242">
         <v>0.11854131335046647</v>
       </c>
       <c r="F35" s="441">
-        <f t="shared" ref="F35:F40" si="9">F22</f>
+        <f t="shared" ref="F35:F40" si="13">F22</f>
         <v>10.2044</v>
       </c>
       <c r="G35" s="240">
+        <f t="shared" si="9"/>
         <v>1.1616686267734161E-2</v>
       </c>
       <c r="H35" s="242">
         <v>-1.5595514376973254</v>
       </c>
       <c r="I35" s="440">
-        <f t="shared" ref="I35:I40" si="10">I22</f>
+        <f t="shared" ref="I35:I40" si="14">I22</f>
         <v>7.0654710684273754</v>
       </c>
       <c r="J35" s="240">
+        <f t="shared" si="10"/>
         <v>-0.22072858590650893</v>
       </c>
       <c r="K35" s="239">
         <v>-9.8289875653147785E-2</v>
       </c>
       <c r="L35" s="440">
-        <f t="shared" ref="L35:L40" si="11">L22</f>
+        <f t="shared" ref="L35:L40" si="15">L22</f>
         <v>0.45884337735094055</v>
       </c>
       <c r="M35" s="420">
+        <f t="shared" si="11"/>
         <v>-0.2142122573951242</v>
       </c>
       <c r="N35" s="381">
@@ -33621,41 +33633,45 @@
         <v>-3.7258000000000004</v>
       </c>
       <c r="C36" s="443">
+        <f t="shared" si="12"/>
+        <v>6.3470000000000004</v>
+      </c>
+      <c r="D36" s="240">
         <f t="shared" si="8"/>
-        <v>6.3470000000000004</v>
-      </c>
-      <c r="D36" s="240">
         <v>-0.58701748857728064</v>
       </c>
       <c r="E36" s="242">
         <v>0.20527559701143749</v>
       </c>
       <c r="F36" s="441">
+        <f t="shared" si="13"/>
+        <v>8.2335999999999991</v>
+      </c>
+      <c r="G36" s="240">
         <f t="shared" si="9"/>
-        <v>8.2335999999999991</v>
-      </c>
-      <c r="G36" s="240">
         <v>2.4931451249931683E-2</v>
       </c>
       <c r="H36" s="242">
         <v>0.76175130767380761</v>
       </c>
       <c r="I36" s="440">
+        <f t="shared" si="14"/>
+        <v>5.0778449889732853</v>
+      </c>
+      <c r="J36" s="240">
         <f t="shared" si="10"/>
-        <v>5.0778449889732853</v>
-      </c>
-      <c r="J36" s="240">
         <v>0.15001468326189096</v>
       </c>
       <c r="K36" s="239">
         <v>-6.4526904685237904E-2</v>
       </c>
       <c r="L36" s="440">
+        <f t="shared" si="15"/>
+        <v>0.53364981622151375</v>
+      </c>
+      <c r="M36" s="420">
         <f t="shared" si="11"/>
-        <v>0.53364981622151375</v>
-      </c>
-      <c r="M36" s="420">
-        <v>-0.12091619396052283</v>
+        <v>-0.12091619396052281</v>
       </c>
       <c r="N36" s="381">
         <v>0.11743877238132332</v>
@@ -33669,40 +33685,44 @@
         <v>-5.5202999999999998</v>
       </c>
       <c r="C37" s="443">
+        <f t="shared" si="12"/>
+        <v>6.3075000000000001</v>
+      </c>
+      <c r="D37" s="240">
         <f t="shared" si="8"/>
-        <v>6.3075000000000001</v>
-      </c>
-      <c r="D37" s="240">
         <v>-0.87519619500594525</v>
       </c>
       <c r="E37" s="242">
         <v>0.25186380023202659</v>
       </c>
       <c r="F37" s="441">
+        <f t="shared" si="13"/>
+        <v>6.8244000000000007</v>
+      </c>
+      <c r="G37" s="240">
         <f t="shared" si="9"/>
-        <v>6.8244000000000007</v>
-      </c>
-      <c r="G37" s="240">
         <v>3.6906365428759531E-2</v>
       </c>
       <c r="H37" s="242">
         <v>0.65548799899290877</v>
       </c>
       <c r="I37" s="440">
+        <f t="shared" si="14"/>
+        <v>3.4966024327251528</v>
+      </c>
+      <c r="J37" s="240">
         <f t="shared" si="10"/>
-        <v>3.4966024327251528</v>
-      </c>
-      <c r="J37" s="240">
         <v>0.18746426326828355</v>
       </c>
       <c r="K37" s="239">
         <v>4.5248200775063058E-2</v>
       </c>
       <c r="L37" s="440">
+        <f t="shared" si="15"/>
+        <v>0.23523687411480473</v>
+      </c>
+      <c r="M37" s="420">
         <f t="shared" si="11"/>
-        <v>0.23523687411480473</v>
-      </c>
-      <c r="M37" s="420">
         <v>0.19235164956740658</v>
       </c>
       <c r="N37" s="225">
@@ -33717,40 +33737,44 @@
         <v>-2.0448999999999997</v>
       </c>
       <c r="C38" s="443">
+        <f t="shared" si="12"/>
+        <v>3.1258999999999997</v>
+      </c>
+      <c r="D38" s="240">
         <f t="shared" si="8"/>
-        <v>3.1258999999999997</v>
-      </c>
-      <c r="D38" s="240">
         <v>-0.65417959627627242</v>
       </c>
       <c r="E38" s="242">
         <v>1.849413921397858</v>
       </c>
       <c r="F38" s="441">
+        <f t="shared" si="13"/>
+        <v>7.5085999999999995</v>
+      </c>
+      <c r="G38" s="240">
         <f t="shared" si="9"/>
-        <v>7.5085999999999995</v>
-      </c>
-      <c r="G38" s="240">
         <v>0.24630609186770611</v>
       </c>
       <c r="H38" s="242">
         <v>0.63760360773591351</v>
       </c>
       <c r="I38" s="440">
+        <f t="shared" si="14"/>
+        <v>4.2943881967213136</v>
+      </c>
+      <c r="J38" s="240">
         <f t="shared" si="10"/>
-        <v>4.2943881967213136</v>
-      </c>
-      <c r="J38" s="240">
         <v>0.14847367739663409</v>
       </c>
       <c r="K38" s="239">
         <v>1.9282470866228862E-2</v>
       </c>
       <c r="L38" s="440">
+        <f t="shared" si="15"/>
+        <v>0.27809010795681738</v>
+      </c>
+      <c r="M38" s="420">
         <f t="shared" si="11"/>
-        <v>0.27809010795681738</v>
-      </c>
-      <c r="M38" s="420">
         <v>6.9338931211544927E-2</v>
       </c>
       <c r="N38" s="380">
@@ -33765,47 +33789,51 @@
         <v>-0.77380000000000015</v>
       </c>
       <c r="C39" s="443">
+        <f t="shared" si="12"/>
+        <v>1.2892000000000001</v>
+      </c>
+      <c r="D39" s="240">
         <f t="shared" si="8"/>
-        <v>1.2892000000000001</v>
-      </c>
-      <c r="D39" s="240">
         <v>-0.60021718895439036</v>
       </c>
       <c r="E39" s="242">
         <v>-0.87190683761703458</v>
       </c>
       <c r="F39" s="441">
+        <f t="shared" si="13"/>
+        <v>8.2502999999999993</v>
+      </c>
+      <c r="G39" s="240">
         <f t="shared" si="9"/>
-        <v>8.2502999999999993</v>
-      </c>
-      <c r="G39" s="240">
         <v>-0.10568183431112016</v>
       </c>
       <c r="H39" s="242">
         <v>0.51081309197247027</v>
       </c>
       <c r="I39" s="440">
+        <f t="shared" si="14"/>
+        <v>5.5288184321347602</v>
+      </c>
+      <c r="J39" s="240">
         <f t="shared" si="10"/>
-        <v>5.5288184321347602</v>
-      </c>
-      <c r="J39" s="240">
         <v>9.2391005102194612E-2</v>
       </c>
       <c r="K39" s="239">
         <v>0.10979374564456568</v>
       </c>
       <c r="L39" s="440">
+        <f t="shared" si="15"/>
+        <v>0.3598969808875932</v>
+      </c>
+      <c r="M39" s="420">
         <f t="shared" si="11"/>
-        <v>0.3598969808875932</v>
-      </c>
-      <c r="M39" s="420">
         <v>0.30506992688237528</v>
       </c>
       <c r="N39" s="380">
         <v>-0.11251612892623995</v>
       </c>
     </row>
-    <row r="40" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40" s="236" t="s">
         <v>89</v>
       </c>
@@ -33813,41 +33841,45 @@
         <v>-0.69299999999999962</v>
       </c>
       <c r="C40" s="443">
+        <f t="shared" si="12"/>
+        <v>2.1473999999999998</v>
+      </c>
+      <c r="D40" s="240">
         <f t="shared" si="8"/>
-        <v>2.1473999999999998</v>
-      </c>
-      <c r="D40" s="241">
         <v>-0.32271584241408202</v>
       </c>
       <c r="E40" s="242">
         <v>-0.90590974459061657</v>
       </c>
       <c r="F40" s="441">
+        <f t="shared" si="13"/>
+        <v>9.2515999999999998</v>
+      </c>
+      <c r="G40" s="240">
         <f t="shared" si="9"/>
-        <v>9.2515999999999998</v>
-      </c>
-      <c r="G40" s="241">
         <v>-9.7919251220396103E-2</v>
       </c>
       <c r="H40" s="242">
         <v>2.7966349436854614</v>
       </c>
       <c r="I40" s="440">
+        <f t="shared" si="14"/>
+        <v>4.0606493176648994</v>
+      </c>
+      <c r="J40" s="240">
         <f t="shared" si="10"/>
-        <v>4.0606493176648994</v>
-      </c>
-      <c r="J40" s="241">
         <v>0.68871619411195129</v>
       </c>
       <c r="K40" s="239">
         <v>0.20807480090515129</v>
       </c>
       <c r="L40" s="440">
-        <f t="shared" si="11"/>
+        <f t="shared" si="15"/>
         <v>0.8784301134521878</v>
       </c>
-      <c r="M40" s="421">
-        <v>0.73881089123312471</v>
+      <c r="M40" s="420">
+        <f>K40/L40</f>
+        <v>0.23687120662044178</v>
       </c>
       <c r="N40" s="382">
         <v>-4.9570413884485784E-2</v>
@@ -33855,11 +33887,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="A30:N30"/>
-    <mergeCell ref="B31:D31"/>
-    <mergeCell ref="E31:G31"/>
-    <mergeCell ref="H31:J31"/>
-    <mergeCell ref="K31:M31"/>
     <mergeCell ref="B17:D17"/>
     <mergeCell ref="E17:G17"/>
     <mergeCell ref="H17:J17"/>
@@ -33870,6 +33897,11 @@
     <mergeCell ref="H2:J2"/>
     <mergeCell ref="K2:M2"/>
     <mergeCell ref="A16:N16"/>
+    <mergeCell ref="A30:N30"/>
+    <mergeCell ref="B31:D31"/>
+    <mergeCell ref="E31:G31"/>
+    <mergeCell ref="H31:J31"/>
+    <mergeCell ref="K31:M31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>